<commit_message>
Added some of my stuff
</commit_message>
<xml_diff>
--- a/docs/ganttChart.xlsx
+++ b/docs/ganttChart.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Management Summary" sheetId="1" state="visible" r:id="rId2"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="39">
   <si>
     <t xml:space="preserve">Total</t>
   </si>
@@ -127,16 +127,19 @@
     <t xml:space="preserve">Individual schedule</t>
   </si>
   <si>
+    <t xml:space="preserve">RFP – part 6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Champion</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Presentation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Subtotal</t>
+  </si>
+  <si>
     <t xml:space="preserve">RFP</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Champion</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Presentation</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Subtotal</t>
   </si>
 </sst>
 </file>
@@ -349,7 +352,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="45">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -371,10 +374,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -633,8 +632,8 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="14.15"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="5.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="12.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="14.7"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="11.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="14.69"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="11.3"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="18" style="0" width="8.45"/>
   </cols>
   <sheetData>
@@ -672,23 +671,22 @@
       <c r="E3" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="F3" s="6"/>
-      <c r="G3" s="7" t="s">
+      <c r="G3" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="H3" s="8" t="s">
+      <c r="H3" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="I3" s="9" t="s">
+      <c r="I3" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="K3" s="7" t="s">
+      <c r="K3" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="L3" s="8" t="s">
+      <c r="L3" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="M3" s="9" t="s">
+      <c r="M3" s="8" t="s">
         <v>6</v>
       </c>
       <c r="O3" s="3" t="s">
@@ -702,103 +700,101 @@
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B4" s="10" t="s">
+      <c r="B4" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="11" t="n">
+      <c r="C4" s="10" t="n">
         <f aca="false">(G4+K4+O4)</f>
+        <v>1500</v>
+      </c>
+      <c r="D4" s="11" t="n">
+        <f aca="false">(H4+L4+P4)</f>
+        <v>425</v>
+      </c>
+      <c r="E4" s="12" t="n">
+        <f aca="false">(C4-D4)</f>
+        <v>1075</v>
+      </c>
+      <c r="G4" s="13" t="n">
+        <v>0</v>
+      </c>
+      <c r="H4" s="14" t="n">
+        <v>0</v>
+      </c>
+      <c r="I4" s="15" t="n">
+        <f aca="false">(G4-H4)</f>
+        <v>0</v>
+      </c>
+      <c r="K4" s="10" t="n">
         <v>1000</v>
       </c>
-      <c r="D4" s="12" t="n">
-        <f aca="false">(H4+L4+P4)</f>
-        <v>350</v>
-      </c>
-      <c r="E4" s="13" t="n">
-        <f aca="false">(C4-D4)</f>
-        <v>650</v>
-      </c>
-      <c r="F4" s="6"/>
-      <c r="G4" s="14" t="n">
-        <v>0</v>
-      </c>
-      <c r="H4" s="15" t="n">
-        <v>0</v>
-      </c>
-      <c r="I4" s="16" t="n">
-        <f aca="false">(G4-H4)</f>
-        <v>0</v>
-      </c>
-      <c r="K4" s="11" t="n">
-        <v>1000</v>
-      </c>
-      <c r="L4" s="12" t="n">
+      <c r="L4" s="11" t="n">
         <f aca="false">Meetings!B4*100</f>
         <v>350</v>
       </c>
-      <c r="M4" s="13" t="n">
+      <c r="M4" s="12" t="n">
         <f aca="false">(K4-L4)</f>
         <v>650</v>
       </c>
-      <c r="O4" s="11" t="n">
+      <c r="O4" s="10" t="n">
         <f aca="false">(SA!C6)*100</f>
-        <v>0</v>
-      </c>
-      <c r="P4" s="12" t="n">
+        <v>500</v>
+      </c>
+      <c r="P4" s="11" t="n">
         <f aca="false">(SA!D6)*100</f>
-        <v>0</v>
-      </c>
-      <c r="Q4" s="13" t="n">
+        <v>75</v>
+      </c>
+      <c r="Q4" s="12" t="n">
         <f aca="false">(O4-P4)</f>
-        <v>0</v>
+        <v>425</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B5" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="14" t="n">
+      <c r="C5" s="13" t="n">
         <f aca="false">(G5+K5+O5)</f>
         <v>1000</v>
       </c>
-      <c r="D5" s="15" t="n">
+      <c r="D5" s="14" t="n">
         <f aca="false">(H5+L5+P5)</f>
         <v>300</v>
       </c>
-      <c r="E5" s="16" t="n">
+      <c r="E5" s="15" t="n">
         <f aca="false">(C5-D5)</f>
         <v>700</v>
       </c>
-      <c r="F5" s="6"/>
-      <c r="G5" s="14" t="n">
-        <v>0</v>
-      </c>
-      <c r="H5" s="15" t="n">
-        <v>0</v>
-      </c>
-      <c r="I5" s="16" t="n">
+      <c r="G5" s="13" t="n">
+        <v>0</v>
+      </c>
+      <c r="H5" s="14" t="n">
+        <v>0</v>
+      </c>
+      <c r="I5" s="15" t="n">
         <f aca="false">(G5-H5)</f>
         <v>0</v>
       </c>
-      <c r="K5" s="14" t="n">
+      <c r="K5" s="13" t="n">
         <v>1000</v>
       </c>
-      <c r="L5" s="15" t="n">
+      <c r="L5" s="14" t="n">
         <f aca="false">Meetings!B5*100</f>
         <v>300</v>
       </c>
-      <c r="M5" s="16" t="n">
+      <c r="M5" s="15" t="n">
         <f aca="false">(K5-L5)</f>
         <v>700</v>
       </c>
-      <c r="O5" s="14" t="n">
+      <c r="O5" s="13" t="n">
         <f aca="false">(SA!C11)*100</f>
         <v>0</v>
       </c>
-      <c r="P5" s="15" t="n">
+      <c r="P5" s="14" t="n">
         <f aca="false">(SA!D11)*100</f>
         <v>0</v>
       </c>
-      <c r="Q5" s="16" t="n">
+      <c r="Q5" s="15" t="n">
         <f aca="false">(O5-P5)</f>
         <v>0</v>
       </c>
@@ -807,49 +803,48 @@
       <c r="B6" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C6" s="14" t="n">
+      <c r="C6" s="13" t="n">
         <f aca="false">(G6+K6+O6)</f>
         <v>1000</v>
       </c>
-      <c r="D6" s="15" t="n">
+      <c r="D6" s="14" t="n">
         <f aca="false">(H6+L6+P6)</f>
         <v>350</v>
       </c>
-      <c r="E6" s="16" t="n">
+      <c r="E6" s="15" t="n">
         <f aca="false">(C6-D6)</f>
         <v>650</v>
       </c>
-      <c r="F6" s="6"/>
-      <c r="G6" s="14" t="n">
-        <v>0</v>
-      </c>
-      <c r="H6" s="15" t="n">
-        <v>0</v>
-      </c>
-      <c r="I6" s="16" t="n">
+      <c r="G6" s="13" t="n">
+        <v>0</v>
+      </c>
+      <c r="H6" s="14" t="n">
+        <v>0</v>
+      </c>
+      <c r="I6" s="15" t="n">
         <f aca="false">(G6-H6)</f>
         <v>0</v>
       </c>
-      <c r="K6" s="14" t="n">
+      <c r="K6" s="13" t="n">
         <v>1000</v>
       </c>
-      <c r="L6" s="15" t="n">
+      <c r="L6" s="14" t="n">
         <f aca="false">Meetings!B6*100</f>
         <v>350</v>
       </c>
-      <c r="M6" s="16" t="n">
+      <c r="M6" s="15" t="n">
         <f aca="false">(K6-L6)</f>
         <v>650</v>
       </c>
-      <c r="O6" s="14" t="n">
+      <c r="O6" s="13" t="n">
         <f aca="false">(SA!C16)*100</f>
         <v>0</v>
       </c>
-      <c r="P6" s="15" t="n">
+      <c r="P6" s="14" t="n">
         <f aca="false">(SA!D16)*100</f>
         <v>0</v>
       </c>
-      <c r="Q6" s="16" t="n">
+      <c r="Q6" s="15" t="n">
         <f aca="false">(O6-P6)</f>
         <v>0</v>
       </c>
@@ -858,201 +853,197 @@
       <c r="B7" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C7" s="14" t="n">
+      <c r="C7" s="13" t="n">
         <f aca="false">(G7+K7+O7)</f>
         <v>1000</v>
       </c>
-      <c r="D7" s="15" t="n">
+      <c r="D7" s="14" t="n">
         <f aca="false">(H7+L7+P7)</f>
         <v>350</v>
       </c>
-      <c r="E7" s="16" t="n">
+      <c r="E7" s="15" t="n">
         <f aca="false">(C7-D7)</f>
         <v>650</v>
       </c>
-      <c r="F7" s="6"/>
-      <c r="G7" s="14" t="n">
-        <v>0</v>
-      </c>
-      <c r="H7" s="15" t="n">
-        <v>0</v>
-      </c>
-      <c r="I7" s="16" t="n">
+      <c r="G7" s="13" t="n">
+        <v>0</v>
+      </c>
+      <c r="H7" s="14" t="n">
+        <v>0</v>
+      </c>
+      <c r="I7" s="15" t="n">
         <f aca="false">(G7-H7)</f>
         <v>0</v>
       </c>
-      <c r="K7" s="14" t="n">
+      <c r="K7" s="13" t="n">
         <v>1000</v>
       </c>
-      <c r="L7" s="15" t="n">
+      <c r="L7" s="14" t="n">
         <f aca="false">Meetings!B7*100</f>
         <v>350</v>
       </c>
-      <c r="M7" s="16" t="n">
+      <c r="M7" s="15" t="n">
         <f aca="false">(K7-L7)</f>
         <v>650</v>
       </c>
-      <c r="O7" s="14" t="n">
+      <c r="O7" s="13" t="n">
         <f aca="false">(SA!C26)*100</f>
         <v>0</v>
       </c>
-      <c r="P7" s="15" t="n">
+      <c r="P7" s="14" t="n">
         <f aca="false">(SA!D26)*100</f>
         <v>0</v>
       </c>
-      <c r="Q7" s="16" t="n">
+      <c r="Q7" s="15" t="n">
         <f aca="false">(O7-P7)</f>
         <v>0</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B8" s="17" t="s">
+      <c r="B8" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="C8" s="15" t="n">
+      <c r="C8" s="14" t="n">
         <f aca="false">(G8+K8+O8)</f>
         <v>1000</v>
       </c>
-      <c r="D8" s="15" t="n">
+      <c r="D8" s="14" t="n">
         <f aca="false">(H8+L8+P8)</f>
         <v>350</v>
       </c>
-      <c r="E8" s="16" t="n">
+      <c r="E8" s="15" t="n">
         <f aca="false">(C8-D8)</f>
         <v>650</v>
       </c>
-      <c r="F8" s="6"/>
-      <c r="G8" s="14" t="n">
-        <v>0</v>
-      </c>
-      <c r="H8" s="15" t="n">
-        <v>0</v>
-      </c>
-      <c r="I8" s="16" t="n">
+      <c r="G8" s="13" t="n">
+        <v>0</v>
+      </c>
+      <c r="H8" s="14" t="n">
+        <v>0</v>
+      </c>
+      <c r="I8" s="15" t="n">
         <f aca="false">(G8-H8)</f>
         <v>0</v>
       </c>
-      <c r="K8" s="14" t="n">
+      <c r="K8" s="13" t="n">
         <v>1000</v>
       </c>
-      <c r="L8" s="15" t="n">
+      <c r="L8" s="14" t="n">
         <f aca="false">Meetings!B8*100</f>
         <v>350</v>
       </c>
-      <c r="M8" s="16" t="n">
+      <c r="M8" s="15" t="n">
         <f aca="false">(K8-L8)</f>
         <v>650</v>
       </c>
-      <c r="O8" s="14" t="n">
-        <v>0</v>
-      </c>
-      <c r="P8" s="15" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q8" s="16" t="n">
+      <c r="O8" s="13" t="n">
+        <v>0</v>
+      </c>
+      <c r="P8" s="14" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q8" s="15" t="n">
         <f aca="false">(O8-P8)</f>
         <v>0</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B9" s="17" t="s">
+      <c r="B9" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="C9" s="15" t="n">
+      <c r="C9" s="14" t="n">
         <f aca="false">+(G9+K9+O9)</f>
         <v>1000</v>
       </c>
-      <c r="D9" s="15" t="n">
+      <c r="D9" s="14" t="n">
         <f aca="false">(H9+L9+P9)</f>
         <v>200</v>
       </c>
-      <c r="E9" s="18" t="n">
+      <c r="E9" s="17" t="n">
         <f aca="false">(C9-D9)</f>
         <v>800</v>
       </c>
-      <c r="F9" s="6"/>
-      <c r="G9" s="14" t="n">
-        <v>0</v>
-      </c>
-      <c r="H9" s="19" t="n">
-        <v>0</v>
-      </c>
-      <c r="I9" s="16" t="n">
+      <c r="G9" s="13" t="n">
+        <v>0</v>
+      </c>
+      <c r="H9" s="18" t="n">
+        <v>0</v>
+      </c>
+      <c r="I9" s="15" t="n">
         <f aca="false">(G9-H9)</f>
         <v>0</v>
       </c>
-      <c r="K9" s="20" t="n">
+      <c r="K9" s="19" t="n">
         <v>1000</v>
       </c>
-      <c r="L9" s="15" t="n">
+      <c r="L9" s="14" t="n">
         <f aca="false">Meetings!B9*100</f>
         <v>200</v>
       </c>
-      <c r="M9" s="16" t="n">
+      <c r="M9" s="15" t="n">
         <f aca="false">(K9-L9)</f>
         <v>800</v>
       </c>
-      <c r="O9" s="14" t="n">
-        <v>0</v>
-      </c>
-      <c r="P9" s="15" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q9" s="16" t="n">
+      <c r="O9" s="13" t="n">
+        <v>0</v>
+      </c>
+      <c r="P9" s="14" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q9" s="15" t="n">
         <f aca="false">(O9-P9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B10" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="C10" s="21" t="n">
+      <c r="B10" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="C10" s="20" t="n">
         <f aca="false">SUM(C4:C9)</f>
-        <v>6000</v>
-      </c>
-      <c r="D10" s="22" t="n">
+        <v>6500</v>
+      </c>
+      <c r="D10" s="21" t="n">
         <f aca="false">SUM(D4:D9)</f>
-        <v>1900</v>
-      </c>
-      <c r="E10" s="23" t="n">
+        <v>1975</v>
+      </c>
+      <c r="E10" s="22" t="n">
         <f aca="false">SUM(E4:E9)</f>
-        <v>4100</v>
-      </c>
-      <c r="F10" s="6"/>
-      <c r="G10" s="21" t="n">
+        <v>4525</v>
+      </c>
+      <c r="G10" s="20" t="n">
         <f aca="false">SUM(G5:G9)</f>
         <v>0</v>
       </c>
-      <c r="H10" s="22" t="n">
+      <c r="H10" s="21" t="n">
         <f aca="false">SUM(H5:H9)</f>
         <v>0</v>
       </c>
-      <c r="I10" s="23" t="n">
+      <c r="I10" s="22" t="n">
         <f aca="false">SUM(I5:I9)</f>
         <v>0</v>
       </c>
-      <c r="K10" s="21" t="n">
+      <c r="K10" s="20" t="n">
         <f aca="false">SUM(K5:K9)</f>
         <v>5000</v>
       </c>
-      <c r="L10" s="22" t="n">
+      <c r="L10" s="21" t="n">
         <f aca="false">SUM(L5:L9)</f>
         <v>1550</v>
       </c>
-      <c r="M10" s="23" t="n">
+      <c r="M10" s="22" t="n">
         <f aca="false">SUM(M5:M9)</f>
         <v>3450</v>
       </c>
-      <c r="O10" s="24" t="n">
+      <c r="O10" s="23" t="n">
         <f aca="false">SUM(O5:O9)</f>
         <v>0</v>
       </c>
-      <c r="P10" s="25" t="n">
+      <c r="P10" s="24" t="n">
         <f aca="false">SUM(P5:P9)</f>
         <v>0</v>
       </c>
-      <c r="Q10" s="26" t="n">
+      <c r="Q10" s="25" t="n">
         <f aca="false">SUM(Q5:Q9)</f>
         <v>0</v>
       </c>
@@ -1087,8 +1078,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="28.99"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="17.58"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="28.98"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="17.59"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="15.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="4" style="0" width="8.45"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="10.71"/>
@@ -1105,21 +1096,21 @@
       <c r="D1" s="0" t="s">
         <v>15</v>
       </c>
-      <c r="E1" s="27"/>
+      <c r="E1" s="26"/>
       <c r="F1" s="0" t="s">
         <v>16</v>
       </c>
-      <c r="H1" s="28"/>
+      <c r="H1" s="27"/>
       <c r="I1" s="0" t="s">
         <v>17</v>
       </c>
-      <c r="K1" s="29"/>
+      <c r="K1" s="28"/>
       <c r="L1" s="0" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="30" t="s">
+      <c r="A2" s="29" t="s">
         <v>7</v>
       </c>
       <c r="D2" s="0" t="s">
@@ -1218,15 +1209,9 @@
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="31" t="s">
+      <c r="A11" s="30" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J16" s="6"/>
-    </row>
-    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="V17" s="6"/>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
@@ -1242,7 +1227,7 @@
       </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="31" t="s">
+      <c r="A21" s="30" t="s">
         <v>9</v>
       </c>
     </row>
@@ -1260,7 +1245,7 @@
       </c>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="31" t="s">
+      <c r="A29" s="30" t="s">
         <v>10</v>
       </c>
     </row>
@@ -1278,7 +1263,7 @@
       </c>
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="31" t="s">
+      <c r="A37" s="30" t="s">
         <v>11</v>
       </c>
     </row>
@@ -1296,7 +1281,7 @@
       </c>
     </row>
     <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="31" t="s">
+      <c r="A46" s="30" t="s">
         <v>12</v>
       </c>
     </row>
@@ -1330,11 +1315,11 @@
       <c r="A55" s="0" t="s">
         <v>22</v>
       </c>
-      <c r="B55" s="32" t="n">
+      <c r="B55" s="31" t="n">
         <f aca="false">B54*100</f>
         <v>0</v>
       </c>
-      <c r="C55" s="32" t="n">
+      <c r="C55" s="31" t="n">
         <f aca="false">C54*100</f>
         <v>0</v>
       </c>
@@ -1357,7 +1342,7 @@
   </sheetPr>
   <dimension ref="A1:L12"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="F4" activeCellId="0" sqref="F4"/>
     </sheetView>
   </sheetViews>
@@ -1367,307 +1352,304 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B1" s="33" t="s">
+      <c r="B1" s="32" t="s">
         <v>23</v>
       </c>
-      <c r="C1" s="34" t="n">
+      <c r="C1" s="33" t="n">
         <v>43489</v>
       </c>
-      <c r="D1" s="34" t="n">
+      <c r="D1" s="33" t="n">
         <v>43494</v>
       </c>
-      <c r="E1" s="34" t="n">
+      <c r="E1" s="33" t="n">
         <v>43496</v>
       </c>
-      <c r="F1" s="34" t="n">
+      <c r="F1" s="33" t="n">
         <v>43497</v>
       </c>
-      <c r="G1" s="33" t="s">
+      <c r="G1" s="32" t="s">
         <v>24</v>
       </c>
-      <c r="H1" s="33" t="s">
+      <c r="H1" s="32" t="s">
         <v>24</v>
       </c>
-      <c r="I1" s="33" t="s">
+      <c r="I1" s="32" t="s">
         <v>24</v>
       </c>
-      <c r="J1" s="33" t="s">
+      <c r="J1" s="32" t="s">
         <v>24</v>
       </c>
-      <c r="K1" s="33" t="s">
+      <c r="K1" s="32" t="s">
         <v>24</v>
       </c>
-      <c r="L1" s="33" t="s">
+      <c r="L1" s="32" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="62.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B2" s="33" t="s">
+      <c r="B2" s="32" t="s">
         <v>25</v>
       </c>
-      <c r="C2" s="35" t="s">
+      <c r="C2" s="34" t="s">
         <v>26</v>
       </c>
-      <c r="D2" s="35" t="s">
+      <c r="D2" s="34" t="s">
         <v>27</v>
       </c>
-      <c r="E2" s="35" t="s">
+      <c r="E2" s="34" t="s">
         <v>27</v>
       </c>
-      <c r="F2" s="35" t="s">
+      <c r="F2" s="34" t="s">
         <v>27</v>
       </c>
-      <c r="G2" s="35" t="s">
+      <c r="G2" s="34" t="s">
         <v>24</v>
       </c>
-      <c r="H2" s="35" t="s">
+      <c r="H2" s="34" t="s">
         <v>24</v>
       </c>
-      <c r="I2" s="35" t="s">
+      <c r="I2" s="34" t="s">
         <v>24</v>
       </c>
-      <c r="J2" s="35" t="s">
+      <c r="J2" s="34" t="s">
         <v>24</v>
       </c>
-      <c r="K2" s="35" t="s">
+      <c r="K2" s="34" t="s">
         <v>24</v>
       </c>
-      <c r="L2" s="35" t="s">
+      <c r="L2" s="34" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B3" s="33" t="s">
+      <c r="B3" s="32" t="s">
         <v>28</v>
       </c>
-      <c r="C3" s="33" t="n">
+      <c r="C3" s="32" t="n">
         <v>1.5</v>
       </c>
-      <c r="D3" s="33" t="n">
+      <c r="D3" s="32" t="n">
         <v>0.5</v>
       </c>
-      <c r="E3" s="33" t="n">
+      <c r="E3" s="32" t="n">
         <v>0.5</v>
       </c>
-      <c r="F3" s="33" t="n">
+      <c r="F3" s="32" t="n">
         <v>1</v>
       </c>
-      <c r="G3" s="33" t="n">
-        <v>0</v>
-      </c>
-      <c r="H3" s="33" t="n">
-        <v>0</v>
-      </c>
-      <c r="I3" s="33" t="n">
-        <v>0</v>
-      </c>
-      <c r="J3" s="33" t="n">
-        <v>0</v>
-      </c>
-      <c r="K3" s="33" t="n">
-        <v>0</v>
-      </c>
-      <c r="L3" s="33" t="n">
+      <c r="G3" s="32" t="n">
+        <v>0</v>
+      </c>
+      <c r="H3" s="32" t="n">
+        <v>0</v>
+      </c>
+      <c r="I3" s="32" t="n">
+        <v>0</v>
+      </c>
+      <c r="J3" s="32" t="n">
+        <v>0</v>
+      </c>
+      <c r="K3" s="32" t="n">
+        <v>0</v>
+      </c>
+      <c r="L3" s="32" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="33" t="s">
+      <c r="A4" s="32" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="33" t="n">
+      <c r="B4" s="32" t="n">
         <f aca="false">SUMIF(C4:L4,A$12,C$3:Z$3)</f>
         <v>3.5</v>
       </c>
-      <c r="C4" s="36" t="s">
-        <v>29</v>
-      </c>
-      <c r="D4" s="36" t="s">
-        <v>29</v>
-      </c>
-      <c r="E4" s="36" t="s">
-        <v>29</v>
-      </c>
-      <c r="F4" s="36" t="s">
-        <v>29</v>
-      </c>
-      <c r="G4" s="36"/>
-      <c r="H4" s="36"/>
-      <c r="I4" s="36"/>
-      <c r="J4" s="36"/>
-      <c r="K4" s="36"/>
-      <c r="L4" s="36"/>
+      <c r="C4" s="35" t="s">
+        <v>29</v>
+      </c>
+      <c r="D4" s="35" t="s">
+        <v>29</v>
+      </c>
+      <c r="E4" s="35" t="s">
+        <v>29</v>
+      </c>
+      <c r="F4" s="35" t="s">
+        <v>29</v>
+      </c>
+      <c r="G4" s="35"/>
+      <c r="H4" s="35"/>
+      <c r="I4" s="35"/>
+      <c r="J4" s="35"/>
+      <c r="K4" s="35"/>
+      <c r="L4" s="35"/>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="33" t="s">
+      <c r="A5" s="32" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="33" t="n">
+      <c r="B5" s="32" t="n">
         <f aca="false">SUMIF(C5:L5,A$12,C$3:Z$3)</f>
         <v>3</v>
       </c>
-      <c r="C5" s="36" t="s">
-        <v>29</v>
-      </c>
-      <c r="D5" s="36"/>
-      <c r="E5" s="36" t="s">
-        <v>29</v>
-      </c>
-      <c r="F5" s="36" t="s">
-        <v>29</v>
-      </c>
-      <c r="G5" s="36"/>
-      <c r="J5" s="36"/>
-      <c r="K5" s="36"/>
-      <c r="L5" s="36"/>
+      <c r="C5" s="35" t="s">
+        <v>29</v>
+      </c>
+      <c r="D5" s="35"/>
+      <c r="E5" s="35" t="s">
+        <v>29</v>
+      </c>
+      <c r="F5" s="35" t="s">
+        <v>29</v>
+      </c>
+      <c r="G5" s="35"/>
+      <c r="J5" s="35"/>
+      <c r="K5" s="35"/>
+      <c r="L5" s="35"/>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="33" t="s">
+      <c r="A6" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="B6" s="33" t="n">
+      <c r="B6" s="32" t="n">
         <f aca="false">SUMIF(C6:L6,A$12,C$3:Z$3)</f>
         <v>3.5</v>
       </c>
-      <c r="C6" s="36" t="s">
-        <v>29</v>
-      </c>
-      <c r="D6" s="36" t="s">
-        <v>29</v>
-      </c>
-      <c r="E6" s="36" t="s">
-        <v>29</v>
-      </c>
-      <c r="F6" s="36" t="s">
-        <v>29</v>
-      </c>
-      <c r="G6" s="36"/>
-      <c r="H6" s="36"/>
-      <c r="I6" s="36"/>
-      <c r="J6" s="36"/>
-      <c r="K6" s="36"/>
-      <c r="L6" s="36"/>
+      <c r="C6" s="35" t="s">
+        <v>29</v>
+      </c>
+      <c r="D6" s="35" t="s">
+        <v>29</v>
+      </c>
+      <c r="E6" s="35" t="s">
+        <v>29</v>
+      </c>
+      <c r="F6" s="35" t="s">
+        <v>29</v>
+      </c>
+      <c r="G6" s="35"/>
+      <c r="H6" s="35"/>
+      <c r="I6" s="35"/>
+      <c r="J6" s="35"/>
+      <c r="K6" s="35"/>
+      <c r="L6" s="35"/>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="33" t="s">
+      <c r="A7" s="32" t="s">
         <v>10</v>
       </c>
-      <c r="B7" s="33" t="n">
+      <c r="B7" s="32" t="n">
         <f aca="false">SUMIF(C7:L7,A$12,C$3:Z$3)</f>
         <v>3.5</v>
       </c>
-      <c r="C7" s="36" t="s">
-        <v>29</v>
-      </c>
-      <c r="D7" s="36" t="s">
-        <v>29</v>
-      </c>
-      <c r="E7" s="36" t="s">
-        <v>29</v>
-      </c>
-      <c r="F7" s="36" t="s">
-        <v>29</v>
-      </c>
-      <c r="G7" s="36"/>
-      <c r="H7" s="36"/>
-      <c r="I7" s="36"/>
-      <c r="J7" s="36"/>
-      <c r="K7" s="36"/>
-      <c r="L7" s="36"/>
+      <c r="C7" s="35" t="s">
+        <v>29</v>
+      </c>
+      <c r="D7" s="35" t="s">
+        <v>29</v>
+      </c>
+      <c r="E7" s="35" t="s">
+        <v>29</v>
+      </c>
+      <c r="F7" s="35" t="s">
+        <v>29</v>
+      </c>
+      <c r="G7" s="35"/>
+      <c r="H7" s="35"/>
+      <c r="I7" s="35"/>
+      <c r="J7" s="35"/>
+      <c r="K7" s="35"/>
+      <c r="L7" s="35"/>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="33" t="s">
+      <c r="A8" s="32" t="s">
         <v>11</v>
       </c>
-      <c r="B8" s="33" t="n">
+      <c r="B8" s="32" t="n">
         <f aca="false">SUMIF(C8:L8,A$12,C$3:Z$3)</f>
         <v>3.5</v>
       </c>
-      <c r="C8" s="36" t="s">
-        <v>29</v>
-      </c>
-      <c r="D8" s="36" t="s">
-        <v>29</v>
-      </c>
-      <c r="E8" s="36" t="s">
-        <v>29</v>
-      </c>
-      <c r="F8" s="36" t="s">
+      <c r="C8" s="35" t="s">
+        <v>29</v>
+      </c>
+      <c r="D8" s="35" t="s">
+        <v>29</v>
+      </c>
+      <c r="E8" s="35" t="s">
+        <v>29</v>
+      </c>
+      <c r="F8" s="35" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="33" t="s">
+      <c r="A9" s="32" t="s">
         <v>12</v>
       </c>
-      <c r="B9" s="33" t="n">
+      <c r="B9" s="32" t="n">
         <f aca="false">SUMIF(C9:L9,A$12,C$3:Z$3)</f>
         <v>2</v>
       </c>
-      <c r="D9" s="36" t="s">
-        <v>29</v>
-      </c>
-      <c r="E9" s="36" t="s">
-        <v>29</v>
-      </c>
-      <c r="F9" s="36" t="s">
+      <c r="D9" s="35" t="s">
+        <v>29</v>
+      </c>
+      <c r="E9" s="35" t="s">
+        <v>29</v>
+      </c>
+      <c r="F9" s="35" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="33" t="s">
-        <v>0</v>
-      </c>
-      <c r="B10" s="33" t="n">
+      <c r="A10" s="32" t="s">
+        <v>0</v>
+      </c>
+      <c r="B10" s="32" t="n">
         <f aca="false">SUM(B4:B7)</f>
         <v>13.5</v>
       </c>
-      <c r="C10" s="33" t="n">
+      <c r="C10" s="32" t="n">
         <f aca="false">COUNTIF(C4:C7,"*ü*") * C3</f>
         <v>6</v>
       </c>
-      <c r="D10" s="33" t="n">
+      <c r="D10" s="32" t="n">
         <f aca="false">COUNTIF(D4:D7,"*ü*") * D3</f>
         <v>1.5</v>
       </c>
-      <c r="E10" s="33" t="n">
+      <c r="E10" s="32" t="n">
         <f aca="false">COUNTIF(E4:E7,"*ü*") * E3</f>
         <v>2</v>
       </c>
-      <c r="F10" s="33" t="n">
+      <c r="F10" s="32" t="n">
         <f aca="false">COUNTIF(F4:F7,"*ü*") * F3</f>
         <v>4</v>
       </c>
-      <c r="G10" s="33" t="n">
+      <c r="G10" s="32" t="n">
         <f aca="false">COUNTIF(G4:G7,"*ü*") * G3</f>
         <v>0</v>
       </c>
-      <c r="H10" s="33" t="n">
+      <c r="H10" s="32" t="n">
         <f aca="false">COUNTIF(H4:H7,"*ü*") * H3</f>
         <v>0</v>
       </c>
-      <c r="I10" s="33" t="n">
+      <c r="I10" s="32" t="n">
         <f aca="false">COUNTIF(I4:I7,"*ü*") * I3</f>
         <v>0</v>
       </c>
-      <c r="J10" s="33" t="n">
+      <c r="J10" s="32" t="n">
         <f aca="false">COUNTIF(J4:J7,"*ü*") * J3</f>
         <v>0</v>
       </c>
-      <c r="K10" s="33" t="n">
+      <c r="K10" s="32" t="n">
         <f aca="false">COUNTIF(K4:K7,"*ü*") * K3</f>
         <v>0</v>
       </c>
-      <c r="L10" s="33" t="n">
+      <c r="L10" s="32" t="n">
         <f aca="false">COUNTIF(L4:L7,"*ü*") * L3</f>
         <v>0</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="6"/>
-    </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="36" t="s">
+      <c r="A12" s="35" t="s">
         <v>29</v>
       </c>
     </row>
@@ -1689,8 +1671,8 @@
   </sheetPr>
   <dimension ref="A1:S32"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D34" activeCellId="0" sqref="D34"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C5" activeCellId="0" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1704,14 +1686,14 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="37"/>
-      <c r="B1" s="38" t="s">
+      <c r="A1" s="36"/>
+      <c r="B1" s="37" t="s">
         <v>30</v>
       </c>
-      <c r="C1" s="38" t="s">
+      <c r="C1" s="37" t="s">
         <v>31</v>
       </c>
-      <c r="D1" s="39" t="s">
+      <c r="D1" s="38" t="s">
         <v>32</v>
       </c>
       <c r="E1" s="0" t="n">
@@ -1767,50 +1749,51 @@
       <c r="B2" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="C2" s="40"/>
-      <c r="D2" s="41"/>
-      <c r="E2" s="6"/>
-      <c r="F2" s="6"/>
+      <c r="C2" s="39"/>
+      <c r="D2" s="40"/>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B3" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="D3" s="41"/>
-      <c r="E3" s="6"/>
-      <c r="F3" s="6"/>
+      <c r="C3" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D3" s="40" t="n">
+        <v>0.75</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B4" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="D4" s="41"/>
-      <c r="E4" s="6"/>
-      <c r="F4" s="6"/>
+      <c r="C4" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="D4" s="40"/>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B5" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="D5" s="41"/>
-      <c r="E5" s="6"/>
-      <c r="F5" s="6"/>
+      <c r="C5" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D5" s="40"/>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="42"/>
+      <c r="A6" s="41"/>
       <c r="B6" s="4" t="s">
         <v>37</v>
       </c>
       <c r="C6" s="4" t="n">
         <f aca="false">SUM(C2:C5)</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="D6" s="5" t="n">
         <f aca="false">SUM(D2:D5)</f>
-        <v>0</v>
-      </c>
-      <c r="E6" s="6"/>
-      <c r="F6" s="6"/>
+        <v>0.75</v>
+      </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="3" t="s">
@@ -1819,33 +1802,29 @@
       <c r="B7" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="C7" s="40"/>
-      <c r="D7" s="41"/>
-      <c r="E7" s="6"/>
-      <c r="F7" s="6"/>
+      <c r="C7" s="39"/>
+      <c r="D7" s="40"/>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B8" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="D8" s="41"/>
-      <c r="E8" s="6"/>
-      <c r="F8" s="6"/>
+        <v>38</v>
+      </c>
+      <c r="D8" s="40"/>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B9" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="D9" s="41"/>
+      <c r="D9" s="40"/>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B10" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="D10" s="41"/>
+      <c r="D10" s="40"/>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="42"/>
+      <c r="A11" s="41"/>
       <c r="B11" s="4" t="s">
         <v>37</v>
       </c>
@@ -1865,30 +1844,30 @@
       <c r="B12" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="C12" s="40"/>
-      <c r="D12" s="41"/>
+      <c r="C12" s="39"/>
+      <c r="D12" s="40"/>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B13" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="D13" s="41"/>
+        <v>38</v>
+      </c>
+      <c r="D13" s="40"/>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B14" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="D14" s="41"/>
+      <c r="D14" s="40"/>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B15" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="D15" s="41"/>
+      <c r="D15" s="40"/>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="42"/>
-      <c r="B16" s="43" t="s">
+      <c r="A16" s="41"/>
+      <c r="B16" s="42" t="s">
         <v>37</v>
       </c>
       <c r="C16" s="4" t="n">
@@ -1907,30 +1886,30 @@
       <c r="B17" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="C17" s="40"/>
-      <c r="D17" s="41"/>
+      <c r="C17" s="39"/>
+      <c r="D17" s="40"/>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B18" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="D18" s="41"/>
+        <v>38</v>
+      </c>
+      <c r="D18" s="40"/>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B19" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="D19" s="41"/>
+      <c r="D19" s="40"/>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B20" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="D20" s="41"/>
+      <c r="D20" s="40"/>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="42"/>
-      <c r="B21" s="43" t="s">
+      <c r="A21" s="41"/>
+      <c r="B21" s="42" t="s">
         <v>37</v>
       </c>
       <c r="C21" s="4" t="n">
@@ -1949,28 +1928,28 @@
       <c r="B22" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="D22" s="41"/>
+      <c r="D22" s="40"/>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B23" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="D23" s="41"/>
+        <v>38</v>
+      </c>
+      <c r="D23" s="40"/>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B24" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="D24" s="41"/>
+      <c r="D24" s="40"/>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B25" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="D25" s="41"/>
+      <c r="D25" s="40"/>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B26" s="43" t="s">
+      <c r="B26" s="42" t="s">
         <v>37</v>
       </c>
       <c r="C26" s="4" t="n">
@@ -1989,28 +1968,28 @@
       <c r="B27" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="D27" s="41"/>
+      <c r="D27" s="40"/>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B28" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="D28" s="41"/>
+        <v>38</v>
+      </c>
+      <c r="D28" s="40"/>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B29" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="D29" s="41"/>
+      <c r="D29" s="40"/>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B30" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="D30" s="41"/>
+      <c r="D30" s="40"/>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B31" s="43" t="s">
+      <c r="B31" s="42" t="s">
         <v>37</v>
       </c>
       <c r="C31" s="4" t="n">
@@ -2023,17 +2002,17 @@
       </c>
     </row>
     <row r="32" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="44"/>
-      <c r="B32" s="45" t="s">
-        <v>0</v>
-      </c>
-      <c r="C32" s="8" t="n">
+      <c r="A32" s="43"/>
+      <c r="B32" s="44" t="s">
+        <v>0</v>
+      </c>
+      <c r="C32" s="7" t="n">
         <f aca="false">SUM(C6,C11,C16,C21,C26,C31)</f>
-        <v>0</v>
-      </c>
-      <c r="D32" s="9" t="n">
+        <v>5</v>
+      </c>
+      <c r="D32" s="8" t="n">
         <f aca="false">SUM(D6,D11,D16,D21,D26,D31)</f>
-        <v>0</v>
+        <v>0.75</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added today's meeting to gantt chart
</commit_message>
<xml_diff>
--- a/docs/ganttChart.xlsx
+++ b/docs/ganttChart.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Management Summary" sheetId="1" state="visible" r:id="rId2"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="39">
   <si>
     <t xml:space="preserve">Total</t>
   </si>
@@ -146,11 +146,12 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="4">
+  <numFmts count="5">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="\$#,##0.00_);[RED]&quot;($&quot;#,##0.00\)"/>
     <numFmt numFmtId="166" formatCode="\$#,##0.00;[RED]\$#,##0.00"/>
     <numFmt numFmtId="167" formatCode="D\-MMM\-YY"/>
+    <numFmt numFmtId="168" formatCode="MM/DD/YY"/>
   </numFmts>
   <fonts count="6">
     <font>
@@ -352,7 +353,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="46">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -486,6 +487,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="167" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="168" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -613,7 +618,7 @@
   <dimension ref="B1:Q10"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E8" activeCellId="0" sqref="E8"/>
+      <selection pane="topLeft" activeCell="E8" activeCellId="1" sqref="G9 E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -709,11 +714,11 @@
       </c>
       <c r="D4" s="11" t="n">
         <f aca="false">(H4+L4+P4)</f>
-        <v>425</v>
+        <v>475</v>
       </c>
       <c r="E4" s="12" t="n">
         <f aca="false">(C4-D4)</f>
-        <v>1075</v>
+        <v>1025</v>
       </c>
       <c r="G4" s="13" t="n">
         <v>0</v>
@@ -730,11 +735,11 @@
       </c>
       <c r="L4" s="11" t="n">
         <f aca="false">Meetings!B4*100</f>
-        <v>350</v>
+        <v>400</v>
       </c>
       <c r="M4" s="12" t="n">
         <f aca="false">(K4-L4)</f>
-        <v>650</v>
+        <v>600</v>
       </c>
       <c r="O4" s="10" t="n">
         <f aca="false">(SA!C6)*100</f>
@@ -759,11 +764,11 @@
       </c>
       <c r="D5" s="14" t="n">
         <f aca="false">(H5+L5+P5)</f>
-        <v>300</v>
+        <v>350</v>
       </c>
       <c r="E5" s="15" t="n">
         <f aca="false">(C5-D5)</f>
-        <v>700</v>
+        <v>650</v>
       </c>
       <c r="G5" s="13" t="n">
         <v>0</v>
@@ -780,11 +785,11 @@
       </c>
       <c r="L5" s="14" t="n">
         <f aca="false">Meetings!B5*100</f>
-        <v>300</v>
+        <v>350</v>
       </c>
       <c r="M5" s="15" t="n">
         <f aca="false">(K5-L5)</f>
-        <v>700</v>
+        <v>650</v>
       </c>
       <c r="O5" s="13" t="n">
         <f aca="false">(SA!C11)*100</f>
@@ -809,11 +814,11 @@
       </c>
       <c r="D6" s="14" t="n">
         <f aca="false">(H6+L6+P6)</f>
-        <v>350</v>
+        <v>400</v>
       </c>
       <c r="E6" s="15" t="n">
         <f aca="false">(C6-D6)</f>
-        <v>650</v>
+        <v>600</v>
       </c>
       <c r="G6" s="13" t="n">
         <v>0</v>
@@ -830,11 +835,11 @@
       </c>
       <c r="L6" s="14" t="n">
         <f aca="false">Meetings!B6*100</f>
-        <v>350</v>
+        <v>400</v>
       </c>
       <c r="M6" s="15" t="n">
         <f aca="false">(K6-L6)</f>
-        <v>650</v>
+        <v>600</v>
       </c>
       <c r="O6" s="13" t="n">
         <f aca="false">(SA!C16)*100</f>
@@ -859,11 +864,11 @@
       </c>
       <c r="D7" s="14" t="n">
         <f aca="false">(H7+L7+P7)</f>
-        <v>350</v>
+        <v>400</v>
       </c>
       <c r="E7" s="15" t="n">
         <f aca="false">(C7-D7)</f>
-        <v>650</v>
+        <v>600</v>
       </c>
       <c r="G7" s="13" t="n">
         <v>0</v>
@@ -880,11 +885,11 @@
       </c>
       <c r="L7" s="14" t="n">
         <f aca="false">Meetings!B7*100</f>
-        <v>350</v>
+        <v>400</v>
       </c>
       <c r="M7" s="15" t="n">
         <f aca="false">(K7-L7)</f>
-        <v>650</v>
+        <v>600</v>
       </c>
       <c r="O7" s="13" t="n">
         <f aca="false">(SA!C26)*100</f>
@@ -909,11 +914,11 @@
       </c>
       <c r="D8" s="14" t="n">
         <f aca="false">(H8+L8+P8)</f>
-        <v>350</v>
+        <v>400</v>
       </c>
       <c r="E8" s="15" t="n">
         <f aca="false">(C8-D8)</f>
-        <v>650</v>
+        <v>600</v>
       </c>
       <c r="G8" s="13" t="n">
         <v>0</v>
@@ -930,11 +935,11 @@
       </c>
       <c r="L8" s="14" t="n">
         <f aca="false">Meetings!B8*100</f>
-        <v>350</v>
+        <v>400</v>
       </c>
       <c r="M8" s="15" t="n">
         <f aca="false">(K8-L8)</f>
-        <v>650</v>
+        <v>600</v>
       </c>
       <c r="O8" s="13" t="n">
         <v>0</v>
@@ -957,11 +962,11 @@
       </c>
       <c r="D9" s="14" t="n">
         <f aca="false">(H9+L9+P9)</f>
-        <v>200</v>
+        <v>250</v>
       </c>
       <c r="E9" s="17" t="n">
         <f aca="false">(C9-D9)</f>
-        <v>800</v>
+        <v>750</v>
       </c>
       <c r="G9" s="13" t="n">
         <v>0</v>
@@ -978,11 +983,11 @@
       </c>
       <c r="L9" s="14" t="n">
         <f aca="false">Meetings!B9*100</f>
-        <v>200</v>
+        <v>250</v>
       </c>
       <c r="M9" s="15" t="n">
         <f aca="false">(K9-L9)</f>
-        <v>800</v>
+        <v>750</v>
       </c>
       <c r="O9" s="13" t="n">
         <v>0</v>
@@ -1005,11 +1010,11 @@
       </c>
       <c r="D10" s="21" t="n">
         <f aca="false">SUM(D4:D9)</f>
-        <v>1975</v>
+        <v>2275</v>
       </c>
       <c r="E10" s="22" t="n">
         <f aca="false">SUM(E4:E9)</f>
-        <v>4525</v>
+        <v>4225</v>
       </c>
       <c r="G10" s="20" t="n">
         <f aca="false">SUM(G5:G9)</f>
@@ -1029,11 +1034,11 @@
       </c>
       <c r="L10" s="21" t="n">
         <f aca="false">SUM(L5:L9)</f>
-        <v>1550</v>
+        <v>1800</v>
       </c>
       <c r="M10" s="22" t="n">
         <f aca="false">SUM(M5:M9)</f>
-        <v>3450</v>
+        <v>3200</v>
       </c>
       <c r="O10" s="23" t="n">
         <f aca="false">SUM(O5:O9)</f>
@@ -1073,7 +1078,7 @@
   <dimension ref="A1:AD55"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E4" activeCellId="0" sqref="E4"/>
+      <selection pane="topLeft" activeCell="E4" activeCellId="1" sqref="G9 E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1342,8 +1347,8 @@
   </sheetPr>
   <dimension ref="A1:L12"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F4" activeCellId="0" sqref="F4"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G9" activeCellId="0" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1367,8 +1372,8 @@
       <c r="F1" s="33" t="n">
         <v>43497</v>
       </c>
-      <c r="G1" s="32" t="s">
-        <v>24</v>
+      <c r="G1" s="34" t="n">
+        <v>43502</v>
       </c>
       <c r="H1" s="32" t="s">
         <v>24</v>
@@ -1390,34 +1395,34 @@
       <c r="B2" s="32" t="s">
         <v>25</v>
       </c>
-      <c r="C2" s="34" t="s">
+      <c r="C2" s="35" t="s">
         <v>26</v>
       </c>
-      <c r="D2" s="34" t="s">
+      <c r="D2" s="35" t="s">
         <v>27</v>
       </c>
-      <c r="E2" s="34" t="s">
+      <c r="E2" s="35" t="s">
         <v>27</v>
       </c>
-      <c r="F2" s="34" t="s">
+      <c r="F2" s="35" t="s">
         <v>27</v>
       </c>
-      <c r="G2" s="34" t="s">
+      <c r="G2" s="35" t="s">
         <v>24</v>
       </c>
-      <c r="H2" s="34" t="s">
+      <c r="H2" s="35" t="s">
         <v>24</v>
       </c>
-      <c r="I2" s="34" t="s">
+      <c r="I2" s="35" t="s">
         <v>24</v>
       </c>
-      <c r="J2" s="34" t="s">
+      <c r="J2" s="35" t="s">
         <v>24</v>
       </c>
-      <c r="K2" s="34" t="s">
+      <c r="K2" s="35" t="s">
         <v>24</v>
       </c>
-      <c r="L2" s="34" t="s">
+      <c r="L2" s="35" t="s">
         <v>24</v>
       </c>
     </row>
@@ -1438,7 +1443,7 @@
         <v>1</v>
       </c>
       <c r="G3" s="32" t="n">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="H3" s="32" t="n">
         <v>0</v>
@@ -1456,146 +1461,160 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="32" t="s">
         <v>7</v>
       </c>
       <c r="B4" s="32" t="n">
         <f aca="false">SUMIF(C4:L4,A$12,C$3:Z$3)</f>
-        <v>3.5</v>
-      </c>
-      <c r="C4" s="35" t="s">
-        <v>29</v>
-      </c>
-      <c r="D4" s="35" t="s">
-        <v>29</v>
-      </c>
-      <c r="E4" s="35" t="s">
-        <v>29</v>
-      </c>
-      <c r="F4" s="35" t="s">
-        <v>29</v>
-      </c>
-      <c r="G4" s="35"/>
-      <c r="H4" s="35"/>
-      <c r="I4" s="35"/>
-      <c r="J4" s="35"/>
-      <c r="K4" s="35"/>
-      <c r="L4" s="35"/>
-    </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>4</v>
+      </c>
+      <c r="C4" s="36" t="s">
+        <v>29</v>
+      </c>
+      <c r="D4" s="36" t="s">
+        <v>29</v>
+      </c>
+      <c r="E4" s="36" t="s">
+        <v>29</v>
+      </c>
+      <c r="F4" s="36" t="s">
+        <v>29</v>
+      </c>
+      <c r="G4" s="36" t="s">
+        <v>29</v>
+      </c>
+      <c r="H4" s="36"/>
+      <c r="I4" s="36"/>
+      <c r="J4" s="36"/>
+      <c r="K4" s="36"/>
+      <c r="L4" s="36"/>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="32" t="s">
         <v>8</v>
       </c>
       <c r="B5" s="32" t="n">
         <f aca="false">SUMIF(C5:L5,A$12,C$3:Z$3)</f>
-        <v>3</v>
-      </c>
-      <c r="C5" s="35" t="s">
-        <v>29</v>
-      </c>
-      <c r="D5" s="35"/>
-      <c r="E5" s="35" t="s">
-        <v>29</v>
-      </c>
-      <c r="F5" s="35" t="s">
-        <v>29</v>
-      </c>
-      <c r="G5" s="35"/>
-      <c r="J5" s="35"/>
-      <c r="K5" s="35"/>
-      <c r="L5" s="35"/>
-    </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>3.5</v>
+      </c>
+      <c r="C5" s="36" t="s">
+        <v>29</v>
+      </c>
+      <c r="D5" s="36"/>
+      <c r="E5" s="36" t="s">
+        <v>29</v>
+      </c>
+      <c r="F5" s="36" t="s">
+        <v>29</v>
+      </c>
+      <c r="G5" s="36" t="s">
+        <v>29</v>
+      </c>
+      <c r="J5" s="36"/>
+      <c r="K5" s="36"/>
+      <c r="L5" s="36"/>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="32" t="s">
         <v>9</v>
       </c>
       <c r="B6" s="32" t="n">
         <f aca="false">SUMIF(C6:L6,A$12,C$3:Z$3)</f>
-        <v>3.5</v>
-      </c>
-      <c r="C6" s="35" t="s">
-        <v>29</v>
-      </c>
-      <c r="D6" s="35" t="s">
-        <v>29</v>
-      </c>
-      <c r="E6" s="35" t="s">
-        <v>29</v>
-      </c>
-      <c r="F6" s="35" t="s">
-        <v>29</v>
-      </c>
-      <c r="G6" s="35"/>
-      <c r="H6" s="35"/>
-      <c r="I6" s="35"/>
-      <c r="J6" s="35"/>
-      <c r="K6" s="35"/>
-      <c r="L6" s="35"/>
-    </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>4</v>
+      </c>
+      <c r="C6" s="36" t="s">
+        <v>29</v>
+      </c>
+      <c r="D6" s="36" t="s">
+        <v>29</v>
+      </c>
+      <c r="E6" s="36" t="s">
+        <v>29</v>
+      </c>
+      <c r="F6" s="36" t="s">
+        <v>29</v>
+      </c>
+      <c r="G6" s="36" t="s">
+        <v>29</v>
+      </c>
+      <c r="H6" s="36"/>
+      <c r="I6" s="36"/>
+      <c r="J6" s="36"/>
+      <c r="K6" s="36"/>
+      <c r="L6" s="36"/>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="32" t="s">
         <v>10</v>
       </c>
       <c r="B7" s="32" t="n">
         <f aca="false">SUMIF(C7:L7,A$12,C$3:Z$3)</f>
-        <v>3.5</v>
-      </c>
-      <c r="C7" s="35" t="s">
-        <v>29</v>
-      </c>
-      <c r="D7" s="35" t="s">
-        <v>29</v>
-      </c>
-      <c r="E7" s="35" t="s">
-        <v>29</v>
-      </c>
-      <c r="F7" s="35" t="s">
-        <v>29</v>
-      </c>
-      <c r="G7" s="35"/>
-      <c r="H7" s="35"/>
-      <c r="I7" s="35"/>
-      <c r="J7" s="35"/>
-      <c r="K7" s="35"/>
-      <c r="L7" s="35"/>
-    </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>4</v>
+      </c>
+      <c r="C7" s="36" t="s">
+        <v>29</v>
+      </c>
+      <c r="D7" s="36" t="s">
+        <v>29</v>
+      </c>
+      <c r="E7" s="36" t="s">
+        <v>29</v>
+      </c>
+      <c r="F7" s="36" t="s">
+        <v>29</v>
+      </c>
+      <c r="G7" s="36" t="s">
+        <v>29</v>
+      </c>
+      <c r="H7" s="36"/>
+      <c r="I7" s="36"/>
+      <c r="J7" s="36"/>
+      <c r="K7" s="36"/>
+      <c r="L7" s="36"/>
+    </row>
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="32" t="s">
         <v>11</v>
       </c>
       <c r="B8" s="32" t="n">
         <f aca="false">SUMIF(C8:L8,A$12,C$3:Z$3)</f>
-        <v>3.5</v>
-      </c>
-      <c r="C8" s="35" t="s">
-        <v>29</v>
-      </c>
-      <c r="D8" s="35" t="s">
-        <v>29</v>
-      </c>
-      <c r="E8" s="35" t="s">
-        <v>29</v>
-      </c>
-      <c r="F8" s="35" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>4</v>
+      </c>
+      <c r="C8" s="36" t="s">
+        <v>29</v>
+      </c>
+      <c r="D8" s="36" t="s">
+        <v>29</v>
+      </c>
+      <c r="E8" s="36" t="s">
+        <v>29</v>
+      </c>
+      <c r="F8" s="36" t="s">
+        <v>29</v>
+      </c>
+      <c r="G8" s="36" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="32" t="s">
         <v>12</v>
       </c>
       <c r="B9" s="32" t="n">
         <f aca="false">SUMIF(C9:L9,A$12,C$3:Z$3)</f>
-        <v>2</v>
-      </c>
-      <c r="D9" s="35" t="s">
-        <v>29</v>
-      </c>
-      <c r="E9" s="35" t="s">
-        <v>29</v>
-      </c>
-      <c r="F9" s="35" t="s">
+        <v>2.5</v>
+      </c>
+      <c r="D9" s="36" t="s">
+        <v>29</v>
+      </c>
+      <c r="E9" s="36" t="s">
+        <v>29</v>
+      </c>
+      <c r="F9" s="36" t="s">
+        <v>29</v>
+      </c>
+      <c r="G9" s="36" t="s">
         <v>29</v>
       </c>
     </row>
@@ -1605,7 +1624,7 @@
       </c>
       <c r="B10" s="32" t="n">
         <f aca="false">SUM(B4:B7)</f>
-        <v>13.5</v>
+        <v>15.5</v>
       </c>
       <c r="C10" s="32" t="n">
         <f aca="false">COUNTIF(C4:C7,"*ü*") * C3</f>
@@ -1625,7 +1644,7 @@
       </c>
       <c r="G10" s="32" t="n">
         <f aca="false">COUNTIF(G4:G7,"*ü*") * G3</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H10" s="32" t="n">
         <f aca="false">COUNTIF(H4:H7,"*ü*") * H3</f>
@@ -1649,7 +1668,7 @@
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="35" t="s">
+      <c r="A12" s="36" t="s">
         <v>29</v>
       </c>
     </row>
@@ -1671,8 +1690,8 @@
   </sheetPr>
   <dimension ref="A1:S32"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C5" activeCellId="0" sqref="C5"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C5" activeCellId="1" sqref="G9 C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1686,14 +1705,14 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="36"/>
-      <c r="B1" s="37" t="s">
+      <c r="A1" s="37"/>
+      <c r="B1" s="38" t="s">
         <v>30</v>
       </c>
-      <c r="C1" s="37" t="s">
+      <c r="C1" s="38" t="s">
         <v>31</v>
       </c>
-      <c r="D1" s="38" t="s">
+      <c r="D1" s="39" t="s">
         <v>32</v>
       </c>
       <c r="E1" s="0" t="n">
@@ -1749,8 +1768,8 @@
       <c r="B2" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="C2" s="39"/>
-      <c r="D2" s="40"/>
+      <c r="C2" s="40"/>
+      <c r="D2" s="41"/>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B3" s="4" t="s">
@@ -1759,7 +1778,7 @@
       <c r="C3" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="D3" s="40" t="n">
+      <c r="D3" s="41" t="n">
         <v>0.75</v>
       </c>
     </row>
@@ -1770,7 +1789,7 @@
       <c r="C4" s="0" t="n">
         <v>3</v>
       </c>
-      <c r="D4" s="40"/>
+      <c r="D4" s="41"/>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B5" s="4" t="s">
@@ -1779,10 +1798,10 @@
       <c r="C5" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="D5" s="40"/>
+      <c r="D5" s="41"/>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="41"/>
+      <c r="A6" s="42"/>
       <c r="B6" s="4" t="s">
         <v>37</v>
       </c>
@@ -1802,29 +1821,29 @@
       <c r="B7" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="C7" s="39"/>
-      <c r="D7" s="40"/>
+      <c r="C7" s="40"/>
+      <c r="D7" s="41"/>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B8" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="D8" s="40"/>
+      <c r="D8" s="41"/>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B9" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="D9" s="40"/>
+      <c r="D9" s="41"/>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B10" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="D10" s="40"/>
+      <c r="D10" s="41"/>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="41"/>
+      <c r="A11" s="42"/>
       <c r="B11" s="4" t="s">
         <v>37</v>
       </c>
@@ -1844,30 +1863,30 @@
       <c r="B12" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="C12" s="39"/>
-      <c r="D12" s="40"/>
+      <c r="C12" s="40"/>
+      <c r="D12" s="41"/>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B13" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="D13" s="40"/>
+      <c r="D13" s="41"/>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B14" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="D14" s="40"/>
+      <c r="D14" s="41"/>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B15" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="D15" s="40"/>
+      <c r="D15" s="41"/>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="41"/>
-      <c r="B16" s="42" t="s">
+      <c r="A16" s="42"/>
+      <c r="B16" s="43" t="s">
         <v>37</v>
       </c>
       <c r="C16" s="4" t="n">
@@ -1886,30 +1905,30 @@
       <c r="B17" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="C17" s="39"/>
-      <c r="D17" s="40"/>
+      <c r="C17" s="40"/>
+      <c r="D17" s="41"/>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B18" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="D18" s="40"/>
+      <c r="D18" s="41"/>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B19" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="D19" s="40"/>
+      <c r="D19" s="41"/>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B20" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="D20" s="40"/>
+      <c r="D20" s="41"/>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="41"/>
-      <c r="B21" s="42" t="s">
+      <c r="A21" s="42"/>
+      <c r="B21" s="43" t="s">
         <v>37</v>
       </c>
       <c r="C21" s="4" t="n">
@@ -1928,28 +1947,28 @@
       <c r="B22" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="D22" s="40"/>
+      <c r="D22" s="41"/>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B23" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="D23" s="40"/>
+      <c r="D23" s="41"/>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B24" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="D24" s="40"/>
+      <c r="D24" s="41"/>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B25" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="D25" s="40"/>
+      <c r="D25" s="41"/>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B26" s="42" t="s">
+      <c r="B26" s="43" t="s">
         <v>37</v>
       </c>
       <c r="C26" s="4" t="n">
@@ -1968,28 +1987,28 @@
       <c r="B27" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="D27" s="40"/>
+      <c r="D27" s="41"/>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B28" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="D28" s="40"/>
+      <c r="D28" s="41"/>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B29" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="D29" s="40"/>
+      <c r="D29" s="41"/>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B30" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="D30" s="40"/>
+      <c r="D30" s="41"/>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B31" s="42" t="s">
+      <c r="B31" s="43" t="s">
         <v>37</v>
       </c>
       <c r="C31" s="4" t="n">
@@ -2002,8 +2021,8 @@
       </c>
     </row>
     <row r="32" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="43"/>
-      <c r="B32" s="44" t="s">
+      <c r="A32" s="44"/>
+      <c r="B32" s="45" t="s">
         <v>0</v>
       </c>
       <c r="C32" s="7" t="n">

</xml_diff>

<commit_message>
Added presentation slides & champion
</commit_message>
<xml_diff>
--- a/docs/ganttChart.xlsx
+++ b/docs/ganttChart.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11015"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\cs383 banana\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/blakelyfrechette/Documents/School/banana/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6626945-49C5-4572-94AA-9BC9ECE70F53}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6137DEFD-5402-9540-B634-4186ACC9319F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="28035" windowHeight="16440" tabRatio="500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="980" yWindow="0" windowWidth="27820" windowHeight="16440" tabRatio="500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Management Summary" sheetId="1" r:id="rId1"/>
@@ -18,14 +18,8 @@
     <sheet name="Meetings" sheetId="3" r:id="rId3"/>
     <sheet name="SA" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="191029" iterateDelta="1E-4"/>
+  <calcPr calcId="179021" iterateDelta="1E-4"/>
   <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-      </xcalcf:calcFeatures>
-    </ext>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
     </ext>
@@ -376,9 +370,6 @@
   </cellStyleXfs>
   <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -427,6 +418,9 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -815,433 +809,433 @@
       <selection activeCell="E8" activeCellId="1" sqref="G9 E8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="2" width="8.42578125" customWidth="1"/>
-    <col min="3" max="3" width="14.28515625" customWidth="1"/>
-    <col min="4" max="4" width="13.85546875" customWidth="1"/>
-    <col min="5" max="5" width="13.28515625" customWidth="1"/>
-    <col min="6" max="6" width="3.42578125" customWidth="1"/>
-    <col min="7" max="7" width="15.28515625" customWidth="1"/>
-    <col min="8" max="8" width="12.28515625" customWidth="1"/>
-    <col min="9" max="9" width="14.5703125" customWidth="1"/>
-    <col min="10" max="10" width="2.85546875" customWidth="1"/>
-    <col min="11" max="11" width="13.85546875" customWidth="1"/>
+    <col min="1" max="2" width="8.5" customWidth="1"/>
+    <col min="3" max="3" width="14.33203125" customWidth="1"/>
+    <col min="4" max="4" width="13.83203125" customWidth="1"/>
+    <col min="5" max="5" width="13.33203125" customWidth="1"/>
+    <col min="6" max="6" width="3.5" customWidth="1"/>
+    <col min="7" max="7" width="15.33203125" customWidth="1"/>
+    <col min="8" max="8" width="12.33203125" customWidth="1"/>
+    <col min="9" max="9" width="14.5" customWidth="1"/>
+    <col min="10" max="10" width="2.83203125" customWidth="1"/>
+    <col min="11" max="11" width="13.83203125" customWidth="1"/>
     <col min="12" max="12" width="14" customWidth="1"/>
-    <col min="13" max="13" width="14.140625" customWidth="1"/>
-    <col min="14" max="14" width="5.42578125" customWidth="1"/>
-    <col min="15" max="15" width="12.28515625" customWidth="1"/>
-    <col min="16" max="16" width="14.7109375" customWidth="1"/>
-    <col min="17" max="17" width="11.28515625" customWidth="1"/>
-    <col min="18" max="1025" width="8.42578125" customWidth="1"/>
+    <col min="13" max="13" width="14.1640625" customWidth="1"/>
+    <col min="14" max="14" width="5.5" customWidth="1"/>
+    <col min="15" max="15" width="12.33203125" customWidth="1"/>
+    <col min="16" max="16" width="14.6640625" customWidth="1"/>
+    <col min="17" max="17" width="11.33203125" customWidth="1"/>
+    <col min="18" max="1025" width="8.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="C2" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
-      <c r="F2" s="2"/>
-      <c r="G2" s="1" t="s">
+    <row r="2" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="C2" s="45" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2" s="45"/>
+      <c r="E2" s="45"/>
+      <c r="F2" s="1"/>
+      <c r="G2" s="45" t="s">
         <v>1</v>
       </c>
-      <c r="H2" s="1"/>
-      <c r="I2" s="1"/>
-      <c r="K2" s="1" t="s">
+      <c r="H2" s="45"/>
+      <c r="I2" s="45"/>
+      <c r="K2" s="45" t="s">
         <v>2</v>
       </c>
-      <c r="L2" s="1"/>
-      <c r="M2" s="1"/>
-      <c r="O2" s="1" t="s">
+      <c r="L2" s="45"/>
+      <c r="M2" s="45"/>
+      <c r="O2" s="45" t="s">
         <v>3</v>
       </c>
-      <c r="P2" s="1"/>
-      <c r="Q2" s="1"/>
-    </row>
-    <row r="3" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="C3" s="3" t="s">
+      <c r="P2" s="45"/>
+      <c r="Q2" s="45"/>
+    </row>
+    <row r="3" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="C3" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="D3" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="E3" s="5" t="s">
+      <c r="E3" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="G3" s="6" t="s">
+      <c r="G3" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="H3" s="7" t="s">
+      <c r="H3" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="I3" s="8" t="s">
+      <c r="I3" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="K3" s="6" t="s">
+      <c r="K3" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="L3" s="7" t="s">
+      <c r="L3" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="M3" s="8" t="s">
+      <c r="M3" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="O3" s="3" t="s">
+      <c r="O3" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="P3" s="4" t="s">
+      <c r="P3" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="Q3" s="5" t="s">
+      <c r="Q3" s="4" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B4" s="9" t="s">
+    <row r="4" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="B4" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="10">
+      <c r="C4" s="9">
         <f t="shared" ref="C4:D8" si="0">(G4+K4+O4)</f>
         <v>1500</v>
       </c>
-      <c r="D4" s="11">
+      <c r="D4" s="10">
         <f t="shared" si="0"/>
         <v>475</v>
       </c>
-      <c r="E4" s="12">
+      <c r="E4" s="11">
         <f t="shared" ref="E4:E9" si="1">(C4-D4)</f>
         <v>1025</v>
       </c>
-      <c r="G4" s="13">
-        <v>0</v>
-      </c>
-      <c r="H4" s="14">
-        <v>0</v>
-      </c>
-      <c r="I4" s="15">
+      <c r="G4" s="12">
+        <v>0</v>
+      </c>
+      <c r="H4" s="13">
+        <v>0</v>
+      </c>
+      <c r="I4" s="14">
         <f t="shared" ref="I4:I9" si="2">(G4-H4)</f>
         <v>0</v>
       </c>
-      <c r="K4" s="10">
+      <c r="K4" s="9">
         <v>1000</v>
       </c>
-      <c r="L4" s="11">
+      <c r="L4" s="10">
         <f>Meetings!B4*100</f>
         <v>400</v>
       </c>
-      <c r="M4" s="12">
+      <c r="M4" s="11">
         <f t="shared" ref="M4:M9" si="3">(K4-L4)</f>
         <v>600</v>
       </c>
-      <c r="O4" s="10">
+      <c r="O4" s="9">
         <f>(SA!C6)*100</f>
         <v>500</v>
       </c>
-      <c r="P4" s="11">
+      <c r="P4" s="10">
         <f>(SA!D6)*100</f>
         <v>75</v>
       </c>
-      <c r="Q4" s="12">
+      <c r="Q4" s="11">
         <f t="shared" ref="Q4:Q9" si="4">(O4-P4)</f>
         <v>425</v>
       </c>
     </row>
-    <row r="5" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B5" s="3" t="s">
+    <row r="5" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="B5" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="13">
+      <c r="C5" s="12">
         <f t="shared" si="0"/>
         <v>1000</v>
       </c>
-      <c r="D5" s="14">
+      <c r="D5" s="13">
         <f t="shared" si="0"/>
         <v>350</v>
       </c>
-      <c r="E5" s="15">
+      <c r="E5" s="14">
         <f t="shared" si="1"/>
         <v>650</v>
       </c>
-      <c r="G5" s="13">
-        <v>0</v>
-      </c>
-      <c r="H5" s="14">
-        <v>0</v>
-      </c>
-      <c r="I5" s="15">
+      <c r="G5" s="12">
+        <v>0</v>
+      </c>
+      <c r="H5" s="13">
+        <v>0</v>
+      </c>
+      <c r="I5" s="14">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="K5" s="13">
+      <c r="K5" s="12">
         <v>1000</v>
       </c>
-      <c r="L5" s="14">
+      <c r="L5" s="13">
         <f>Meetings!B5*100</f>
         <v>350</v>
       </c>
-      <c r="M5" s="15">
+      <c r="M5" s="14">
         <f t="shared" si="3"/>
         <v>650</v>
       </c>
-      <c r="O5" s="13">
+      <c r="O5" s="12">
         <f>(SA!C11)*100</f>
         <v>0</v>
       </c>
-      <c r="P5" s="14">
+      <c r="P5" s="13">
         <f>(SA!D11)*100</f>
         <v>0</v>
       </c>
-      <c r="Q5" s="15">
+      <c r="Q5" s="14">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B6" s="3" t="s">
+    <row r="6" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="B6" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C6" s="13">
+      <c r="C6" s="12">
         <f t="shared" si="0"/>
         <v>1800</v>
       </c>
-      <c r="D6" s="14">
+      <c r="D6" s="13">
         <f t="shared" si="0"/>
         <v>950</v>
       </c>
-      <c r="E6" s="15">
+      <c r="E6" s="14">
         <f t="shared" si="1"/>
         <v>850</v>
       </c>
-      <c r="G6" s="13">
-        <v>0</v>
-      </c>
-      <c r="H6" s="14">
-        <v>0</v>
-      </c>
-      <c r="I6" s="15">
+      <c r="G6" s="12">
+        <v>0</v>
+      </c>
+      <c r="H6" s="13">
+        <v>0</v>
+      </c>
+      <c r="I6" s="14">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="K6" s="13">
+      <c r="K6" s="12">
         <v>1000</v>
       </c>
-      <c r="L6" s="14">
+      <c r="L6" s="13">
         <f>Meetings!B6*100</f>
         <v>400</v>
       </c>
-      <c r="M6" s="15">
+      <c r="M6" s="14">
         <f t="shared" si="3"/>
         <v>600</v>
       </c>
-      <c r="O6" s="13">
+      <c r="O6" s="12">
         <f>(SA!C16)*100</f>
         <v>800</v>
       </c>
-      <c r="P6" s="14">
+      <c r="P6" s="13">
         <f>(SA!D16)*100</f>
         <v>550</v>
       </c>
-      <c r="Q6" s="15">
+      <c r="Q6" s="14">
         <f t="shared" si="4"/>
         <v>250</v>
       </c>
     </row>
-    <row r="7" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B7" s="3" t="s">
+    <row r="7" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="B7" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C7" s="13">
+      <c r="C7" s="12">
+        <f t="shared" si="0"/>
+        <v>1600</v>
+      </c>
+      <c r="D7" s="13">
         <f t="shared" si="0"/>
         <v>1000</v>
       </c>
-      <c r="D7" s="14">
+      <c r="E7" s="14">
+        <f t="shared" si="1"/>
+        <v>600</v>
+      </c>
+      <c r="G7" s="12">
+        <v>0</v>
+      </c>
+      <c r="H7" s="13">
+        <v>0</v>
+      </c>
+      <c r="I7" s="14">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="K7" s="12">
+        <v>1000</v>
+      </c>
+      <c r="L7" s="13">
+        <f>Meetings!B7*100</f>
+        <v>400</v>
+      </c>
+      <c r="M7" s="14">
+        <f t="shared" si="3"/>
+        <v>600</v>
+      </c>
+      <c r="O7" s="12">
+        <f>(SA!C26)*100</f>
+        <v>600</v>
+      </c>
+      <c r="P7" s="13">
+        <f>(SA!D26)*100</f>
+        <v>600</v>
+      </c>
+      <c r="Q7" s="14">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="B8" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="C8" s="13">
+        <f t="shared" si="0"/>
+        <v>1000</v>
+      </c>
+      <c r="D8" s="13">
         <f t="shared" si="0"/>
         <v>400</v>
       </c>
-      <c r="E7" s="15">
+      <c r="E8" s="14">
         <f t="shared" si="1"/>
         <v>600</v>
       </c>
-      <c r="G7" s="13">
-        <v>0</v>
-      </c>
-      <c r="H7" s="14">
-        <v>0</v>
-      </c>
-      <c r="I7" s="15">
+      <c r="G8" s="12">
+        <v>0</v>
+      </c>
+      <c r="H8" s="13">
+        <v>0</v>
+      </c>
+      <c r="I8" s="14">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="K7" s="13">
+      <c r="K8" s="12">
         <v>1000</v>
       </c>
-      <c r="L7" s="14">
-        <f>Meetings!B7*100</f>
+      <c r="L8" s="13">
+        <f>Meetings!B8*100</f>
         <v>400</v>
       </c>
-      <c r="M7" s="15">
+      <c r="M8" s="14">
         <f t="shared" si="3"/>
         <v>600</v>
       </c>
-      <c r="O7" s="13">
-        <f>(SA!C26)*100</f>
-        <v>0</v>
-      </c>
-      <c r="P7" s="14">
-        <f>(SA!D26)*100</f>
-        <v>0</v>
-      </c>
-      <c r="Q7" s="15">
+      <c r="O8" s="12">
+        <v>0</v>
+      </c>
+      <c r="P8" s="13">
+        <v>0</v>
+      </c>
+      <c r="Q8" s="14">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B8" s="16" t="s">
-        <v>11</v>
-      </c>
-      <c r="C8" s="14">
-        <f t="shared" si="0"/>
-        <v>1000</v>
-      </c>
-      <c r="D8" s="14">
-        <f t="shared" si="0"/>
-        <v>400</v>
-      </c>
-      <c r="E8" s="15">
-        <f t="shared" si="1"/>
-        <v>600</v>
-      </c>
-      <c r="G8" s="13">
-        <v>0</v>
-      </c>
-      <c r="H8" s="14">
-        <v>0</v>
-      </c>
-      <c r="I8" s="15">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="K8" s="13">
-        <v>1000</v>
-      </c>
-      <c r="L8" s="14">
-        <f>Meetings!B8*100</f>
-        <v>400</v>
-      </c>
-      <c r="M8" s="15">
-        <f t="shared" si="3"/>
-        <v>600</v>
-      </c>
-      <c r="O8" s="13">
-        <v>0</v>
-      </c>
-      <c r="P8" s="14">
-        <v>0</v>
-      </c>
-      <c r="Q8" s="15">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B9" s="16" t="s">
+    <row r="9" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="B9" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="C9" s="14">
+      <c r="C9" s="13">
         <f>+(G9+K9+O9)</f>
         <v>1000</v>
       </c>
-      <c r="D9" s="14">
+      <c r="D9" s="13">
         <f>(H9+L9+P9)</f>
         <v>250</v>
       </c>
-      <c r="E9" s="17">
+      <c r="E9" s="16">
         <f t="shared" si="1"/>
         <v>750</v>
       </c>
-      <c r="G9" s="13">
-        <v>0</v>
-      </c>
-      <c r="H9" s="18">
-        <v>0</v>
-      </c>
-      <c r="I9" s="15">
+      <c r="G9" s="12">
+        <v>0</v>
+      </c>
+      <c r="H9" s="17">
+        <v>0</v>
+      </c>
+      <c r="I9" s="14">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="K9" s="19">
+      <c r="K9" s="18">
         <v>1000</v>
       </c>
-      <c r="L9" s="14">
+      <c r="L9" s="13">
         <f>Meetings!B9*100</f>
         <v>250</v>
       </c>
-      <c r="M9" s="15">
+      <c r="M9" s="14">
         <f t="shared" si="3"/>
         <v>750</v>
       </c>
-      <c r="O9" s="13">
-        <v>0</v>
-      </c>
-      <c r="P9" s="14">
-        <v>0</v>
-      </c>
-      <c r="Q9" s="15">
+      <c r="O9" s="12">
+        <v>0</v>
+      </c>
+      <c r="P9" s="13">
+        <v>0</v>
+      </c>
+      <c r="Q9" s="14">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B10" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="C10" s="20">
+    <row r="10" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="B10" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="C10" s="19">
         <f>SUM(C4:C9)</f>
-        <v>7300</v>
-      </c>
-      <c r="D10" s="21">
+        <v>7900</v>
+      </c>
+      <c r="D10" s="20">
         <f>SUM(D4:D9)</f>
-        <v>2825</v>
-      </c>
-      <c r="E10" s="22">
+        <v>3425</v>
+      </c>
+      <c r="E10" s="21">
         <f>SUM(E4:E9)</f>
         <v>4475</v>
       </c>
-      <c r="G10" s="20">
+      <c r="G10" s="19">
         <f>SUM(G5:G9)</f>
         <v>0</v>
       </c>
-      <c r="H10" s="21">
+      <c r="H10" s="20">
         <f>SUM(H5:H9)</f>
         <v>0</v>
       </c>
-      <c r="I10" s="22">
+      <c r="I10" s="21">
         <f>SUM(I5:I9)</f>
         <v>0</v>
       </c>
-      <c r="K10" s="20">
+      <c r="K10" s="19">
         <f>SUM(K5:K9)</f>
         <v>5000</v>
       </c>
-      <c r="L10" s="21">
+      <c r="L10" s="20">
         <f>SUM(L5:L9)</f>
         <v>1800</v>
       </c>
-      <c r="M10" s="22">
+      <c r="M10" s="21">
         <f>SUM(M5:M9)</f>
         <v>3200</v>
       </c>
-      <c r="O10" s="23">
+      <c r="O10" s="22">
         <f>SUM(O5:O9)</f>
-        <v>800</v>
-      </c>
-      <c r="P10" s="24">
+        <v>1400</v>
+      </c>
+      <c r="P10" s="23">
         <f>SUM(P5:P9)</f>
-        <v>550</v>
-      </c>
-      <c r="Q10" s="25">
+        <v>1150</v>
+      </c>
+      <c r="Q10" s="24">
         <f>SUM(Q5:Q9)</f>
         <v>250</v>
       </c>
@@ -1266,17 +1260,17 @@
       <selection activeCell="E4" activeCellId="1" sqref="G9 E4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="29" customWidth="1"/>
-    <col min="2" max="2" width="17.5703125" customWidth="1"/>
-    <col min="3" max="3" width="15.7109375" customWidth="1"/>
-    <col min="4" max="5" width="8.42578125" customWidth="1"/>
-    <col min="6" max="6" width="10.7109375" customWidth="1"/>
-    <col min="7" max="1025" width="8.42578125" customWidth="1"/>
+    <col min="2" max="2" width="17.5" customWidth="1"/>
+    <col min="3" max="3" width="15.6640625" customWidth="1"/>
+    <col min="4" max="5" width="8.5" customWidth="1"/>
+    <col min="6" max="6" width="10.6640625" customWidth="1"/>
+    <col min="7" max="1025" width="8.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:30" x14ac:dyDescent="0.2">
       <c r="B1" t="s">
         <v>13</v>
       </c>
@@ -1286,21 +1280,21 @@
       <c r="D1" t="s">
         <v>15</v>
       </c>
-      <c r="E1" s="26"/>
+      <c r="E1" s="25"/>
       <c r="F1" t="s">
         <v>16</v>
       </c>
-      <c r="H1" s="27"/>
+      <c r="H1" s="26"/>
       <c r="I1" t="s">
         <v>17</v>
       </c>
-      <c r="K1" s="28"/>
+      <c r="K1" s="27"/>
       <c r="L1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A2" s="29" t="s">
+    <row r="2" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="A2" s="28" t="s">
         <v>7</v>
       </c>
       <c r="D2" t="s">
@@ -1385,7 +1379,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="10" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>20</v>
       </c>
@@ -1398,12 +1392,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A11" s="30" t="s">
+    <row r="11" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="A11" s="29" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>20</v>
       </c>
@@ -1416,12 +1410,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" s="30" t="s">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A21" s="29" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>20</v>
       </c>
@@ -1434,12 +1428,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A29" s="30" t="s">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A29" s="29" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>20</v>
       </c>
@@ -1452,12 +1446,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A37" s="30" t="s">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A37" s="29" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>20</v>
       </c>
@@ -1470,12 +1464,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A46" s="30" t="s">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A46" s="29" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>20</v>
       </c>
@@ -1488,7 +1482,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>21</v>
       </c>
@@ -1501,15 +1495,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>22</v>
       </c>
-      <c r="B55" s="31">
+      <c r="B55" s="30">
         <f>B54*100</f>
         <v>0</v>
       </c>
-      <c r="C55" s="31">
+      <c r="C55" s="30">
         <f>C54*100</f>
         <v>0</v>
       </c>
@@ -1528,324 +1522,324 @@
       <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1025" width="8.42578125" customWidth="1"/>
+    <col min="1" max="1025" width="8.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B1" s="32" t="s">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="B1" s="31" t="s">
         <v>23</v>
       </c>
-      <c r="C1" s="33">
+      <c r="C1" s="32">
         <v>43489</v>
       </c>
-      <c r="D1" s="33">
+      <c r="D1" s="32">
         <v>43494</v>
       </c>
-      <c r="E1" s="33">
+      <c r="E1" s="32">
         <v>43496</v>
       </c>
-      <c r="F1" s="33">
+      <c r="F1" s="32">
         <v>43497</v>
       </c>
-      <c r="G1" s="34">
+      <c r="G1" s="33">
         <v>43502</v>
       </c>
-      <c r="H1" s="32" t="s">
+      <c r="H1" s="31" t="s">
         <v>24</v>
       </c>
-      <c r="I1" s="32" t="s">
+      <c r="I1" s="31" t="s">
         <v>24</v>
       </c>
-      <c r="J1" s="32" t="s">
+      <c r="J1" s="31" t="s">
         <v>24</v>
       </c>
-      <c r="K1" s="32" t="s">
+      <c r="K1" s="31" t="s">
         <v>24</v>
       </c>
-      <c r="L1" s="32" t="s">
+      <c r="L1" s="31" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="62.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="32" t="s">
+    <row r="2" spans="1:12" ht="62.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B2" s="31" t="s">
         <v>25</v>
       </c>
-      <c r="C2" s="35" t="s">
+      <c r="C2" s="34" t="s">
         <v>26</v>
       </c>
-      <c r="D2" s="35" t="s">
+      <c r="D2" s="34" t="s">
         <v>27</v>
       </c>
-      <c r="E2" s="35" t="s">
+      <c r="E2" s="34" t="s">
         <v>27</v>
       </c>
-      <c r="F2" s="35" t="s">
+      <c r="F2" s="34" t="s">
         <v>27</v>
       </c>
-      <c r="G2" s="35" t="s">
+      <c r="G2" s="34" t="s">
         <v>24</v>
       </c>
-      <c r="H2" s="35" t="s">
+      <c r="H2" s="34" t="s">
         <v>24</v>
       </c>
-      <c r="I2" s="35" t="s">
+      <c r="I2" s="34" t="s">
         <v>24</v>
       </c>
-      <c r="J2" s="35" t="s">
+      <c r="J2" s="34" t="s">
         <v>24</v>
       </c>
-      <c r="K2" s="35" t="s">
+      <c r="K2" s="34" t="s">
         <v>24</v>
       </c>
-      <c r="L2" s="35" t="s">
+      <c r="L2" s="34" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B3" s="32" t="s">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="B3" s="31" t="s">
         <v>28</v>
       </c>
-      <c r="C3" s="32">
+      <c r="C3" s="31">
         <v>1.5</v>
       </c>
-      <c r="D3" s="32">
+      <c r="D3" s="31">
         <v>0.5</v>
       </c>
-      <c r="E3" s="32">
+      <c r="E3" s="31">
         <v>0.5</v>
       </c>
-      <c r="F3" s="32">
+      <c r="F3" s="31">
         <v>1</v>
       </c>
-      <c r="G3" s="32">
+      <c r="G3" s="31">
         <v>0.5</v>
       </c>
-      <c r="H3" s="32">
-        <v>0</v>
-      </c>
-      <c r="I3" s="32">
-        <v>0</v>
-      </c>
-      <c r="J3" s="32">
-        <v>0</v>
-      </c>
-      <c r="K3" s="32">
-        <v>0</v>
-      </c>
-      <c r="L3" s="32">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A4" s="32" t="s">
+      <c r="H3" s="31">
+        <v>0</v>
+      </c>
+      <c r="I3" s="31">
+        <v>0</v>
+      </c>
+      <c r="J3" s="31">
+        <v>0</v>
+      </c>
+      <c r="K3" s="31">
+        <v>0</v>
+      </c>
+      <c r="L3" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A4" s="31" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="32">
+      <c r="B4" s="31">
         <f t="shared" ref="B4:B9" si="0">SUMIF(C4:L4,A$12,C$3:Z$3)</f>
         <v>4</v>
       </c>
-      <c r="C4" s="36" t="s">
-        <v>29</v>
-      </c>
-      <c r="D4" s="36" t="s">
-        <v>29</v>
-      </c>
-      <c r="E4" s="36" t="s">
-        <v>29</v>
-      </c>
-      <c r="F4" s="36" t="s">
-        <v>29</v>
-      </c>
-      <c r="G4" s="36" t="s">
-        <v>29</v>
-      </c>
-      <c r="H4" s="36"/>
-      <c r="I4" s="36"/>
-      <c r="J4" s="36"/>
-      <c r="K4" s="36"/>
-      <c r="L4" s="36"/>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A5" s="32" t="s">
+      <c r="C4" s="35" t="s">
+        <v>29</v>
+      </c>
+      <c r="D4" s="35" t="s">
+        <v>29</v>
+      </c>
+      <c r="E4" s="35" t="s">
+        <v>29</v>
+      </c>
+      <c r="F4" s="35" t="s">
+        <v>29</v>
+      </c>
+      <c r="G4" s="35" t="s">
+        <v>29</v>
+      </c>
+      <c r="H4" s="35"/>
+      <c r="I4" s="35"/>
+      <c r="J4" s="35"/>
+      <c r="K4" s="35"/>
+      <c r="L4" s="35"/>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A5" s="31" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="32">
+      <c r="B5" s="31">
         <f t="shared" si="0"/>
         <v>3.5</v>
       </c>
-      <c r="C5" s="36" t="s">
-        <v>29</v>
-      </c>
-      <c r="D5" s="36"/>
-      <c r="E5" s="36" t="s">
-        <v>29</v>
-      </c>
-      <c r="F5" s="36" t="s">
-        <v>29</v>
-      </c>
-      <c r="G5" s="36" t="s">
-        <v>29</v>
-      </c>
-      <c r="J5" s="36"/>
-      <c r="K5" s="36"/>
-      <c r="L5" s="36"/>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A6" s="32" t="s">
+      <c r="C5" s="35" t="s">
+        <v>29</v>
+      </c>
+      <c r="D5" s="35"/>
+      <c r="E5" s="35" t="s">
+        <v>29</v>
+      </c>
+      <c r="F5" s="35" t="s">
+        <v>29</v>
+      </c>
+      <c r="G5" s="35" t="s">
+        <v>29</v>
+      </c>
+      <c r="J5" s="35"/>
+      <c r="K5" s="35"/>
+      <c r="L5" s="35"/>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A6" s="31" t="s">
         <v>9</v>
       </c>
-      <c r="B6" s="32">
+      <c r="B6" s="31">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="C6" s="36" t="s">
-        <v>29</v>
-      </c>
-      <c r="D6" s="36" t="s">
-        <v>29</v>
-      </c>
-      <c r="E6" s="36" t="s">
-        <v>29</v>
-      </c>
-      <c r="F6" s="36" t="s">
-        <v>29</v>
-      </c>
-      <c r="G6" s="36" t="s">
-        <v>29</v>
-      </c>
-      <c r="H6" s="36"/>
-      <c r="I6" s="36"/>
-      <c r="J6" s="36"/>
-      <c r="K6" s="36"/>
-      <c r="L6" s="36"/>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A7" s="32" t="s">
+      <c r="C6" s="35" t="s">
+        <v>29</v>
+      </c>
+      <c r="D6" s="35" t="s">
+        <v>29</v>
+      </c>
+      <c r="E6" s="35" t="s">
+        <v>29</v>
+      </c>
+      <c r="F6" s="35" t="s">
+        <v>29</v>
+      </c>
+      <c r="G6" s="35" t="s">
+        <v>29</v>
+      </c>
+      <c r="H6" s="35"/>
+      <c r="I6" s="35"/>
+      <c r="J6" s="35"/>
+      <c r="K6" s="35"/>
+      <c r="L6" s="35"/>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A7" s="31" t="s">
         <v>10</v>
       </c>
-      <c r="B7" s="32">
+      <c r="B7" s="31">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="C7" s="36" t="s">
-        <v>29</v>
-      </c>
-      <c r="D7" s="36" t="s">
-        <v>29</v>
-      </c>
-      <c r="E7" s="36" t="s">
-        <v>29</v>
-      </c>
-      <c r="F7" s="36" t="s">
-        <v>29</v>
-      </c>
-      <c r="G7" s="36" t="s">
-        <v>29</v>
-      </c>
-      <c r="H7" s="36"/>
-      <c r="I7" s="36"/>
-      <c r="J7" s="36"/>
-      <c r="K7" s="36"/>
-      <c r="L7" s="36"/>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A8" s="32" t="s">
+      <c r="C7" s="35" t="s">
+        <v>29</v>
+      </c>
+      <c r="D7" s="35" t="s">
+        <v>29</v>
+      </c>
+      <c r="E7" s="35" t="s">
+        <v>29</v>
+      </c>
+      <c r="F7" s="35" t="s">
+        <v>29</v>
+      </c>
+      <c r="G7" s="35" t="s">
+        <v>29</v>
+      </c>
+      <c r="H7" s="35"/>
+      <c r="I7" s="35"/>
+      <c r="J7" s="35"/>
+      <c r="K7" s="35"/>
+      <c r="L7" s="35"/>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A8" s="31" t="s">
         <v>11</v>
       </c>
-      <c r="B8" s="32">
+      <c r="B8" s="31">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="C8" s="36" t="s">
-        <v>29</v>
-      </c>
-      <c r="D8" s="36" t="s">
-        <v>29</v>
-      </c>
-      <c r="E8" s="36" t="s">
-        <v>29</v>
-      </c>
-      <c r="F8" s="36" t="s">
-        <v>29</v>
-      </c>
-      <c r="G8" s="36" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A9" s="32" t="s">
+      <c r="C8" s="35" t="s">
+        <v>29</v>
+      </c>
+      <c r="D8" s="35" t="s">
+        <v>29</v>
+      </c>
+      <c r="E8" s="35" t="s">
+        <v>29</v>
+      </c>
+      <c r="F8" s="35" t="s">
+        <v>29</v>
+      </c>
+      <c r="G8" s="35" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A9" s="31" t="s">
         <v>12</v>
       </c>
-      <c r="B9" s="32">
+      <c r="B9" s="31">
         <f t="shared" si="0"/>
         <v>2.5</v>
       </c>
-      <c r="D9" s="36" t="s">
-        <v>29</v>
-      </c>
-      <c r="E9" s="36" t="s">
-        <v>29</v>
-      </c>
-      <c r="F9" s="36" t="s">
-        <v>29</v>
-      </c>
-      <c r="G9" s="36" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A10" s="32" t="s">
-        <v>0</v>
-      </c>
-      <c r="B10" s="32">
+      <c r="D9" s="35" t="s">
+        <v>29</v>
+      </c>
+      <c r="E9" s="35" t="s">
+        <v>29</v>
+      </c>
+      <c r="F9" s="35" t="s">
+        <v>29</v>
+      </c>
+      <c r="G9" s="35" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A10" s="31" t="s">
+        <v>0</v>
+      </c>
+      <c r="B10" s="31">
         <f>SUM(B4:B7)</f>
         <v>15.5</v>
       </c>
-      <c r="C10" s="32">
+      <c r="C10" s="31">
         <f t="shared" ref="C10:L10" si="1">COUNTIF(C4:C7,"*ü*") * C3</f>
         <v>6</v>
       </c>
-      <c r="D10" s="32">
+      <c r="D10" s="31">
         <f t="shared" si="1"/>
         <v>1.5</v>
       </c>
-      <c r="E10" s="32">
+      <c r="E10" s="31">
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
-      <c r="F10" s="32">
+      <c r="F10" s="31">
         <f t="shared" si="1"/>
         <v>4</v>
       </c>
-      <c r="G10" s="32">
+      <c r="G10" s="31">
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
-      <c r="H10" s="32">
+      <c r="H10" s="31">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="I10" s="32">
+      <c r="I10" s="31">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="J10" s="32">
+      <c r="J10" s="31">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="K10" s="32">
+      <c r="K10" s="31">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="L10" s="32">
+      <c r="L10" s="31">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A12" s="36" t="s">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A12" s="35" t="s">
         <v>29</v>
       </c>
     </row>
@@ -1860,28 +1854,28 @@
   <dimension ref="A1:S32"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I16" sqref="I16"/>
+      <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="15" customWidth="1"/>
-    <col min="2" max="2" width="29.7109375" customWidth="1"/>
-    <col min="3" max="3" width="14.5703125" customWidth="1"/>
-    <col min="4" max="4" width="10.5703125" customWidth="1"/>
-    <col min="5" max="19" width="3.7109375" customWidth="1"/>
-    <col min="20" max="1025" width="8.42578125" customWidth="1"/>
+    <col min="2" max="2" width="29.6640625" customWidth="1"/>
+    <col min="3" max="3" width="14.5" customWidth="1"/>
+    <col min="4" max="4" width="10.5" customWidth="1"/>
+    <col min="5" max="19" width="3.6640625" customWidth="1"/>
+    <col min="20" max="1025" width="8.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A1" s="37"/>
-      <c r="B1" s="38" t="s">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A1" s="36"/>
+      <c r="B1" s="37" t="s">
         <v>30</v>
       </c>
-      <c r="C1" s="38" t="s">
+      <c r="C1" s="37" t="s">
         <v>31</v>
       </c>
-      <c r="D1" s="39" t="s">
+      <c r="D1" s="38" t="s">
         <v>32</v>
       </c>
       <c r="E1">
@@ -1930,292 +1924,307 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="C2" s="40"/>
-      <c r="D2" s="41"/>
-    </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B3" s="4" t="s">
+      <c r="C2" s="39"/>
+      <c r="D2" s="40"/>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="B3" s="3" t="s">
         <v>34</v>
       </c>
       <c r="C3">
         <v>1</v>
       </c>
-      <c r="D3" s="41">
+      <c r="D3" s="40">
         <v>0.75</v>
       </c>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B4" s="4" t="s">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="B4" s="3" t="s">
         <v>35</v>
       </c>
       <c r="C4">
         <v>3</v>
       </c>
-      <c r="D4" s="41"/>
-    </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B5" s="4" t="s">
+      <c r="D4" s="40"/>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="B5" s="3" t="s">
         <v>36</v>
       </c>
       <c r="C5">
         <v>1</v>
       </c>
-      <c r="D5" s="41"/>
-    </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A6" s="42"/>
-      <c r="B6" s="4" t="s">
+      <c r="D5" s="40"/>
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A6" s="41"/>
+      <c r="B6" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="C6" s="4">
+      <c r="C6" s="3">
         <f>SUM(C2:C5)</f>
         <v>5</v>
       </c>
-      <c r="D6" s="5">
+      <c r="D6" s="4">
         <f>SUM(D2:D5)</f>
         <v>0.75</v>
       </c>
     </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A7" s="3" t="s">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A7" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="4" t="s">
+      <c r="B7" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="C7" s="40"/>
-      <c r="D7" s="41"/>
-    </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B8" s="4" t="s">
+      <c r="C7" s="39"/>
+      <c r="D7" s="40"/>
+    </row>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="B8" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="D8" s="41"/>
-    </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B9" s="4" t="s">
+      <c r="D8" s="40"/>
+    </row>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="B9" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="D9" s="41"/>
-    </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B10" s="4" t="s">
+      <c r="D9" s="40"/>
+    </row>
+    <row r="10" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="B10" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="D10" s="41"/>
-    </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A11" s="42"/>
-      <c r="B11" s="4" t="s">
+      <c r="D10" s="40"/>
+    </row>
+    <row r="11" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A11" s="41"/>
+      <c r="B11" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="C11" s="4">
+      <c r="C11" s="3">
         <f>SUM(C7:C10)</f>
         <v>0</v>
       </c>
-      <c r="D11" s="5">
+      <c r="D11" s="4">
         <f>SUM(D7:D10)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A12" s="3" t="s">
+    <row r="12" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A12" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B12" s="4" t="s">
+      <c r="B12" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="C12" s="40"/>
-      <c r="D12" s="41"/>
-    </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B13" s="4" t="s">
+      <c r="C12" s="39"/>
+      <c r="D12" s="40"/>
+    </row>
+    <row r="13" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="B13" s="3" t="s">
         <v>38</v>
       </c>
       <c r="C13">
         <v>2</v>
       </c>
-      <c r="D13" s="41">
+      <c r="D13" s="40">
         <v>1.5</v>
       </c>
     </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B14" s="4" t="s">
+    <row r="14" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="B14" s="3" t="s">
         <v>35</v>
       </c>
       <c r="C14">
         <v>4</v>
       </c>
-      <c r="D14" s="41">
+      <c r="D14" s="40">
         <v>3</v>
       </c>
     </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B15" s="4" t="s">
+    <row r="15" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="B15" s="3" t="s">
         <v>36</v>
       </c>
       <c r="C15">
         <v>2</v>
       </c>
-      <c r="D15" s="41">
+      <c r="D15" s="40">
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A16" s="42"/>
-      <c r="B16" s="43" t="s">
+    <row r="16" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A16" s="41"/>
+      <c r="B16" s="42" t="s">
         <v>37</v>
       </c>
-      <c r="C16" s="4">
+      <c r="C16" s="3">
         <f>SUM(C12:C15)</f>
         <v>8</v>
       </c>
-      <c r="D16" s="5">
+      <c r="D16" s="4">
         <f>SUM(D12:D15)</f>
         <v>5.5</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="3" t="s">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A17" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B17" s="4" t="s">
+      <c r="B17" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="C17" s="40"/>
-      <c r="D17" s="41"/>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B18" s="4" t="s">
+      <c r="C17" s="39"/>
+      <c r="D17" s="40"/>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B18" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="D18" s="41"/>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B19" s="4" t="s">
+      <c r="D18" s="40"/>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B19" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="D19" s="41"/>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B20" s="4" t="s">
+      <c r="D19" s="40"/>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B20" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="D20" s="41"/>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="42"/>
-      <c r="B21" s="43" t="s">
+      <c r="D20" s="40"/>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A21" s="41"/>
+      <c r="B21" s="42" t="s">
         <v>37</v>
       </c>
-      <c r="C21" s="4">
+      <c r="C21" s="3">
         <f>SUM(C17:C20)</f>
         <v>0</v>
       </c>
-      <c r="D21" s="5">
+      <c r="D21" s="4">
         <f>SUM(D17:D20)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="3" t="s">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A22" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B22" s="4" t="s">
+      <c r="B22" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="D22" s="41"/>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B23" s="4" t="s">
+      <c r="D22" s="40"/>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B23" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="D23" s="41"/>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B24" s="4" t="s">
+      <c r="C23">
+        <v>1.5</v>
+      </c>
+      <c r="D23" s="40">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B24" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="D24" s="41"/>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B25" s="4" t="s">
+      <c r="C24">
+        <v>3</v>
+      </c>
+      <c r="D24" s="40">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B25" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="D25" s="41"/>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B26" s="43" t="s">
+      <c r="C25">
+        <v>1.5</v>
+      </c>
+      <c r="D25" s="40">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B26" s="42" t="s">
         <v>37</v>
       </c>
-      <c r="C26" s="4">
+      <c r="C26" s="3">
         <f>SUM(C22:C25)</f>
-        <v>0</v>
-      </c>
-      <c r="D26" s="5">
+        <v>6</v>
+      </c>
+      <c r="D26" s="4">
         <f>SUM(D22:D25)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A27" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B27" s="4" t="s">
+      <c r="B27" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="D27" s="41"/>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B28" s="4" t="s">
+      <c r="D27" s="40"/>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B28" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="D28" s="41"/>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B29" s="4" t="s">
+      <c r="D28" s="40"/>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B29" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="D29" s="41"/>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B30" s="4" t="s">
+      <c r="D29" s="40"/>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B30" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="D30" s="41"/>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B31" s="43" t="s">
+      <c r="D30" s="40"/>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B31" s="42" t="s">
         <v>37</v>
       </c>
-      <c r="C31" s="4">
+      <c r="C31" s="3">
         <f>SUM(C27:C30)</f>
         <v>0</v>
       </c>
-      <c r="D31" s="5">
+      <c r="D31" s="4">
         <f>SUM(D27:D30)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" s="44"/>
-      <c r="B32" s="45" t="s">
-        <v>0</v>
-      </c>
-      <c r="C32" s="7">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A32" s="43"/>
+      <c r="B32" s="44" t="s">
+        <v>0</v>
+      </c>
+      <c r="C32" s="6">
         <f>SUM(C6,C11,C16,C21,C26,C31)</f>
-        <v>13</v>
-      </c>
-      <c r="D32" s="8">
+        <v>19</v>
+      </c>
+      <c r="D32" s="7">
         <f>SUM(D6,D11,D16,D21,D26,D31)</f>
-        <v>6.25</v>
+        <v>12.25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added times - josh
</commit_message>
<xml_diff>
--- a/docs/ganttChart.xlsx
+++ b/docs/ganttChart.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11015"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/blakelyfrechette/Desktop/banana/docs/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\cs383 banana\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB96CADC-5291-914E-9930-BFDCBF2B08D5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFCFF798-DADE-4D46-86CA-29ECD4BFA7C1}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="980" yWindow="0" windowWidth="20760" windowHeight="12340" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="28110" windowHeight="16440" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Management Summary" sheetId="1" r:id="rId1"/>
@@ -18,8 +18,14 @@
     <sheet name="Meetings" sheetId="3" r:id="rId3"/>
     <sheet name="SA" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="179021" iterateDelta="1E-4"/>
+  <calcPr calcId="191029" iterateDelta="1E-4"/>
   <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
+    </ext>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
     </ext>
@@ -28,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="41">
   <si>
     <t>Total</t>
   </si>
@@ -183,7 +189,7 @@
       <charset val="2"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -220,6 +226,12 @@
         <bgColor rgb="FF33CCCC"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="14">
     <border>
@@ -374,11 +386,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -427,6 +436,10 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -815,435 +828,435 @@
       <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="8.5" customWidth="1"/>
-    <col min="3" max="3" width="14.33203125" customWidth="1"/>
-    <col min="4" max="4" width="13.83203125" customWidth="1"/>
-    <col min="5" max="5" width="13.33203125" customWidth="1"/>
-    <col min="6" max="6" width="3.5" customWidth="1"/>
-    <col min="7" max="7" width="15.33203125" customWidth="1"/>
-    <col min="8" max="8" width="12.33203125" customWidth="1"/>
-    <col min="9" max="9" width="14.5" customWidth="1"/>
-    <col min="10" max="10" width="2.83203125" customWidth="1"/>
-    <col min="11" max="11" width="13.83203125" customWidth="1"/>
+    <col min="1" max="2" width="8.42578125" customWidth="1"/>
+    <col min="3" max="3" width="14.28515625" customWidth="1"/>
+    <col min="4" max="4" width="13.85546875" customWidth="1"/>
+    <col min="5" max="5" width="13.28515625" customWidth="1"/>
+    <col min="6" max="6" width="3.42578125" customWidth="1"/>
+    <col min="7" max="7" width="15.28515625" customWidth="1"/>
+    <col min="8" max="8" width="12.28515625" customWidth="1"/>
+    <col min="9" max="9" width="14.42578125" customWidth="1"/>
+    <col min="10" max="10" width="2.85546875" customWidth="1"/>
+    <col min="11" max="11" width="13.85546875" customWidth="1"/>
     <col min="12" max="12" width="14" customWidth="1"/>
-    <col min="13" max="13" width="14.1640625" customWidth="1"/>
-    <col min="14" max="14" width="5.5" customWidth="1"/>
-    <col min="15" max="15" width="12.33203125" customWidth="1"/>
-    <col min="16" max="16" width="14.6640625" customWidth="1"/>
-    <col min="17" max="17" width="11.33203125" customWidth="1"/>
-    <col min="18" max="1025" width="8.5" customWidth="1"/>
+    <col min="13" max="13" width="14.140625" customWidth="1"/>
+    <col min="14" max="14" width="5.42578125" customWidth="1"/>
+    <col min="15" max="15" width="12.28515625" customWidth="1"/>
+    <col min="16" max="16" width="14.7109375" customWidth="1"/>
+    <col min="17" max="17" width="11.28515625" customWidth="1"/>
+    <col min="18" max="1025" width="8.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:17" x14ac:dyDescent="0.2">
-      <c r="C2" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
-      <c r="F2" s="2"/>
-      <c r="G2" s="1" t="s">
+    <row r="2" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="C2" s="45" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2" s="45"/>
+      <c r="E2" s="45"/>
+      <c r="F2" s="1"/>
+      <c r="G2" s="45" t="s">
         <v>1</v>
       </c>
-      <c r="H2" s="1"/>
-      <c r="I2" s="1"/>
-      <c r="K2" s="1" t="s">
+      <c r="H2" s="45"/>
+      <c r="I2" s="45"/>
+      <c r="K2" s="45" t="s">
         <v>2</v>
       </c>
-      <c r="L2" s="1"/>
-      <c r="M2" s="1"/>
-      <c r="O2" s="1" t="s">
+      <c r="L2" s="45"/>
+      <c r="M2" s="45"/>
+      <c r="O2" s="45" t="s">
         <v>3</v>
       </c>
-      <c r="P2" s="1"/>
-      <c r="Q2" s="1"/>
-    </row>
-    <row r="3" spans="2:17" x14ac:dyDescent="0.2">
-      <c r="C3" s="3" t="s">
+      <c r="P2" s="45"/>
+      <c r="Q2" s="45"/>
+    </row>
+    <row r="3" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="C3" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="D3" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="E3" s="5" t="s">
+      <c r="E3" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="G3" s="6" t="s">
+      <c r="G3" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="H3" s="7" t="s">
+      <c r="H3" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="I3" s="8" t="s">
+      <c r="I3" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="K3" s="6" t="s">
+      <c r="K3" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="L3" s="7" t="s">
+      <c r="L3" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="M3" s="8" t="s">
+      <c r="M3" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="O3" s="3" t="s">
+      <c r="O3" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="P3" s="4" t="s">
+      <c r="P3" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="Q3" s="5" t="s">
+      <c r="Q3" s="4" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="2:17" x14ac:dyDescent="0.2">
-      <c r="B4" s="9" t="s">
+    <row r="4" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B4" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="10">
+      <c r="C4" s="9">
         <f t="shared" ref="C4:D8" si="0">(G4+K4+O4)</f>
         <v>1500</v>
       </c>
-      <c r="D4" s="11">
+      <c r="D4" s="10">
         <f t="shared" si="0"/>
         <v>1275</v>
       </c>
-      <c r="E4" s="12">
+      <c r="E4" s="11">
         <f t="shared" ref="E4:E9" si="1">(C4-D4)</f>
         <v>225</v>
       </c>
-      <c r="G4" s="13">
-        <v>0</v>
-      </c>
-      <c r="H4" s="14">
-        <v>0</v>
-      </c>
-      <c r="I4" s="15">
+      <c r="G4" s="12">
+        <v>0</v>
+      </c>
+      <c r="H4" s="13">
+        <v>0</v>
+      </c>
+      <c r="I4" s="14">
         <f t="shared" ref="I4:I9" si="2">(G4-H4)</f>
         <v>0</v>
       </c>
-      <c r="K4" s="10">
+      <c r="K4" s="9">
         <v>1000</v>
       </c>
-      <c r="L4" s="11">
+      <c r="L4" s="10">
         <f>Meetings!B4*100</f>
         <v>400</v>
       </c>
-      <c r="M4" s="12">
+      <c r="M4" s="11">
         <f t="shared" ref="M4:M9" si="3">(K4-L4)</f>
         <v>600</v>
       </c>
-      <c r="O4" s="10">
+      <c r="O4" s="9">
         <f>(SA!C6)*100</f>
         <v>500</v>
       </c>
-      <c r="P4" s="11">
+      <c r="P4" s="10">
         <f>(SA!D6)*100</f>
         <v>875</v>
       </c>
-      <c r="Q4" s="12">
+      <c r="Q4" s="11">
         <f t="shared" ref="Q4:Q9" si="4">(O4-P4)</f>
         <v>-375</v>
       </c>
     </row>
-    <row r="5" spans="2:17" x14ac:dyDescent="0.2">
-      <c r="B5" s="3" t="s">
+    <row r="5" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B5" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="13">
+      <c r="C5" s="12">
         <f t="shared" si="0"/>
         <v>1000</v>
       </c>
-      <c r="D5" s="14">
+      <c r="D5" s="13">
         <f t="shared" si="0"/>
         <v>350</v>
       </c>
-      <c r="E5" s="15">
+      <c r="E5" s="14">
         <f t="shared" si="1"/>
         <v>650</v>
       </c>
-      <c r="G5" s="13">
-        <v>0</v>
-      </c>
-      <c r="H5" s="14">
-        <v>0</v>
-      </c>
-      <c r="I5" s="15">
+      <c r="G5" s="12">
+        <v>0</v>
+      </c>
+      <c r="H5" s="13">
+        <v>0</v>
+      </c>
+      <c r="I5" s="14">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="K5" s="13">
+      <c r="K5" s="12">
         <v>1000</v>
       </c>
-      <c r="L5" s="14">
+      <c r="L5" s="13">
         <f>Meetings!B5*100</f>
         <v>350</v>
       </c>
-      <c r="M5" s="15">
+      <c r="M5" s="14">
         <f t="shared" si="3"/>
         <v>650</v>
       </c>
-      <c r="O5" s="13">
+      <c r="O5" s="12">
         <f>(SA!C11)*100</f>
         <v>0</v>
       </c>
-      <c r="P5" s="14">
+      <c r="P5" s="13">
         <f>(SA!D11)*100</f>
         <v>0</v>
       </c>
-      <c r="Q5" s="15">
+      <c r="Q5" s="14">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="2:17" x14ac:dyDescent="0.2">
-      <c r="B6" s="3" t="s">
+    <row r="6" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B6" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C6" s="13">
+      <c r="C6" s="12">
         <f t="shared" si="0"/>
-        <v>1800</v>
-      </c>
-      <c r="D6" s="14">
+        <v>2000</v>
+      </c>
+      <c r="D6" s="13">
         <f t="shared" si="0"/>
+        <v>1050</v>
+      </c>
+      <c r="E6" s="14">
+        <f t="shared" si="1"/>
         <v>950</v>
       </c>
-      <c r="E6" s="15">
-        <f t="shared" si="1"/>
-        <v>850</v>
-      </c>
-      <c r="G6" s="13">
-        <v>0</v>
-      </c>
-      <c r="H6" s="14">
-        <v>0</v>
-      </c>
-      <c r="I6" s="15">
+      <c r="G6" s="12">
+        <v>0</v>
+      </c>
+      <c r="H6" s="13">
+        <v>0</v>
+      </c>
+      <c r="I6" s="14">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="K6" s="13">
+      <c r="K6" s="12">
         <v>1000</v>
       </c>
-      <c r="L6" s="14">
+      <c r="L6" s="13">
         <f>Meetings!B6*100</f>
         <v>400</v>
       </c>
-      <c r="M6" s="15">
+      <c r="M6" s="14">
         <f t="shared" si="3"/>
         <v>600</v>
       </c>
-      <c r="O6" s="13">
-        <f>(SA!C16)*100</f>
-        <v>800</v>
-      </c>
-      <c r="P6" s="14">
-        <f>(SA!D16)*100</f>
-        <v>550</v>
-      </c>
-      <c r="Q6" s="15">
+      <c r="O6" s="12">
+        <f>(SA!C18)*100</f>
+        <v>1000</v>
+      </c>
+      <c r="P6" s="13">
+        <f>(SA!D18)*100</f>
+        <v>650</v>
+      </c>
+      <c r="Q6" s="14">
         <f t="shared" si="4"/>
-        <v>250</v>
-      </c>
-    </row>
-    <row r="7" spans="2:17" x14ac:dyDescent="0.2">
-      <c r="B7" s="3" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="7" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B7" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C7" s="13">
+      <c r="C7" s="12">
         <f t="shared" si="0"/>
         <v>1600</v>
       </c>
-      <c r="D7" s="14">
+      <c r="D7" s="13">
         <f t="shared" si="0"/>
         <v>1000</v>
       </c>
-      <c r="E7" s="15">
+      <c r="E7" s="14">
         <f t="shared" si="1"/>
         <v>600</v>
       </c>
-      <c r="G7" s="13">
-        <v>0</v>
-      </c>
-      <c r="H7" s="14">
-        <v>0</v>
-      </c>
-      <c r="I7" s="15">
+      <c r="G7" s="12">
+        <v>0</v>
+      </c>
+      <c r="H7" s="13">
+        <v>0</v>
+      </c>
+      <c r="I7" s="14">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="K7" s="13">
+      <c r="K7" s="12">
         <v>1000</v>
       </c>
-      <c r="L7" s="14">
+      <c r="L7" s="13">
         <f>Meetings!B7*100</f>
         <v>400</v>
       </c>
-      <c r="M7" s="15">
+      <c r="M7" s="14">
         <f t="shared" si="3"/>
         <v>600</v>
       </c>
-      <c r="O7" s="13">
-        <f>(SA!C26)*100</f>
+      <c r="O7" s="12">
+        <f>(SA!C28)*100</f>
         <v>600</v>
       </c>
-      <c r="P7" s="14">
-        <f>(SA!D26)*100</f>
+      <c r="P7" s="13">
+        <f>(SA!D28)*100</f>
         <v>600</v>
       </c>
-      <c r="Q7" s="15">
+      <c r="Q7" s="14">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="2:17" x14ac:dyDescent="0.2">
-      <c r="B8" s="16" t="s">
+    <row r="8" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B8" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="C8" s="14">
+      <c r="C8" s="13">
         <f t="shared" si="0"/>
         <v>1000</v>
       </c>
-      <c r="D8" s="14">
+      <c r="D8" s="13">
         <f t="shared" si="0"/>
         <v>400</v>
       </c>
-      <c r="E8" s="15">
+      <c r="E8" s="14">
         <f t="shared" si="1"/>
         <v>600</v>
       </c>
-      <c r="G8" s="13">
-        <v>0</v>
-      </c>
-      <c r="H8" s="14">
-        <v>0</v>
-      </c>
-      <c r="I8" s="15">
+      <c r="G8" s="12">
+        <v>0</v>
+      </c>
+      <c r="H8" s="13">
+        <v>0</v>
+      </c>
+      <c r="I8" s="14">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="K8" s="13">
+      <c r="K8" s="12">
         <v>1000</v>
       </c>
-      <c r="L8" s="14">
+      <c r="L8" s="13">
         <f>Meetings!B8*100</f>
         <v>400</v>
       </c>
-      <c r="M8" s="15">
+      <c r="M8" s="14">
         <f t="shared" si="3"/>
         <v>600</v>
       </c>
-      <c r="O8" s="13">
-        <v>0</v>
-      </c>
-      <c r="P8" s="14">
-        <v>0</v>
-      </c>
-      <c r="Q8" s="15">
+      <c r="O8" s="12">
+        <v>0</v>
+      </c>
+      <c r="P8" s="13">
+        <v>0</v>
+      </c>
+      <c r="Q8" s="14">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="2:17" x14ac:dyDescent="0.2">
-      <c r="B9" s="16" t="s">
+    <row r="9" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B9" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="C9" s="14">
+      <c r="C9" s="13">
         <f>+(G9+K9+O9)</f>
         <v>1000</v>
       </c>
-      <c r="D9" s="14">
+      <c r="D9" s="13">
         <f>(H9+L9+P9)</f>
         <v>250</v>
       </c>
-      <c r="E9" s="17">
+      <c r="E9" s="16">
         <f t="shared" si="1"/>
         <v>750</v>
       </c>
-      <c r="G9" s="13">
-        <v>0</v>
-      </c>
-      <c r="H9" s="18">
-        <v>0</v>
-      </c>
-      <c r="I9" s="15">
+      <c r="G9" s="12">
+        <v>0</v>
+      </c>
+      <c r="H9" s="17">
+        <v>0</v>
+      </c>
+      <c r="I9" s="14">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="K9" s="19">
+      <c r="K9" s="18">
         <v>1000</v>
       </c>
-      <c r="L9" s="14">
+      <c r="L9" s="13">
         <f>Meetings!B9*100</f>
         <v>250</v>
       </c>
-      <c r="M9" s="15">
+      <c r="M9" s="14">
         <f t="shared" si="3"/>
         <v>750</v>
       </c>
-      <c r="O9" s="13">
-        <v>0</v>
-      </c>
-      <c r="P9" s="14">
-        <v>0</v>
-      </c>
-      <c r="Q9" s="15">
+      <c r="O9" s="12">
+        <v>0</v>
+      </c>
+      <c r="P9" s="13">
+        <v>0</v>
+      </c>
+      <c r="Q9" s="14">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="2:17" x14ac:dyDescent="0.2">
-      <c r="B10" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="C10" s="20">
+    <row r="10" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B10" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="C10" s="19">
         <f>SUM(C4:C9)</f>
-        <v>7900</v>
-      </c>
-      <c r="D10" s="21">
+        <v>8100</v>
+      </c>
+      <c r="D10" s="20">
         <f>SUM(D4:D9)</f>
-        <v>4225</v>
-      </c>
-      <c r="E10" s="22">
+        <v>4325</v>
+      </c>
+      <c r="E10" s="21">
         <f>SUM(E4:E9)</f>
-        <v>3675</v>
-      </c>
-      <c r="G10" s="20">
+        <v>3775</v>
+      </c>
+      <c r="G10" s="19">
         <f>SUM(G5:G9)</f>
         <v>0</v>
       </c>
-      <c r="H10" s="21">
+      <c r="H10" s="20">
         <f>SUM(H5:H9)</f>
         <v>0</v>
       </c>
-      <c r="I10" s="22">
+      <c r="I10" s="21">
         <f>SUM(I5:I9)</f>
         <v>0</v>
       </c>
-      <c r="K10" s="20">
+      <c r="K10" s="19">
         <f>SUM(K5:K9)</f>
         <v>5000</v>
       </c>
-      <c r="L10" s="21">
+      <c r="L10" s="20">
         <f>SUM(L5:L9)</f>
         <v>1800</v>
       </c>
-      <c r="M10" s="22">
+      <c r="M10" s="21">
         <f>SUM(M5:M9)</f>
         <v>3200</v>
       </c>
-      <c r="O10" s="23">
+      <c r="O10" s="22">
         <f>SUM(O5:O9)</f>
-        <v>1400</v>
-      </c>
-      <c r="P10" s="24">
+        <v>1600</v>
+      </c>
+      <c r="P10" s="23">
         <f>SUM(P5:P9)</f>
-        <v>1150</v>
-      </c>
-      <c r="Q10" s="25">
+        <v>1250</v>
+      </c>
+      <c r="Q10" s="24">
         <f>SUM(Q5:Q9)</f>
-        <v>250</v>
+        <v>350</v>
       </c>
     </row>
   </sheetData>
@@ -1262,21 +1275,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AD55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G47" sqref="G47"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G23" sqref="G23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="29" customWidth="1"/>
-    <col min="2" max="2" width="17.5" customWidth="1"/>
-    <col min="3" max="3" width="15.6640625" customWidth="1"/>
-    <col min="4" max="5" width="8.5" customWidth="1"/>
-    <col min="6" max="6" width="10.6640625" customWidth="1"/>
-    <col min="7" max="1025" width="8.5" customWidth="1"/>
+    <col min="2" max="2" width="17.42578125" customWidth="1"/>
+    <col min="3" max="3" width="15.7109375" customWidth="1"/>
+    <col min="4" max="5" width="8.42578125" customWidth="1"/>
+    <col min="6" max="6" width="10.7109375" customWidth="1"/>
+    <col min="7" max="1025" width="8.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:30" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>13</v>
       </c>
@@ -1286,21 +1299,21 @@
       <c r="D1" t="s">
         <v>15</v>
       </c>
-      <c r="E1" s="26"/>
+      <c r="E1" s="25"/>
       <c r="F1" t="s">
         <v>16</v>
       </c>
-      <c r="H1" s="27"/>
+      <c r="H1" s="26"/>
       <c r="I1" t="s">
         <v>17</v>
       </c>
-      <c r="K1" s="28"/>
+      <c r="K1" s="27"/>
       <c r="L1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A2" s="29" t="s">
+    <row r="2" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A2" s="28" t="s">
         <v>7</v>
       </c>
       <c r="D2" t="s">
@@ -1385,7 +1398,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="10" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>20</v>
       </c>
@@ -1398,12 +1411,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A11" s="30" t="s">
+    <row r="11" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A11" s="29" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>20</v>
       </c>
@@ -1416,12 +1429,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A21" s="30" t="s">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" s="29" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E22" s="46"/>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>20</v>
       </c>
@@ -1434,12 +1450,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A29" s="30" t="s">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" s="29" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>20</v>
       </c>
@@ -1452,12 +1468,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A37" s="30" t="s">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A37" s="29" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>39</v>
       </c>
@@ -1467,9 +1483,9 @@
       <c r="C38">
         <v>1</v>
       </c>
-      <c r="E38" s="26"/>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E38" s="25"/>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>40</v>
       </c>
@@ -1479,9 +1495,9 @@
       <c r="C39">
         <v>1</v>
       </c>
-      <c r="E39" s="26"/>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E39" s="25"/>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>20</v>
       </c>
@@ -1494,12 +1510,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A46" s="30" t="s">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A46" s="29" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>20</v>
       </c>
@@ -1512,7 +1528,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>21</v>
       </c>
@@ -1525,15 +1541,15 @@
         <v>2</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>22</v>
       </c>
-      <c r="B55" s="31">
+      <c r="B55" s="30">
         <f>B54*100</f>
         <v>200</v>
       </c>
-      <c r="C55" s="31">
+      <c r="C55" s="30">
         <f>C54*100</f>
         <v>200</v>
       </c>
@@ -1552,324 +1568,324 @@
       <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1025" width="8.5" customWidth="1"/>
+    <col min="1" max="1025" width="8.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="B1" s="32" t="s">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B1" s="31" t="s">
         <v>23</v>
       </c>
-      <c r="C1" s="33">
+      <c r="C1" s="32">
         <v>43489</v>
       </c>
-      <c r="D1" s="33">
+      <c r="D1" s="32">
         <v>43494</v>
       </c>
-      <c r="E1" s="33">
+      <c r="E1" s="32">
         <v>43496</v>
       </c>
-      <c r="F1" s="33">
+      <c r="F1" s="32">
         <v>43497</v>
       </c>
-      <c r="G1" s="34">
+      <c r="G1" s="33">
         <v>43502</v>
       </c>
-      <c r="H1" s="32" t="s">
+      <c r="H1" s="31" t="s">
         <v>24</v>
       </c>
-      <c r="I1" s="32" t="s">
+      <c r="I1" s="31" t="s">
         <v>24</v>
       </c>
-      <c r="J1" s="32" t="s">
+      <c r="J1" s="31" t="s">
         <v>24</v>
       </c>
-      <c r="K1" s="32" t="s">
+      <c r="K1" s="31" t="s">
         <v>24</v>
       </c>
-      <c r="L1" s="32" t="s">
+      <c r="L1" s="31" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="62.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B2" s="32" t="s">
+    <row r="2" spans="1:12" ht="62.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="31" t="s">
         <v>25</v>
       </c>
-      <c r="C2" s="35" t="s">
+      <c r="C2" s="34" t="s">
         <v>26</v>
       </c>
-      <c r="D2" s="35" t="s">
+      <c r="D2" s="34" t="s">
         <v>27</v>
       </c>
-      <c r="E2" s="35" t="s">
+      <c r="E2" s="34" t="s">
         <v>27</v>
       </c>
-      <c r="F2" s="35" t="s">
+      <c r="F2" s="34" t="s">
         <v>27</v>
       </c>
-      <c r="G2" s="35" t="s">
+      <c r="G2" s="34" t="s">
         <v>24</v>
       </c>
-      <c r="H2" s="35" t="s">
+      <c r="H2" s="34" t="s">
         <v>24</v>
       </c>
-      <c r="I2" s="35" t="s">
+      <c r="I2" s="34" t="s">
         <v>24</v>
       </c>
-      <c r="J2" s="35" t="s">
+      <c r="J2" s="34" t="s">
         <v>24</v>
       </c>
-      <c r="K2" s="35" t="s">
+      <c r="K2" s="34" t="s">
         <v>24</v>
       </c>
-      <c r="L2" s="35" t="s">
+      <c r="L2" s="34" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="B3" s="32" t="s">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B3" s="31" t="s">
         <v>28</v>
       </c>
-      <c r="C3" s="32">
+      <c r="C3" s="31">
         <v>1.5</v>
       </c>
-      <c r="D3" s="32">
+      <c r="D3" s="31">
         <v>0.5</v>
       </c>
-      <c r="E3" s="32">
+      <c r="E3" s="31">
         <v>0.5</v>
       </c>
-      <c r="F3" s="32">
+      <c r="F3" s="31">
         <v>1</v>
       </c>
-      <c r="G3" s="32">
+      <c r="G3" s="31">
         <v>0.5</v>
       </c>
-      <c r="H3" s="32">
-        <v>0</v>
-      </c>
-      <c r="I3" s="32">
-        <v>0</v>
-      </c>
-      <c r="J3" s="32">
-        <v>0</v>
-      </c>
-      <c r="K3" s="32">
-        <v>0</v>
-      </c>
-      <c r="L3" s="32">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A4" s="32" t="s">
+      <c r="H3" s="31">
+        <v>0</v>
+      </c>
+      <c r="I3" s="31">
+        <v>0</v>
+      </c>
+      <c r="J3" s="31">
+        <v>0</v>
+      </c>
+      <c r="K3" s="31">
+        <v>0</v>
+      </c>
+      <c r="L3" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A4" s="31" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="32">
+      <c r="B4" s="31">
         <f t="shared" ref="B4:B9" si="0">SUMIF(C4:L4,A$12,C$3:Z$3)</f>
         <v>4</v>
       </c>
-      <c r="C4" s="36" t="s">
-        <v>29</v>
-      </c>
-      <c r="D4" s="36" t="s">
-        <v>29</v>
-      </c>
-      <c r="E4" s="36" t="s">
-        <v>29</v>
-      </c>
-      <c r="F4" s="36" t="s">
-        <v>29</v>
-      </c>
-      <c r="G4" s="36" t="s">
-        <v>29</v>
-      </c>
-      <c r="H4" s="36"/>
-      <c r="I4" s="36"/>
-      <c r="J4" s="36"/>
-      <c r="K4" s="36"/>
-      <c r="L4" s="36"/>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A5" s="32" t="s">
+      <c r="C4" s="35" t="s">
+        <v>29</v>
+      </c>
+      <c r="D4" s="35" t="s">
+        <v>29</v>
+      </c>
+      <c r="E4" s="35" t="s">
+        <v>29</v>
+      </c>
+      <c r="F4" s="35" t="s">
+        <v>29</v>
+      </c>
+      <c r="G4" s="35" t="s">
+        <v>29</v>
+      </c>
+      <c r="H4" s="35"/>
+      <c r="I4" s="35"/>
+      <c r="J4" s="35"/>
+      <c r="K4" s="35"/>
+      <c r="L4" s="35"/>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A5" s="31" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="32">
+      <c r="B5" s="31">
         <f t="shared" si="0"/>
         <v>3.5</v>
       </c>
-      <c r="C5" s="36" t="s">
-        <v>29</v>
-      </c>
-      <c r="D5" s="36"/>
-      <c r="E5" s="36" t="s">
-        <v>29</v>
-      </c>
-      <c r="F5" s="36" t="s">
-        <v>29</v>
-      </c>
-      <c r="G5" s="36" t="s">
-        <v>29</v>
-      </c>
-      <c r="J5" s="36"/>
-      <c r="K5" s="36"/>
-      <c r="L5" s="36"/>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A6" s="32" t="s">
+      <c r="C5" s="35" t="s">
+        <v>29</v>
+      </c>
+      <c r="D5" s="35"/>
+      <c r="E5" s="35" t="s">
+        <v>29</v>
+      </c>
+      <c r="F5" s="35" t="s">
+        <v>29</v>
+      </c>
+      <c r="G5" s="35" t="s">
+        <v>29</v>
+      </c>
+      <c r="J5" s="35"/>
+      <c r="K5" s="35"/>
+      <c r="L5" s="35"/>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A6" s="31" t="s">
         <v>9</v>
       </c>
-      <c r="B6" s="32">
+      <c r="B6" s="31">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="C6" s="36" t="s">
-        <v>29</v>
-      </c>
-      <c r="D6" s="36" t="s">
-        <v>29</v>
-      </c>
-      <c r="E6" s="36" t="s">
-        <v>29</v>
-      </c>
-      <c r="F6" s="36" t="s">
-        <v>29</v>
-      </c>
-      <c r="G6" s="36" t="s">
-        <v>29</v>
-      </c>
-      <c r="H6" s="36"/>
-      <c r="I6" s="36"/>
-      <c r="J6" s="36"/>
-      <c r="K6" s="36"/>
-      <c r="L6" s="36"/>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A7" s="32" t="s">
+      <c r="C6" s="35" t="s">
+        <v>29</v>
+      </c>
+      <c r="D6" s="35" t="s">
+        <v>29</v>
+      </c>
+      <c r="E6" s="35" t="s">
+        <v>29</v>
+      </c>
+      <c r="F6" s="35" t="s">
+        <v>29</v>
+      </c>
+      <c r="G6" s="35" t="s">
+        <v>29</v>
+      </c>
+      <c r="H6" s="35"/>
+      <c r="I6" s="35"/>
+      <c r="J6" s="35"/>
+      <c r="K6" s="35"/>
+      <c r="L6" s="35"/>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A7" s="31" t="s">
         <v>10</v>
       </c>
-      <c r="B7" s="32">
+      <c r="B7" s="31">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="C7" s="36" t="s">
-        <v>29</v>
-      </c>
-      <c r="D7" s="36" t="s">
-        <v>29</v>
-      </c>
-      <c r="E7" s="36" t="s">
-        <v>29</v>
-      </c>
-      <c r="F7" s="36" t="s">
-        <v>29</v>
-      </c>
-      <c r="G7" s="36" t="s">
-        <v>29</v>
-      </c>
-      <c r="H7" s="36"/>
-      <c r="I7" s="36"/>
-      <c r="J7" s="36"/>
-      <c r="K7" s="36"/>
-      <c r="L7" s="36"/>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A8" s="32" t="s">
+      <c r="C7" s="35" t="s">
+        <v>29</v>
+      </c>
+      <c r="D7" s="35" t="s">
+        <v>29</v>
+      </c>
+      <c r="E7" s="35" t="s">
+        <v>29</v>
+      </c>
+      <c r="F7" s="35" t="s">
+        <v>29</v>
+      </c>
+      <c r="G7" s="35" t="s">
+        <v>29</v>
+      </c>
+      <c r="H7" s="35"/>
+      <c r="I7" s="35"/>
+      <c r="J7" s="35"/>
+      <c r="K7" s="35"/>
+      <c r="L7" s="35"/>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A8" s="31" t="s">
         <v>11</v>
       </c>
-      <c r="B8" s="32">
+      <c r="B8" s="31">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="C8" s="36" t="s">
-        <v>29</v>
-      </c>
-      <c r="D8" s="36" t="s">
-        <v>29</v>
-      </c>
-      <c r="E8" s="36" t="s">
-        <v>29</v>
-      </c>
-      <c r="F8" s="36" t="s">
-        <v>29</v>
-      </c>
-      <c r="G8" s="36" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A9" s="32" t="s">
+      <c r="C8" s="35" t="s">
+        <v>29</v>
+      </c>
+      <c r="D8" s="35" t="s">
+        <v>29</v>
+      </c>
+      <c r="E8" s="35" t="s">
+        <v>29</v>
+      </c>
+      <c r="F8" s="35" t="s">
+        <v>29</v>
+      </c>
+      <c r="G8" s="35" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A9" s="31" t="s">
         <v>12</v>
       </c>
-      <c r="B9" s="32">
+      <c r="B9" s="31">
         <f t="shared" si="0"/>
         <v>2.5</v>
       </c>
-      <c r="D9" s="36" t="s">
-        <v>29</v>
-      </c>
-      <c r="E9" s="36" t="s">
-        <v>29</v>
-      </c>
-      <c r="F9" s="36" t="s">
-        <v>29</v>
-      </c>
-      <c r="G9" s="36" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A10" s="32" t="s">
-        <v>0</v>
-      </c>
-      <c r="B10" s="32">
+      <c r="D9" s="35" t="s">
+        <v>29</v>
+      </c>
+      <c r="E9" s="35" t="s">
+        <v>29</v>
+      </c>
+      <c r="F9" s="35" t="s">
+        <v>29</v>
+      </c>
+      <c r="G9" s="35" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A10" s="31" t="s">
+        <v>0</v>
+      </c>
+      <c r="B10" s="31">
         <f>SUM(B4:B7)</f>
         <v>15.5</v>
       </c>
-      <c r="C10" s="32">
+      <c r="C10" s="31">
         <f t="shared" ref="C10:L10" si="1">COUNTIF(C4:C7,"*ü*") * C3</f>
         <v>6</v>
       </c>
-      <c r="D10" s="32">
+      <c r="D10" s="31">
         <f t="shared" si="1"/>
         <v>1.5</v>
       </c>
-      <c r="E10" s="32">
+      <c r="E10" s="31">
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
-      <c r="F10" s="32">
+      <c r="F10" s="31">
         <f t="shared" si="1"/>
         <v>4</v>
       </c>
-      <c r="G10" s="32">
+      <c r="G10" s="31">
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
-      <c r="H10" s="32">
+      <c r="H10" s="31">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="I10" s="32">
+      <c r="I10" s="31">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="J10" s="32">
+      <c r="J10" s="31">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="K10" s="32">
+      <c r="K10" s="31">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="L10" s="32">
+      <c r="L10" s="31">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A12" s="36" t="s">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A12" s="35" t="s">
         <v>29</v>
       </c>
     </row>
@@ -1881,31 +1897,31 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:S32"/>
+  <dimension ref="A1:S34"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15" customWidth="1"/>
-    <col min="2" max="2" width="29.6640625" customWidth="1"/>
-    <col min="3" max="3" width="14.5" customWidth="1"/>
-    <col min="4" max="4" width="10.5" customWidth="1"/>
-    <col min="5" max="19" width="3.6640625" customWidth="1"/>
-    <col min="20" max="1025" width="8.5" customWidth="1"/>
+    <col min="2" max="2" width="29.7109375" customWidth="1"/>
+    <col min="3" max="3" width="14.42578125" customWidth="1"/>
+    <col min="4" max="4" width="10.42578125" customWidth="1"/>
+    <col min="5" max="19" width="3.7109375" customWidth="1"/>
+    <col min="20" max="1025" width="8.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A1" s="37"/>
-      <c r="B1" s="38" t="s">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A1" s="36"/>
+      <c r="B1" s="37" t="s">
         <v>30</v>
       </c>
-      <c r="C1" s="38" t="s">
+      <c r="C1" s="37" t="s">
         <v>31</v>
       </c>
-      <c r="D1" s="39" t="s">
+      <c r="D1" s="38" t="s">
         <v>32</v>
       </c>
       <c r="E1">
@@ -1954,311 +1970,333 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A2" s="3" t="s">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="C2" s="40"/>
-      <c r="D2" s="41"/>
-    </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="B3" s="4" t="s">
+      <c r="C2" s="39"/>
+      <c r="D2" s="40"/>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="B3" s="3" t="s">
         <v>34</v>
       </c>
       <c r="C3">
         <v>1</v>
       </c>
-      <c r="D3" s="41">
+      <c r="D3" s="40">
         <v>0.75</v>
       </c>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="B4" s="4" t="s">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="B4" s="3" t="s">
         <v>35</v>
       </c>
       <c r="C4">
         <v>3</v>
       </c>
-      <c r="D4" s="41">
+      <c r="D4" s="40">
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="B5" s="4" t="s">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="B5" s="3" t="s">
         <v>36</v>
       </c>
       <c r="C5">
         <v>1</v>
       </c>
-      <c r="D5" s="41">
+      <c r="D5" s="40">
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A6" s="42"/>
-      <c r="B6" s="4" t="s">
+    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A6" s="41"/>
+      <c r="B6" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="C6" s="4">
+      <c r="C6" s="3">
         <f>SUM(C2:C5)</f>
         <v>5</v>
       </c>
-      <c r="D6" s="5">
+      <c r="D6" s="4">
         <f>SUM(D2:D5)</f>
         <v>8.75</v>
       </c>
     </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A7" s="3" t="s">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="4" t="s">
+      <c r="B7" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="C7" s="40"/>
-      <c r="D7" s="41"/>
-    </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="B8" s="4" t="s">
+      <c r="C7" s="39"/>
+      <c r="D7" s="40"/>
+    </row>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="B8" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="D8" s="41"/>
-    </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="B9" s="4" t="s">
+      <c r="D8" s="40"/>
+    </row>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="B9" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="D9" s="41"/>
-    </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="B10" s="4" t="s">
+      <c r="D9" s="40"/>
+    </row>
+    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="B10" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="D10" s="41"/>
-    </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A11" s="42"/>
-      <c r="B11" s="4" t="s">
+      <c r="D10" s="40"/>
+    </row>
+    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A11" s="41"/>
+      <c r="B11" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="C11" s="4">
+      <c r="C11" s="3">
         <f>SUM(C7:C10)</f>
         <v>0</v>
       </c>
-      <c r="D11" s="5">
+      <c r="D11" s="4">
         <f>SUM(D7:D10)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A12" s="3" t="s">
+    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B12" s="4" t="s">
+      <c r="B12" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="C12" s="40"/>
-      <c r="D12" s="41"/>
-    </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="B13" s="4" t="s">
+      <c r="C12" s="39"/>
+      <c r="D12" s="40"/>
+    </row>
+    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="B13" s="3" t="s">
         <v>38</v>
       </c>
       <c r="C13">
         <v>2</v>
       </c>
-      <c r="D13" s="41">
+      <c r="D13" s="40">
         <v>1.5</v>
       </c>
     </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="B14" s="4" t="s">
+    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="B14" s="3" t="s">
         <v>35</v>
       </c>
       <c r="C14">
         <v>4</v>
       </c>
-      <c r="D14" s="41">
+      <c r="D14" s="40">
         <v>3</v>
       </c>
     </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="B15" s="4" t="s">
+    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="B15" s="3" t="s">
         <v>36</v>
       </c>
       <c r="C15">
         <v>2</v>
       </c>
-      <c r="D15" s="41">
+      <c r="D15" s="40">
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A16" s="42"/>
-      <c r="B16" s="43" t="s">
+    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="B16" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="C16">
+        <v>1</v>
+      </c>
+      <c r="D16" s="40">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B17" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="C17">
+        <v>1</v>
+      </c>
+      <c r="D17" s="40">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="41"/>
+      <c r="B18" s="42" t="s">
         <v>37</v>
       </c>
-      <c r="C16" s="4">
-        <f>SUM(C12:C15)</f>
-        <v>8</v>
-      </c>
-      <c r="D16" s="5">
-        <f>SUM(D12:D15)</f>
-        <v>5.5</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A17" s="3" t="s">
+      <c r="C18" s="3">
+        <f>SUM(C12:C17)</f>
         <v>10</v>
       </c>
-      <c r="B17" s="4" t="s">
+      <c r="D18" s="4">
+        <f>SUM(D12:D17)</f>
+        <v>6.5</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B19" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="C17" s="40"/>
-      <c r="D17" s="41"/>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B18" s="4" t="s">
+      <c r="C19" s="39"/>
+      <c r="D19" s="40"/>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B20" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="D18" s="41"/>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B19" s="4" t="s">
+      <c r="D20" s="40"/>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B21" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="D19" s="41"/>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B20" s="4" t="s">
+      <c r="D21" s="40"/>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B22" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="D20" s="41"/>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A21" s="42"/>
-      <c r="B21" s="43" t="s">
+      <c r="D22" s="40"/>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" s="41"/>
+      <c r="B23" s="42" t="s">
         <v>37</v>
       </c>
-      <c r="C21" s="4">
-        <f>SUM(C17:C20)</f>
-        <v>0</v>
-      </c>
-      <c r="D21" s="5">
-        <f>SUM(D17:D20)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A22" s="3" t="s">
+      <c r="C23" s="3">
+        <f>SUM(C19:C22)</f>
+        <v>0</v>
+      </c>
+      <c r="D23" s="4">
+        <f>SUM(D19:D22)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B22" s="4" t="s">
+      <c r="B24" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="D22" s="41"/>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B23" s="4" t="s">
+      <c r="D24" s="40"/>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B25" s="3" t="s">
         <v>38</v>
-      </c>
-      <c r="C23">
-        <v>1.5</v>
-      </c>
-      <c r="D23" s="41">
-        <v>1.5</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B24" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="C24">
-        <v>3</v>
-      </c>
-      <c r="D24" s="41">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B25" s="4" t="s">
-        <v>36</v>
       </c>
       <c r="C25">
         <v>1.5</v>
       </c>
-      <c r="D25" s="41">
+      <c r="D25" s="40">
         <v>1.5</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B26" s="43" t="s">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B26" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="C26">
+        <v>3</v>
+      </c>
+      <c r="D26" s="40">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B27" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="C27">
+        <v>1.5</v>
+      </c>
+      <c r="D27" s="40">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B28" s="42" t="s">
         <v>37</v>
       </c>
-      <c r="C26" s="4">
-        <f>SUM(C22:C25)</f>
+      <c r="C28" s="3">
+        <f>SUM(C24:C27)</f>
         <v>6</v>
       </c>
-      <c r="D26" s="5">
-        <f>SUM(D22:D25)</f>
+      <c r="D28" s="4">
+        <f>SUM(D24:D27)</f>
         <v>6</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A27" s="3" t="s">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B27" s="4" t="s">
+      <c r="B29" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="D27" s="41"/>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B28" s="4" t="s">
+      <c r="D29" s="40"/>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B30" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="D28" s="41"/>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B29" s="4" t="s">
+      <c r="D30" s="40"/>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B31" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="D29" s="41"/>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B30" s="4" t="s">
+      <c r="D31" s="40"/>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B32" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="D30" s="41"/>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B31" s="43" t="s">
+      <c r="D32" s="40"/>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B33" s="42" t="s">
         <v>37</v>
       </c>
-      <c r="C31" s="4">
-        <f>SUM(C27:C30)</f>
-        <v>0</v>
-      </c>
-      <c r="D31" s="5">
-        <f>SUM(D27:D30)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A32" s="44"/>
-      <c r="B32" s="45" t="s">
-        <v>0</v>
-      </c>
-      <c r="C32" s="7">
-        <f>SUM(C6,C11,C16,C21,C26,C31)</f>
-        <v>19</v>
-      </c>
-      <c r="D32" s="8">
-        <f>SUM(D6,D11,D16,D21,D26,D31)</f>
-        <v>20.25</v>
+      <c r="C33" s="3">
+        <f>SUM(C29:C32)</f>
+        <v>0</v>
+      </c>
+      <c r="D33" s="4">
+        <f>SUM(D29:D32)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" s="43"/>
+      <c r="B34" s="44" t="s">
+        <v>0</v>
+      </c>
+      <c r="C34" s="6">
+        <f>SUM(C6,C11,C18,C23,C28,C33)</f>
+        <v>21</v>
+      </c>
+      <c r="D34" s="7">
+        <f>SUM(D6,D11,D18,D23,D28,D33)</f>
+        <v>21.25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated planned work for this week
</commit_message>
<xml_diff>
--- a/docs/ganttChart.xlsx
+++ b/docs/ganttChart.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11015"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nathan\School\Spring 2019\CS 383\GitRepos\banana-master\docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/blakelyfrechette/Desktop/banana/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F3D27B1-A1C5-40E1-89DD-B9297F660149}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7AC595CF-0254-2847-8901-81E2D2B3CF0E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="980" yWindow="0" windowWidth="26800" windowHeight="17360" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Management Summary" sheetId="1" r:id="rId1"/>
@@ -18,14 +18,8 @@
     <sheet name="Meetings" sheetId="3" r:id="rId3"/>
     <sheet name="SA" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="191029" iterateDelta="1E-4"/>
+  <calcPr calcId="179021" iterateDelta="1E-4"/>
   <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-      </xcalcf:calcFeatures>
-    </ext>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
     </ext>
@@ -34,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="44">
   <si>
     <t>Total</t>
   </si>
@@ -157,6 +151,15 @@
   </si>
   <si>
     <t>RFP</t>
+  </si>
+  <si>
+    <t>Import sounds in assets folder</t>
+  </si>
+  <si>
+    <t>Script classes for sound</t>
+  </si>
+  <si>
+    <t>Test cases</t>
   </si>
 </sst>
 </file>
@@ -388,9 +391,6 @@
   </cellStyleXfs>
   <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -440,6 +440,9 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -828,433 +831,433 @@
       <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="2" width="8.44140625" customWidth="1"/>
-    <col min="3" max="3" width="14.21875" customWidth="1"/>
-    <col min="4" max="4" width="13.88671875" customWidth="1"/>
+    <col min="1" max="2" width="8.5" customWidth="1"/>
+    <col min="3" max="3" width="14.1640625" customWidth="1"/>
+    <col min="4" max="4" width="13.83203125" customWidth="1"/>
     <col min="5" max="5" width="13.33203125" customWidth="1"/>
-    <col min="6" max="6" width="3.44140625" customWidth="1"/>
+    <col min="6" max="6" width="3.5" customWidth="1"/>
     <col min="7" max="7" width="15.33203125" customWidth="1"/>
     <col min="8" max="8" width="12.33203125" customWidth="1"/>
-    <col min="9" max="9" width="14.44140625" customWidth="1"/>
-    <col min="10" max="10" width="2.88671875" customWidth="1"/>
-    <col min="11" max="11" width="13.88671875" customWidth="1"/>
+    <col min="9" max="9" width="14.5" customWidth="1"/>
+    <col min="10" max="10" width="2.83203125" customWidth="1"/>
+    <col min="11" max="11" width="13.83203125" customWidth="1"/>
     <col min="12" max="12" width="14" customWidth="1"/>
-    <col min="13" max="13" width="14.109375" customWidth="1"/>
-    <col min="14" max="14" width="5.44140625" customWidth="1"/>
+    <col min="13" max="13" width="14.1640625" customWidth="1"/>
+    <col min="14" max="14" width="5.5" customWidth="1"/>
     <col min="15" max="15" width="12.33203125" customWidth="1"/>
     <col min="16" max="16" width="14.6640625" customWidth="1"/>
     <col min="17" max="17" width="11.33203125" customWidth="1"/>
-    <col min="18" max="1025" width="8.44140625" customWidth="1"/>
+    <col min="18" max="1025" width="8.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="C2" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
-      <c r="F2" s="2"/>
-      <c r="G2" s="1" t="s">
+    <row r="2" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="C2" s="46" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2" s="46"/>
+      <c r="E2" s="46"/>
+      <c r="F2" s="1"/>
+      <c r="G2" s="46" t="s">
         <v>1</v>
       </c>
-      <c r="H2" s="1"/>
-      <c r="I2" s="1"/>
-      <c r="K2" s="1" t="s">
+      <c r="H2" s="46"/>
+      <c r="I2" s="46"/>
+      <c r="K2" s="46" t="s">
         <v>2</v>
       </c>
-      <c r="L2" s="1"/>
-      <c r="M2" s="1"/>
-      <c r="O2" s="1" t="s">
+      <c r="L2" s="46"/>
+      <c r="M2" s="46"/>
+      <c r="O2" s="46" t="s">
         <v>3</v>
       </c>
-      <c r="P2" s="1"/>
-      <c r="Q2" s="1"/>
-    </row>
-    <row r="3" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="C3" s="3" t="s">
+      <c r="P2" s="46"/>
+      <c r="Q2" s="46"/>
+    </row>
+    <row r="3" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="C3" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="D3" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="E3" s="5" t="s">
+      <c r="E3" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="G3" s="6" t="s">
+      <c r="G3" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="H3" s="7" t="s">
+      <c r="H3" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="I3" s="8" t="s">
+      <c r="I3" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="K3" s="6" t="s">
+      <c r="K3" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="L3" s="7" t="s">
+      <c r="L3" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="M3" s="8" t="s">
+      <c r="M3" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="O3" s="3" t="s">
+      <c r="O3" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="P3" s="4" t="s">
+      <c r="P3" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="Q3" s="5" t="s">
+      <c r="Q3" s="4" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B4" s="9" t="s">
+    <row r="4" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="B4" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="10">
+      <c r="C4" s="9">
         <f t="shared" ref="C4:D8" si="0">(G4+K4+O4)</f>
         <v>1500</v>
       </c>
-      <c r="D4" s="11">
+      <c r="D4" s="10">
         <f t="shared" si="0"/>
         <v>1275</v>
       </c>
-      <c r="E4" s="12">
+      <c r="E4" s="11">
         <f t="shared" ref="E4:E9" si="1">(C4-D4)</f>
         <v>225</v>
       </c>
-      <c r="G4" s="13">
-        <v>0</v>
-      </c>
-      <c r="H4" s="14">
-        <v>0</v>
-      </c>
-      <c r="I4" s="15">
+      <c r="G4" s="12">
+        <v>0</v>
+      </c>
+      <c r="H4" s="13">
+        <v>0</v>
+      </c>
+      <c r="I4" s="14">
         <f t="shared" ref="I4:I9" si="2">(G4-H4)</f>
         <v>0</v>
       </c>
-      <c r="K4" s="10">
+      <c r="K4" s="9">
         <v>1000</v>
       </c>
-      <c r="L4" s="11">
+      <c r="L4" s="10">
         <f>Meetings!B4*100</f>
         <v>400</v>
       </c>
-      <c r="M4" s="12">
+      <c r="M4" s="11">
         <f t="shared" ref="M4:M9" si="3">(K4-L4)</f>
         <v>600</v>
       </c>
-      <c r="O4" s="10">
+      <c r="O4" s="9">
         <f>(SA!C6)*100</f>
         <v>500</v>
       </c>
-      <c r="P4" s="11">
+      <c r="P4" s="10">
         <f>(SA!D6)*100</f>
         <v>875</v>
       </c>
-      <c r="Q4" s="12">
+      <c r="Q4" s="11">
         <f t="shared" ref="Q4:Q9" si="4">(O4-P4)</f>
         <v>-375</v>
       </c>
     </row>
-    <row r="5" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B5" s="3" t="s">
+    <row r="5" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="B5" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="13">
+      <c r="C5" s="12">
         <f t="shared" si="0"/>
         <v>1000</v>
       </c>
-      <c r="D5" s="14">
+      <c r="D5" s="13">
         <f t="shared" si="0"/>
         <v>350</v>
       </c>
-      <c r="E5" s="15">
+      <c r="E5" s="14">
         <f t="shared" si="1"/>
         <v>650</v>
       </c>
-      <c r="G5" s="13">
-        <v>0</v>
-      </c>
-      <c r="H5" s="14">
-        <v>0</v>
-      </c>
-      <c r="I5" s="15">
+      <c r="G5" s="12">
+        <v>0</v>
+      </c>
+      <c r="H5" s="13">
+        <v>0</v>
+      </c>
+      <c r="I5" s="14">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="K5" s="13">
+      <c r="K5" s="12">
         <v>1000</v>
       </c>
-      <c r="L5" s="14">
+      <c r="L5" s="13">
         <f>Meetings!B5*100</f>
         <v>350</v>
       </c>
-      <c r="M5" s="15">
+      <c r="M5" s="14">
         <f t="shared" si="3"/>
         <v>650</v>
       </c>
-      <c r="O5" s="13">
+      <c r="O5" s="12">
         <f>(SA!C11)*100</f>
         <v>0</v>
       </c>
-      <c r="P5" s="14">
+      <c r="P5" s="13">
         <f>(SA!D11)*100</f>
         <v>0</v>
       </c>
-      <c r="Q5" s="15">
+      <c r="Q5" s="14">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B6" s="3" t="s">
+    <row r="6" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="B6" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C6" s="13">
+      <c r="C6" s="12">
         <f t="shared" si="0"/>
         <v>2000</v>
       </c>
-      <c r="D6" s="14">
+      <c r="D6" s="13">
         <f t="shared" si="0"/>
         <v>1050</v>
       </c>
-      <c r="E6" s="15">
+      <c r="E6" s="14">
         <f t="shared" si="1"/>
         <v>950</v>
       </c>
-      <c r="G6" s="13">
-        <v>0</v>
-      </c>
-      <c r="H6" s="14">
-        <v>0</v>
-      </c>
-      <c r="I6" s="15">
+      <c r="G6" s="12">
+        <v>0</v>
+      </c>
+      <c r="H6" s="13">
+        <v>0</v>
+      </c>
+      <c r="I6" s="14">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="K6" s="13">
+      <c r="K6" s="12">
         <v>1000</v>
       </c>
-      <c r="L6" s="14">
+      <c r="L6" s="13">
         <f>Meetings!B6*100</f>
         <v>400</v>
       </c>
-      <c r="M6" s="15">
+      <c r="M6" s="14">
         <f t="shared" si="3"/>
         <v>600</v>
       </c>
-      <c r="O6" s="13">
+      <c r="O6" s="12">
         <f>(SA!C18)*100</f>
         <v>1000</v>
       </c>
-      <c r="P6" s="14">
+      <c r="P6" s="13">
         <f>(SA!D18)*100</f>
         <v>650</v>
       </c>
-      <c r="Q6" s="15">
+      <c r="Q6" s="14">
         <f t="shared" si="4"/>
         <v>350</v>
       </c>
     </row>
-    <row r="7" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B7" s="3" t="s">
+    <row r="7" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="B7" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C7" s="13">
+      <c r="C7" s="12">
         <f t="shared" si="0"/>
         <v>1600</v>
       </c>
-      <c r="D7" s="14">
+      <c r="D7" s="13">
         <f t="shared" si="0"/>
         <v>1000</v>
       </c>
-      <c r="E7" s="15">
+      <c r="E7" s="14">
         <f t="shared" si="1"/>
         <v>600</v>
       </c>
-      <c r="G7" s="13">
-        <v>0</v>
-      </c>
-      <c r="H7" s="14">
-        <v>0</v>
-      </c>
-      <c r="I7" s="15">
+      <c r="G7" s="12">
+        <v>0</v>
+      </c>
+      <c r="H7" s="13">
+        <v>0</v>
+      </c>
+      <c r="I7" s="14">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="K7" s="13">
+      <c r="K7" s="12">
         <v>1000</v>
       </c>
-      <c r="L7" s="14">
+      <c r="L7" s="13">
         <f>Meetings!B7*100</f>
         <v>400</v>
       </c>
-      <c r="M7" s="15">
+      <c r="M7" s="14">
         <f t="shared" si="3"/>
         <v>600</v>
       </c>
-      <c r="O7" s="13">
+      <c r="O7" s="12">
         <f>(SA!C28)*100</f>
         <v>600</v>
       </c>
-      <c r="P7" s="14">
+      <c r="P7" s="13">
         <f>(SA!D28)*100</f>
         <v>600</v>
       </c>
-      <c r="Q7" s="15">
+      <c r="Q7" s="14">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B8" s="16" t="s">
+    <row r="8" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="B8" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="C8" s="14">
+      <c r="C8" s="13">
         <f t="shared" si="0"/>
         <v>1000</v>
       </c>
-      <c r="D8" s="14">
+      <c r="D8" s="13">
         <f t="shared" si="0"/>
         <v>400</v>
       </c>
-      <c r="E8" s="15">
+      <c r="E8" s="14">
         <f t="shared" si="1"/>
         <v>600</v>
       </c>
-      <c r="G8" s="13">
-        <v>0</v>
-      </c>
-      <c r="H8" s="14">
-        <v>0</v>
-      </c>
-      <c r="I8" s="15">
+      <c r="G8" s="12">
+        <v>0</v>
+      </c>
+      <c r="H8" s="13">
+        <v>0</v>
+      </c>
+      <c r="I8" s="14">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="K8" s="13">
+      <c r="K8" s="12">
         <v>1000</v>
       </c>
-      <c r="L8" s="14">
+      <c r="L8" s="13">
         <f>Meetings!B8*100</f>
         <v>400</v>
       </c>
-      <c r="M8" s="15">
+      <c r="M8" s="14">
         <f t="shared" si="3"/>
         <v>600</v>
       </c>
-      <c r="O8" s="13">
-        <v>0</v>
-      </c>
-      <c r="P8" s="14">
-        <v>0</v>
-      </c>
-      <c r="Q8" s="15">
+      <c r="O8" s="12">
+        <v>0</v>
+      </c>
+      <c r="P8" s="13">
+        <v>0</v>
+      </c>
+      <c r="Q8" s="14">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B9" s="16" t="s">
+    <row r="9" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="B9" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="C9" s="14">
+      <c r="C9" s="13">
         <f>+(G9+K9+O9)</f>
         <v>1000</v>
       </c>
-      <c r="D9" s="14">
+      <c r="D9" s="13">
         <f>(H9+L9+P9)</f>
         <v>250</v>
       </c>
-      <c r="E9" s="17">
+      <c r="E9" s="16">
         <f t="shared" si="1"/>
         <v>750</v>
       </c>
-      <c r="G9" s="13">
-        <v>0</v>
-      </c>
-      <c r="H9" s="18">
-        <v>0</v>
-      </c>
-      <c r="I9" s="15">
+      <c r="G9" s="12">
+        <v>0</v>
+      </c>
+      <c r="H9" s="17">
+        <v>0</v>
+      </c>
+      <c r="I9" s="14">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="K9" s="19">
+      <c r="K9" s="18">
         <v>1000</v>
       </c>
-      <c r="L9" s="14">
+      <c r="L9" s="13">
         <f>Meetings!B9*100</f>
         <v>250</v>
       </c>
-      <c r="M9" s="15">
+      <c r="M9" s="14">
         <f t="shared" si="3"/>
         <v>750</v>
       </c>
-      <c r="O9" s="13">
-        <v>0</v>
-      </c>
-      <c r="P9" s="14">
-        <v>0</v>
-      </c>
-      <c r="Q9" s="15">
+      <c r="O9" s="12">
+        <v>0</v>
+      </c>
+      <c r="P9" s="13">
+        <v>0</v>
+      </c>
+      <c r="Q9" s="14">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B10" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="C10" s="20">
+    <row r="10" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="B10" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="C10" s="19">
         <f>SUM(C4:C9)</f>
         <v>8100</v>
       </c>
-      <c r="D10" s="21">
+      <c r="D10" s="20">
         <f>SUM(D4:D9)</f>
         <v>4325</v>
       </c>
-      <c r="E10" s="22">
+      <c r="E10" s="21">
         <f>SUM(E4:E9)</f>
         <v>3775</v>
       </c>
-      <c r="G10" s="20">
+      <c r="G10" s="19">
         <f>SUM(G5:G9)</f>
         <v>0</v>
       </c>
-      <c r="H10" s="21">
+      <c r="H10" s="20">
         <f>SUM(H5:H9)</f>
         <v>0</v>
       </c>
-      <c r="I10" s="22">
+      <c r="I10" s="21">
         <f>SUM(I5:I9)</f>
         <v>0</v>
       </c>
-      <c r="K10" s="20">
+      <c r="K10" s="19">
         <f>SUM(K5:K9)</f>
         <v>5000</v>
       </c>
-      <c r="L10" s="21">
+      <c r="L10" s="20">
         <f>SUM(L5:L9)</f>
         <v>1800</v>
       </c>
-      <c r="M10" s="22">
+      <c r="M10" s="21">
         <f>SUM(M5:M9)</f>
         <v>3200</v>
       </c>
-      <c r="O10" s="23">
+      <c r="O10" s="22">
         <f>SUM(O5:O9)</f>
         <v>1600</v>
       </c>
-      <c r="P10" s="24">
+      <c r="P10" s="23">
         <f>SUM(P5:P9)</f>
         <v>1250</v>
       </c>
-      <c r="Q10" s="25">
+      <c r="Q10" s="24">
         <f>SUM(Q5:Q9)</f>
         <v>350</v>
       </c>
@@ -1275,21 +1278,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AD55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E52" sqref="E52"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I45" sqref="I45"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="29" customWidth="1"/>
-    <col min="2" max="2" width="17.44140625" customWidth="1"/>
+    <col min="2" max="2" width="17.5" customWidth="1"/>
     <col min="3" max="3" width="15.6640625" customWidth="1"/>
-    <col min="4" max="5" width="8.44140625" customWidth="1"/>
+    <col min="4" max="5" width="8.5" customWidth="1"/>
     <col min="6" max="6" width="10.6640625" customWidth="1"/>
-    <col min="7" max="1025" width="8.44140625" customWidth="1"/>
+    <col min="7" max="1025" width="8.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:30" x14ac:dyDescent="0.2">
       <c r="B1" t="s">
         <v>13</v>
       </c>
@@ -1299,21 +1302,21 @@
       <c r="D1" t="s">
         <v>15</v>
       </c>
-      <c r="E1" s="26"/>
+      <c r="E1" s="25"/>
       <c r="F1" t="s">
         <v>16</v>
       </c>
-      <c r="H1" s="27"/>
+      <c r="H1" s="26"/>
       <c r="I1" t="s">
         <v>17</v>
       </c>
-      <c r="K1" s="28"/>
+      <c r="K1" s="27"/>
       <c r="L1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:30" x14ac:dyDescent="0.3">
-      <c r="A2" s="29" t="s">
+    <row r="2" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="A2" s="28" t="s">
         <v>7</v>
       </c>
       <c r="D2" t="s">
@@ -1398,7 +1401,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="3" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>20</v>
       </c>
@@ -1409,7 +1412,7 @@
         <v>1.36</v>
       </c>
     </row>
-    <row r="4" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>21</v>
       </c>
@@ -1420,7 +1423,7 @@
         <v>0.45</v>
       </c>
     </row>
-    <row r="10" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>22</v>
       </c>
@@ -1433,12 +1436,12 @@
         <v>1.81</v>
       </c>
     </row>
-    <row r="11" spans="1:30" x14ac:dyDescent="0.3">
-      <c r="A11" s="30" t="s">
+    <row r="11" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="A11" s="29" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>22</v>
       </c>
@@ -1451,15 +1454,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A21" s="30" t="s">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A21" s="29" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="E22" s="31"/>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E22" s="30"/>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>22</v>
       </c>
@@ -1472,12 +1475,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A29" s="30" t="s">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A29" s="29" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>22</v>
       </c>
@@ -1490,54 +1493,68 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A37" s="30" t="s">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A37" s="29" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>20</v>
+        <v>41</v>
       </c>
       <c r="B38">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="C38">
-        <v>1</v>
-      </c>
-      <c r="E38" s="26"/>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
+        <v>0</v>
+      </c>
+      <c r="E38" s="27"/>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>21</v>
+        <v>42</v>
       </c>
       <c r="B39">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="C39">
-        <v>1</v>
-      </c>
-      <c r="E39" s="26"/>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
+        <v>0</v>
+      </c>
+      <c r="E39" s="27"/>
+      <c r="F39" s="27"/>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>43</v>
+      </c>
+      <c r="B40">
+        <v>6</v>
+      </c>
+      <c r="C40">
+        <v>0</v>
+      </c>
+      <c r="E40" s="27"/>
+      <c r="F40" s="27"/>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>22</v>
       </c>
       <c r="B45">
         <f>SUM(B38:B44)</f>
-        <v>2</v>
+        <v>12.5</v>
       </c>
       <c r="C45">
         <f>SUM(C38:C44)</f>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A46" s="30" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A46" s="29" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>20</v>
       </c>
@@ -1547,9 +1564,9 @@
       <c r="C47">
         <v>1</v>
       </c>
-      <c r="E47" s="26"/>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E47" s="25"/>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>21</v>
       </c>
@@ -1559,9 +1576,9 @@
       <c r="C48">
         <v>1</v>
       </c>
-      <c r="E48" s="26"/>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E48" s="25"/>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>22</v>
       </c>
@@ -1574,30 +1591,30 @@
         <v>2</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>23</v>
       </c>
       <c r="B54">
         <f>SUM(B28,B36,B20,B10,B45,B53)</f>
-        <v>5.5</v>
+        <v>16</v>
       </c>
       <c r="C54">
         <f>SUM(C10,C20,C28,C36,C45,C53)</f>
-        <v>5.8100000000000005</v>
-      </c>
-    </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.3">
+        <v>3.81</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>24</v>
       </c>
-      <c r="B55" s="32">
+      <c r="B55" s="31">
         <f>B54*100</f>
-        <v>550</v>
-      </c>
-      <c r="C55" s="32">
+        <v>1600</v>
+      </c>
+      <c r="C55" s="31">
         <f>C54*100</f>
-        <v>581</v>
+        <v>381</v>
       </c>
     </row>
   </sheetData>
@@ -1614,324 +1631,324 @@
       <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1025" width="8.44140625" customWidth="1"/>
+    <col min="1" max="1025" width="8.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="B1" s="33" t="s">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="B1" s="32" t="s">
         <v>25</v>
       </c>
-      <c r="C1" s="34">
+      <c r="C1" s="33">
         <v>43489</v>
       </c>
-      <c r="D1" s="34">
+      <c r="D1" s="33">
         <v>43494</v>
       </c>
-      <c r="E1" s="34">
+      <c r="E1" s="33">
         <v>43496</v>
       </c>
-      <c r="F1" s="34">
+      <c r="F1" s="33">
         <v>43497</v>
       </c>
-      <c r="G1" s="35">
+      <c r="G1" s="34">
         <v>43502</v>
       </c>
-      <c r="H1" s="33" t="s">
+      <c r="H1" s="32" t="s">
         <v>26</v>
       </c>
-      <c r="I1" s="33" t="s">
+      <c r="I1" s="32" t="s">
         <v>26</v>
       </c>
-      <c r="J1" s="33" t="s">
+      <c r="J1" s="32" t="s">
         <v>26</v>
       </c>
-      <c r="K1" s="33" t="s">
+      <c r="K1" s="32" t="s">
         <v>26</v>
       </c>
-      <c r="L1" s="33" t="s">
+      <c r="L1" s="32" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="62.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="33" t="s">
+    <row r="2" spans="1:12" ht="62.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B2" s="32" t="s">
         <v>27</v>
       </c>
-      <c r="C2" s="36" t="s">
+      <c r="C2" s="35" t="s">
         <v>28</v>
       </c>
-      <c r="D2" s="36" t="s">
+      <c r="D2" s="35" t="s">
         <v>29</v>
       </c>
-      <c r="E2" s="36" t="s">
+      <c r="E2" s="35" t="s">
         <v>29</v>
       </c>
-      <c r="F2" s="36" t="s">
+      <c r="F2" s="35" t="s">
         <v>29</v>
       </c>
-      <c r="G2" s="36" t="s">
+      <c r="G2" s="35" t="s">
         <v>26</v>
       </c>
-      <c r="H2" s="36" t="s">
+      <c r="H2" s="35" t="s">
         <v>26</v>
       </c>
-      <c r="I2" s="36" t="s">
+      <c r="I2" s="35" t="s">
         <v>26</v>
       </c>
-      <c r="J2" s="36" t="s">
+      <c r="J2" s="35" t="s">
         <v>26</v>
       </c>
-      <c r="K2" s="36" t="s">
+      <c r="K2" s="35" t="s">
         <v>26</v>
       </c>
-      <c r="L2" s="36" t="s">
+      <c r="L2" s="35" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="B3" s="33" t="s">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="B3" s="32" t="s">
         <v>30</v>
       </c>
-      <c r="C3" s="33">
+      <c r="C3" s="32">
         <v>1.5</v>
       </c>
-      <c r="D3" s="33">
+      <c r="D3" s="32">
         <v>0.5</v>
       </c>
-      <c r="E3" s="33">
+      <c r="E3" s="32">
         <v>0.5</v>
       </c>
-      <c r="F3" s="33">
+      <c r="F3" s="32">
         <v>1</v>
       </c>
-      <c r="G3" s="33">
+      <c r="G3" s="32">
         <v>0.5</v>
       </c>
-      <c r="H3" s="33">
-        <v>0</v>
-      </c>
-      <c r="I3" s="33">
-        <v>0</v>
-      </c>
-      <c r="J3" s="33">
-        <v>0</v>
-      </c>
-      <c r="K3" s="33">
-        <v>0</v>
-      </c>
-      <c r="L3" s="33">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A4" s="33" t="s">
+      <c r="H3" s="32">
+        <v>0</v>
+      </c>
+      <c r="I3" s="32">
+        <v>0</v>
+      </c>
+      <c r="J3" s="32">
+        <v>0</v>
+      </c>
+      <c r="K3" s="32">
+        <v>0</v>
+      </c>
+      <c r="L3" s="32">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A4" s="32" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="33">
+      <c r="B4" s="32">
         <f t="shared" ref="B4:B9" si="0">SUMIF(C4:L4,A$12,C$3:Z$3)</f>
         <v>4</v>
       </c>
-      <c r="C4" s="37" t="s">
-        <v>31</v>
-      </c>
-      <c r="D4" s="37" t="s">
-        <v>31</v>
-      </c>
-      <c r="E4" s="37" t="s">
-        <v>31</v>
-      </c>
-      <c r="F4" s="37" t="s">
-        <v>31</v>
-      </c>
-      <c r="G4" s="37" t="s">
-        <v>31</v>
-      </c>
-      <c r="H4" s="37"/>
-      <c r="I4" s="37"/>
-      <c r="J4" s="37"/>
-      <c r="K4" s="37"/>
-      <c r="L4" s="37"/>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A5" s="33" t="s">
+      <c r="C4" s="36" t="s">
+        <v>31</v>
+      </c>
+      <c r="D4" s="36" t="s">
+        <v>31</v>
+      </c>
+      <c r="E4" s="36" t="s">
+        <v>31</v>
+      </c>
+      <c r="F4" s="36" t="s">
+        <v>31</v>
+      </c>
+      <c r="G4" s="36" t="s">
+        <v>31</v>
+      </c>
+      <c r="H4" s="36"/>
+      <c r="I4" s="36"/>
+      <c r="J4" s="36"/>
+      <c r="K4" s="36"/>
+      <c r="L4" s="36"/>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A5" s="32" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="33">
+      <c r="B5" s="32">
         <f t="shared" si="0"/>
         <v>3.5</v>
       </c>
-      <c r="C5" s="37" t="s">
-        <v>31</v>
-      </c>
-      <c r="D5" s="37"/>
-      <c r="E5" s="37" t="s">
-        <v>31</v>
-      </c>
-      <c r="F5" s="37" t="s">
-        <v>31</v>
-      </c>
-      <c r="G5" s="37" t="s">
-        <v>31</v>
-      </c>
-      <c r="J5" s="37"/>
-      <c r="K5" s="37"/>
-      <c r="L5" s="37"/>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A6" s="33" t="s">
+      <c r="C5" s="36" t="s">
+        <v>31</v>
+      </c>
+      <c r="D5" s="36"/>
+      <c r="E5" s="36" t="s">
+        <v>31</v>
+      </c>
+      <c r="F5" s="36" t="s">
+        <v>31</v>
+      </c>
+      <c r="G5" s="36" t="s">
+        <v>31</v>
+      </c>
+      <c r="J5" s="36"/>
+      <c r="K5" s="36"/>
+      <c r="L5" s="36"/>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A6" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="B6" s="33">
+      <c r="B6" s="32">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="C6" s="37" t="s">
-        <v>31</v>
-      </c>
-      <c r="D6" s="37" t="s">
-        <v>31</v>
-      </c>
-      <c r="E6" s="37" t="s">
-        <v>31</v>
-      </c>
-      <c r="F6" s="37" t="s">
-        <v>31</v>
-      </c>
-      <c r="G6" s="37" t="s">
-        <v>31</v>
-      </c>
-      <c r="H6" s="37"/>
-      <c r="I6" s="37"/>
-      <c r="J6" s="37"/>
-      <c r="K6" s="37"/>
-      <c r="L6" s="37"/>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A7" s="33" t="s">
+      <c r="C6" s="36" t="s">
+        <v>31</v>
+      </c>
+      <c r="D6" s="36" t="s">
+        <v>31</v>
+      </c>
+      <c r="E6" s="36" t="s">
+        <v>31</v>
+      </c>
+      <c r="F6" s="36" t="s">
+        <v>31</v>
+      </c>
+      <c r="G6" s="36" t="s">
+        <v>31</v>
+      </c>
+      <c r="H6" s="36"/>
+      <c r="I6" s="36"/>
+      <c r="J6" s="36"/>
+      <c r="K6" s="36"/>
+      <c r="L6" s="36"/>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A7" s="32" t="s">
         <v>10</v>
       </c>
-      <c r="B7" s="33">
+      <c r="B7" s="32">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="C7" s="37" t="s">
-        <v>31</v>
-      </c>
-      <c r="D7" s="37" t="s">
-        <v>31</v>
-      </c>
-      <c r="E7" s="37" t="s">
-        <v>31</v>
-      </c>
-      <c r="F7" s="37" t="s">
-        <v>31</v>
-      </c>
-      <c r="G7" s="37" t="s">
-        <v>31</v>
-      </c>
-      <c r="H7" s="37"/>
-      <c r="I7" s="37"/>
-      <c r="J7" s="37"/>
-      <c r="K7" s="37"/>
-      <c r="L7" s="37"/>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A8" s="33" t="s">
+      <c r="C7" s="36" t="s">
+        <v>31</v>
+      </c>
+      <c r="D7" s="36" t="s">
+        <v>31</v>
+      </c>
+      <c r="E7" s="36" t="s">
+        <v>31</v>
+      </c>
+      <c r="F7" s="36" t="s">
+        <v>31</v>
+      </c>
+      <c r="G7" s="36" t="s">
+        <v>31</v>
+      </c>
+      <c r="H7" s="36"/>
+      <c r="I7" s="36"/>
+      <c r="J7" s="36"/>
+      <c r="K7" s="36"/>
+      <c r="L7" s="36"/>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A8" s="32" t="s">
         <v>11</v>
       </c>
-      <c r="B8" s="33">
+      <c r="B8" s="32">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="C8" s="37" t="s">
-        <v>31</v>
-      </c>
-      <c r="D8" s="37" t="s">
-        <v>31</v>
-      </c>
-      <c r="E8" s="37" t="s">
-        <v>31</v>
-      </c>
-      <c r="F8" s="37" t="s">
-        <v>31</v>
-      </c>
-      <c r="G8" s="37" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A9" s="33" t="s">
+      <c r="C8" s="36" t="s">
+        <v>31</v>
+      </c>
+      <c r="D8" s="36" t="s">
+        <v>31</v>
+      </c>
+      <c r="E8" s="36" t="s">
+        <v>31</v>
+      </c>
+      <c r="F8" s="36" t="s">
+        <v>31</v>
+      </c>
+      <c r="G8" s="36" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A9" s="32" t="s">
         <v>12</v>
       </c>
-      <c r="B9" s="33">
+      <c r="B9" s="32">
         <f t="shared" si="0"/>
         <v>2.5</v>
       </c>
-      <c r="D9" s="37" t="s">
-        <v>31</v>
-      </c>
-      <c r="E9" s="37" t="s">
-        <v>31</v>
-      </c>
-      <c r="F9" s="37" t="s">
-        <v>31</v>
-      </c>
-      <c r="G9" s="37" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A10" s="33" t="s">
-        <v>0</v>
-      </c>
-      <c r="B10" s="33">
+      <c r="D9" s="36" t="s">
+        <v>31</v>
+      </c>
+      <c r="E9" s="36" t="s">
+        <v>31</v>
+      </c>
+      <c r="F9" s="36" t="s">
+        <v>31</v>
+      </c>
+      <c r="G9" s="36" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A10" s="32" t="s">
+        <v>0</v>
+      </c>
+      <c r="B10" s="32">
         <f>SUM(B4:B7)</f>
         <v>15.5</v>
       </c>
-      <c r="C10" s="33">
+      <c r="C10" s="32">
         <f t="shared" ref="C10:L10" si="1">COUNTIF(C4:C7,"*ü*") * C3</f>
         <v>6</v>
       </c>
-      <c r="D10" s="33">
+      <c r="D10" s="32">
         <f t="shared" si="1"/>
         <v>1.5</v>
       </c>
-      <c r="E10" s="33">
+      <c r="E10" s="32">
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
-      <c r="F10" s="33">
+      <c r="F10" s="32">
         <f t="shared" si="1"/>
         <v>4</v>
       </c>
-      <c r="G10" s="33">
+      <c r="G10" s="32">
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
-      <c r="H10" s="33">
+      <c r="H10" s="32">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="I10" s="33">
+      <c r="I10" s="32">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="J10" s="33">
+      <c r="J10" s="32">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="K10" s="33">
+      <c r="K10" s="32">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="L10" s="33">
+      <c r="L10" s="32">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A12" s="37" t="s">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A12" s="36" t="s">
         <v>31</v>
       </c>
     </row>
@@ -1945,29 +1962,29 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:S34"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="15" customWidth="1"/>
     <col min="2" max="2" width="29.6640625" customWidth="1"/>
-    <col min="3" max="3" width="14.44140625" customWidth="1"/>
-    <col min="4" max="4" width="10.44140625" customWidth="1"/>
+    <col min="3" max="3" width="14.5" customWidth="1"/>
+    <col min="4" max="4" width="10.5" customWidth="1"/>
     <col min="5" max="19" width="3.6640625" customWidth="1"/>
-    <col min="20" max="1025" width="8.44140625" customWidth="1"/>
+    <col min="20" max="1025" width="8.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A1" s="38"/>
-      <c r="B1" s="39" t="s">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A1" s="37"/>
+      <c r="B1" s="38" t="s">
         <v>32</v>
       </c>
-      <c r="C1" s="39" t="s">
+      <c r="C1" s="38" t="s">
         <v>33</v>
       </c>
-      <c r="D1" s="40" t="s">
+      <c r="D1" s="39" t="s">
         <v>34</v>
       </c>
       <c r="E1">
@@ -2016,331 +2033,331 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A2" s="3" t="s">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="C2" s="41"/>
-      <c r="D2" s="42"/>
-    </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="B3" s="4" t="s">
+      <c r="C2" s="40"/>
+      <c r="D2" s="41"/>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="B3" s="3" t="s">
         <v>36</v>
       </c>
       <c r="C3">
         <v>1</v>
       </c>
-      <c r="D3" s="42">
+      <c r="D3" s="41">
         <v>0.75</v>
       </c>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="B4" s="4" t="s">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="B4" s="3" t="s">
         <v>37</v>
       </c>
       <c r="C4">
         <v>3</v>
       </c>
-      <c r="D4" s="42">
+      <c r="D4" s="41">
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="B5" s="4" t="s">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="B5" s="3" t="s">
         <v>38</v>
       </c>
       <c r="C5">
         <v>1</v>
       </c>
-      <c r="D5" s="42">
+      <c r="D5" s="41">
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A6" s="43"/>
-      <c r="B6" s="4" t="s">
+    <row r="6" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A6" s="42"/>
+      <c r="B6" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="C6" s="4">
+      <c r="C6" s="3">
         <f>SUM(C2:C5)</f>
         <v>5</v>
       </c>
-      <c r="D6" s="5">
+      <c r="D6" s="4">
         <f>SUM(D2:D5)</f>
         <v>8.75</v>
       </c>
     </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A7" s="3" t="s">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A7" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="4" t="s">
+      <c r="B7" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="C7" s="41"/>
-      <c r="D7" s="42"/>
-    </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="B8" s="4" t="s">
+      <c r="C7" s="40"/>
+      <c r="D7" s="41"/>
+    </row>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="B8" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="D8" s="42"/>
-    </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="B9" s="4" t="s">
+      <c r="D8" s="41"/>
+    </row>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="B9" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="D9" s="42"/>
-    </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="B10" s="4" t="s">
+      <c r="D9" s="41"/>
+    </row>
+    <row r="10" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="B10" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="D10" s="42"/>
-    </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A11" s="43"/>
-      <c r="B11" s="4" t="s">
+      <c r="D10" s="41"/>
+    </row>
+    <row r="11" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A11" s="42"/>
+      <c r="B11" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="C11" s="4">
+      <c r="C11" s="3">
         <f>SUM(C7:C10)</f>
         <v>0</v>
       </c>
-      <c r="D11" s="5">
+      <c r="D11" s="4">
         <f>SUM(D7:D10)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A12" s="3" t="s">
+    <row r="12" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A12" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B12" s="4" t="s">
+      <c r="B12" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="C12" s="41"/>
-      <c r="D12" s="42"/>
-    </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="B13" s="4" t="s">
+      <c r="C12" s="40"/>
+      <c r="D12" s="41"/>
+    </row>
+    <row r="13" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="B13" s="3" t="s">
         <v>40</v>
       </c>
       <c r="C13">
         <v>2</v>
       </c>
-      <c r="D13" s="42">
+      <c r="D13" s="41">
         <v>1.5</v>
       </c>
     </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="B14" s="4" t="s">
+    <row r="14" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="B14" s="3" t="s">
         <v>37</v>
       </c>
       <c r="C14">
         <v>4</v>
       </c>
-      <c r="D14" s="42">
+      <c r="D14" s="41">
         <v>3</v>
       </c>
     </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="B15" s="4" t="s">
+    <row r="15" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="B15" s="3" t="s">
         <v>38</v>
       </c>
       <c r="C15">
         <v>2</v>
       </c>
-      <c r="D15" s="42">
+      <c r="D15" s="41">
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="B16" s="4" t="s">
+    <row r="16" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="B16" s="3" t="s">
         <v>20</v>
       </c>
       <c r="C16">
         <v>1</v>
       </c>
-      <c r="D16" s="42">
+      <c r="D16" s="41">
         <v>0.75</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B17" s="4" t="s">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B17" s="3" t="s">
         <v>21</v>
       </c>
       <c r="C17">
         <v>1</v>
       </c>
-      <c r="D17" s="42">
+      <c r="D17" s="41">
         <v>0.25</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A18" s="43"/>
-      <c r="B18" s="44" t="s">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A18" s="42"/>
+      <c r="B18" s="43" t="s">
         <v>39</v>
       </c>
-      <c r="C18" s="4">
+      <c r="C18" s="3">
         <f>SUM(C12:C17)</f>
         <v>10</v>
       </c>
-      <c r="D18" s="5">
+      <c r="D18" s="4">
         <f>SUM(D12:D17)</f>
         <v>6.5</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A19" s="3" t="s">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A19" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B19" s="4" t="s">
+      <c r="B19" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="C19" s="41"/>
-      <c r="D19" s="42"/>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B20" s="4" t="s">
+      <c r="C19" s="40"/>
+      <c r="D19" s="41"/>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B20" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="D20" s="42"/>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B21" s="4" t="s">
+      <c r="D20" s="41"/>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B21" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="D21" s="42"/>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B22" s="4" t="s">
+      <c r="D21" s="41"/>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B22" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="D22" s="42"/>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A23" s="43"/>
-      <c r="B23" s="44" t="s">
+      <c r="D22" s="41"/>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A23" s="42"/>
+      <c r="B23" s="43" t="s">
         <v>39</v>
       </c>
-      <c r="C23" s="4">
+      <c r="C23" s="3">
         <f>SUM(C19:C22)</f>
         <v>0</v>
       </c>
-      <c r="D23" s="5">
+      <c r="D23" s="4">
         <f>SUM(D19:D22)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A24" s="3" t="s">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A24" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B24" s="4" t="s">
+      <c r="B24" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="D24" s="42"/>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B25" s="4" t="s">
+      <c r="D24" s="41"/>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B25" s="3" t="s">
         <v>40</v>
       </c>
       <c r="C25">
         <v>1.5</v>
       </c>
-      <c r="D25" s="42">
+      <c r="D25" s="41">
         <v>1.5</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B26" s="4" t="s">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B26" s="3" t="s">
         <v>37</v>
       </c>
       <c r="C26">
         <v>3</v>
       </c>
-      <c r="D26" s="42">
+      <c r="D26" s="41">
         <v>3</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B27" s="4" t="s">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B27" s="3" t="s">
         <v>38</v>
       </c>
       <c r="C27">
         <v>1.5</v>
       </c>
-      <c r="D27" s="42">
+      <c r="D27" s="41">
         <v>1.5</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B28" s="44" t="s">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B28" s="43" t="s">
         <v>39</v>
       </c>
-      <c r="C28" s="4">
+      <c r="C28" s="3">
         <f>SUM(C24:C27)</f>
         <v>6</v>
       </c>
-      <c r="D28" s="5">
+      <c r="D28" s="4">
         <f>SUM(D24:D27)</f>
         <v>6</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A29" s="3" t="s">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A29" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B29" s="4" t="s">
+      <c r="B29" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="D29" s="42"/>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B30" s="4" t="s">
+      <c r="D29" s="41"/>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B30" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="D30" s="42"/>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B31" s="4" t="s">
+      <c r="D30" s="41"/>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B31" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="D31" s="42"/>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B32" s="4" t="s">
+      <c r="D31" s="41"/>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B32" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="D32" s="42"/>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B33" s="44" t="s">
+      <c r="D32" s="41"/>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B33" s="43" t="s">
         <v>39</v>
       </c>
-      <c r="C33" s="4">
+      <c r="C33" s="3">
         <f>SUM(C29:C32)</f>
         <v>0</v>
       </c>
-      <c r="D33" s="5">
+      <c r="D33" s="4">
         <f>SUM(D29:D32)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A34" s="45"/>
-      <c r="B34" s="46" t="s">
-        <v>0</v>
-      </c>
-      <c r="C34" s="7">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A34" s="44"/>
+      <c r="B34" s="45" t="s">
+        <v>0</v>
+      </c>
+      <c r="C34" s="6">
         <f>SUM(C6,C11,C18,C23,C28,C33)</f>
         <v>21</v>
       </c>
-      <c r="D34" s="8">
+      <c r="D34" s="7">
         <f>SUM(D6,D11,D18,D23,D28,D33)</f>
         <v>21.25</v>
       </c>

</xml_diff>

<commit_message>
Added wave machine creation to Gantt
</commit_message>
<xml_diff>
--- a/docs/ganttChart.xlsx
+++ b/docs/ganttChart.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="46">
   <si>
     <t xml:space="preserve">Total</t>
   </si>
@@ -92,6 +92,9 @@
   </si>
   <si>
     <t xml:space="preserve">Add NavMesh</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Set up Wave Machine</t>
   </si>
   <si>
     <t xml:space="preserve">totals</t>
@@ -568,12 +571,12 @@
     </xf>
   </cellXfs>
   <cellStyles count="6">
-    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Comma" xfId="15" builtinId="3"/>
+    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
+    <cellStyle name="Currency" xfId="17" builtinId="4"/>
+    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
+    <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
   <colors>
     <indexedColors>
@@ -651,7 +654,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="8.51"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="8.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="14.16"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="13.83"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="13.33"/>
@@ -667,7 +670,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="12.33"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="14.66"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="11.33"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="18" style="0" width="8.51"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="18" style="0" width="8.52"/>
   </cols>
   <sheetData>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1110,12 +1113,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="28.99"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="17.51"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="28.98"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="17.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="15.66"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="4" style="0" width="8.51"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="10.66"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="7" style="0" width="8.51"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="4" style="0" width="8.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="10.65"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="7" style="0" width="8.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1257,17 +1260,28 @@
         <v>1</v>
       </c>
     </row>
+    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="B6" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="C6" s="0" t="n">
+        <v>3.52</v>
+      </c>
+    </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B10" s="0" t="n">
         <f aca="false">SUM(B3:B9)</f>
-        <v>1.5</v>
+        <v>4.5</v>
       </c>
       <c r="C10" s="0" t="n">
         <f aca="false">SUM(C3:C9)</f>
-        <v>2.81</v>
+        <v>6.33</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1277,7 +1291,7 @@
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B20" s="0" t="n">
         <f aca="false">SUM(B12:B19)</f>
@@ -1298,7 +1312,7 @@
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B28" s="0" t="n">
         <f aca="false">SUM(B22:B27)</f>
@@ -1316,7 +1330,7 @@
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B36" s="0" t="n">
         <f aca="false">SUM(B30:B35)</f>
@@ -1334,7 +1348,7 @@
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B38" s="0" t="n">
         <v>0.5</v>
@@ -1346,7 +1360,7 @@
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B39" s="0" t="n">
         <v>6</v>
@@ -1359,7 +1373,7 @@
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B40" s="0" t="n">
         <v>6</v>
@@ -1372,7 +1386,7 @@
     </row>
     <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B45" s="0" t="n">
         <f aca="false">SUM(B38:B44)</f>
@@ -1414,7 +1428,7 @@
     </row>
     <row r="53" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B53" s="0" t="n">
         <f aca="false">SUM(B47:B52)</f>
@@ -1427,28 +1441,28 @@
     </row>
     <row r="54" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="0" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B54" s="0" t="n">
         <f aca="false">SUM(B28,B36,B20,B10,B45,B53)</f>
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="C54" s="0" t="n">
         <f aca="false">SUM(C10,C20,C28,C36,C45,C53)</f>
-        <v>4.81</v>
+        <v>8.33</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="0" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B55" s="32" t="n">
         <f aca="false">B54*100</f>
-        <v>1600</v>
+        <v>1900</v>
       </c>
       <c r="C55" s="32" t="n">
         <f aca="false">C54*100</f>
-        <v>481</v>
+        <v>833</v>
       </c>
     </row>
   </sheetData>
@@ -1475,12 +1489,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="8.51"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="8.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B1" s="33" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C1" s="34" t="n">
         <v>43489</v>
@@ -1498,59 +1512,59 @@
         <v>43502</v>
       </c>
       <c r="H1" s="33" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="I1" s="33" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="J1" s="33" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="K1" s="33" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="L1" s="33" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="62.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B2" s="33" t="s">
+        <v>32</v>
+      </c>
+      <c r="C2" s="36" t="s">
+        <v>33</v>
+      </c>
+      <c r="D2" s="36" t="s">
+        <v>34</v>
+      </c>
+      <c r="E2" s="36" t="s">
+        <v>34</v>
+      </c>
+      <c r="F2" s="36" t="s">
+        <v>34</v>
+      </c>
+      <c r="G2" s="36" t="s">
         <v>31</v>
       </c>
-      <c r="C2" s="36" t="s">
-        <v>32</v>
-      </c>
-      <c r="D2" s="36" t="s">
-        <v>33</v>
-      </c>
-      <c r="E2" s="36" t="s">
-        <v>33</v>
-      </c>
-      <c r="F2" s="36" t="s">
-        <v>33</v>
-      </c>
-      <c r="G2" s="36" t="s">
-        <v>30</v>
-      </c>
       <c r="H2" s="36" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="I2" s="36" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="J2" s="36" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="K2" s="36" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="L2" s="36" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B3" s="33" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C3" s="33" t="n">
         <v>1.5</v>
@@ -1592,19 +1606,19 @@
         <v>4</v>
       </c>
       <c r="C4" s="37" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D4" s="37" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="E4" s="37" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="F4" s="37" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="G4" s="37" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="H4" s="37"/>
       <c r="I4" s="37"/>
@@ -1621,17 +1635,17 @@
         <v>3.5</v>
       </c>
       <c r="C5" s="37" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D5" s="37"/>
       <c r="E5" s="37" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="F5" s="37" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="G5" s="37" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="J5" s="37"/>
       <c r="K5" s="37"/>
@@ -1646,19 +1660,19 @@
         <v>4</v>
       </c>
       <c r="C6" s="37" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D6" s="37" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="E6" s="37" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="F6" s="37" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="G6" s="37" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="H6" s="37"/>
       <c r="I6" s="37"/>
@@ -1675,19 +1689,19 @@
         <v>4</v>
       </c>
       <c r="C7" s="37" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D7" s="37" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="E7" s="37" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="F7" s="37" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="G7" s="37" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="H7" s="37"/>
       <c r="I7" s="37"/>
@@ -1704,19 +1718,19 @@
         <v>4</v>
       </c>
       <c r="C8" s="37" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D8" s="37" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="E8" s="37" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="F8" s="37" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="G8" s="37" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1728,16 +1742,16 @@
         <v>2.5</v>
       </c>
       <c r="D9" s="37" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="E9" s="37" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="F9" s="37" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="G9" s="37" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1791,7 +1805,7 @@
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="37" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
   </sheetData>
@@ -1822,20 +1836,20 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="29.66"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="14.5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="10.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="5" style="0" width="3.66"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="20" style="0" width="8.51"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="5" style="0" width="3.65"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="20" style="0" width="8.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="38"/>
       <c r="B1" s="39" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C1" s="39" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D1" s="40" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="E1" s="0" t="n">
         <v>1</v>
@@ -1888,14 +1902,14 @@
         <v>7</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C2" s="41"/>
       <c r="D2" s="42"/>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B3" s="4" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C3" s="0" t="n">
         <v>1</v>
@@ -1906,7 +1920,7 @@
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B4" s="4" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C4" s="0" t="n">
         <v>3</v>
@@ -1917,7 +1931,7 @@
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B5" s="4" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C5" s="0" t="n">
         <v>1</v>
@@ -1929,7 +1943,7 @@
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="43"/>
       <c r="B6" s="4" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C6" s="4" t="n">
         <f aca="false">SUM(C2:C5)</f>
@@ -1945,33 +1959,33 @@
         <v>8</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C7" s="41"/>
       <c r="D7" s="42"/>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B8" s="4" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="D8" s="42"/>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B9" s="4" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D9" s="42"/>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B10" s="4" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="D10" s="42"/>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="43"/>
       <c r="B11" s="4" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C11" s="4" t="n">
         <f aca="false">SUM(C7:C10)</f>
@@ -1987,14 +2001,14 @@
         <v>9</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C12" s="41"/>
       <c r="D12" s="42"/>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B13" s="4" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C13" s="0" t="n">
         <v>2</v>
@@ -2005,7 +2019,7 @@
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B14" s="4" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C14" s="0" t="n">
         <v>4</v>
@@ -2016,7 +2030,7 @@
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B15" s="4" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C15" s="0" t="n">
         <v>2</v>
@@ -2050,7 +2064,7 @@
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="43"/>
       <c r="B18" s="44" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C18" s="4" t="n">
         <f aca="false">SUM(C12:C17)</f>
@@ -2066,33 +2080,33 @@
         <v>10</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C19" s="41"/>
       <c r="D19" s="42"/>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B20" s="4" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="D20" s="42"/>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B21" s="4" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D21" s="42"/>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B22" s="4" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="D22" s="42"/>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="43"/>
       <c r="B23" s="44" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C23" s="4" t="n">
         <f aca="false">SUM(C19:C22)</f>
@@ -2108,13 +2122,13 @@
         <v>11</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D24" s="42"/>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B25" s="4" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C25" s="0" t="n">
         <v>1.5</v>
@@ -2125,7 +2139,7 @@
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B26" s="4" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C26" s="0" t="n">
         <v>3</v>
@@ -2136,7 +2150,7 @@
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B27" s="4" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C27" s="0" t="n">
         <v>1.5</v>
@@ -2147,7 +2161,7 @@
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B28" s="44" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C28" s="4" t="n">
         <f aca="false">SUM(C24:C27)</f>
@@ -2163,31 +2177,31 @@
         <v>12</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D29" s="42"/>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B30" s="4" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="D30" s="42"/>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B31" s="4" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D31" s="42"/>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B32" s="4" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="D32" s="42"/>
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B33" s="44" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C33" s="4" t="n">
         <f aca="false">SUM(C29:C32)</f>

</xml_diff>

<commit_message>
updated Nate's part of the gantt chart
</commit_message>
<xml_diff>
--- a/docs/ganttChart.xlsx
+++ b/docs/ganttChart.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21328"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nathan\School\Spring 2019\CS 383\GitRepos\banana\docs\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88733FC8-6997-46B2-82D3-08FE38BEB2FE}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500" activeTab="3"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Management Summary" sheetId="1" r:id="rId1"/>
@@ -12,8 +18,14 @@
     <sheet name="Meetings" sheetId="3" r:id="rId3"/>
     <sheet name="SA" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="191029"/>
   <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
+    </ext>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
     </ext>
@@ -174,7 +186,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="3">
     <numFmt numFmtId="164" formatCode="\$#,##0.00_);[Red]&quot;($&quot;#,##0.00\)"/>
     <numFmt numFmtId="165" formatCode="\$#,##0.00;[Red]\$#,##0.00"/>
@@ -410,28 +422,25 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
@@ -445,27 +454,28 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="15" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="166" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -544,6 +554,9 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -591,7 +604,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -624,9 +637,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -659,6 +689,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -834,440 +881,440 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:Q10"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="L7" sqref="L7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="2" width="8.5703125" customWidth="1"/>
-    <col min="3" max="3" width="14.140625" customWidth="1"/>
-    <col min="4" max="4" width="13.85546875" customWidth="1"/>
-    <col min="5" max="5" width="13.28515625" customWidth="1"/>
-    <col min="6" max="6" width="3.42578125" customWidth="1"/>
-    <col min="7" max="7" width="15.28515625" customWidth="1"/>
-    <col min="8" max="8" width="12.28515625" customWidth="1"/>
-    <col min="9" max="9" width="14.42578125" customWidth="1"/>
-    <col min="10" max="10" width="2.85546875" customWidth="1"/>
-    <col min="11" max="11" width="13.85546875" customWidth="1"/>
+    <col min="1" max="2" width="8.5546875" customWidth="1"/>
+    <col min="3" max="3" width="14.109375" customWidth="1"/>
+    <col min="4" max="4" width="13.88671875" customWidth="1"/>
+    <col min="5" max="5" width="13.33203125" customWidth="1"/>
+    <col min="6" max="6" width="3.44140625" customWidth="1"/>
+    <col min="7" max="7" width="15.33203125" customWidth="1"/>
+    <col min="8" max="8" width="12.33203125" customWidth="1"/>
+    <col min="9" max="9" width="14.44140625" customWidth="1"/>
+    <col min="10" max="10" width="2.88671875" customWidth="1"/>
+    <col min="11" max="11" width="13.88671875" customWidth="1"/>
     <col min="12" max="12" width="14" customWidth="1"/>
-    <col min="13" max="13" width="14.140625" customWidth="1"/>
-    <col min="14" max="14" width="5.42578125" customWidth="1"/>
-    <col min="15" max="15" width="12.28515625" customWidth="1"/>
-    <col min="16" max="16" width="14.7109375" customWidth="1"/>
-    <col min="17" max="17" width="11.28515625" customWidth="1"/>
-    <col min="18" max="1025" width="8.5703125" customWidth="1"/>
+    <col min="13" max="13" width="14.109375" customWidth="1"/>
+    <col min="14" max="14" width="5.44140625" customWidth="1"/>
+    <col min="15" max="15" width="12.33203125" customWidth="1"/>
+    <col min="16" max="16" width="14.6640625" customWidth="1"/>
+    <col min="17" max="17" width="11.33203125" customWidth="1"/>
+    <col min="18" max="1025" width="8.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="C2" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
-      <c r="F2" s="2"/>
-      <c r="G2" s="1" t="s">
+    <row r="2" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="C2" s="46" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2" s="46"/>
+      <c r="E2" s="46"/>
+      <c r="F2" s="1"/>
+      <c r="G2" s="46" t="s">
         <v>1</v>
       </c>
-      <c r="H2" s="1"/>
-      <c r="I2" s="1"/>
-      <c r="K2" s="1" t="s">
+      <c r="H2" s="46"/>
+      <c r="I2" s="46"/>
+      <c r="K2" s="46" t="s">
         <v>2</v>
       </c>
-      <c r="L2" s="1"/>
-      <c r="M2" s="1"/>
-      <c r="O2" s="1" t="s">
+      <c r="L2" s="46"/>
+      <c r="M2" s="46"/>
+      <c r="O2" s="46" t="s">
         <v>3</v>
       </c>
-      <c r="P2" s="1"/>
-      <c r="Q2" s="1"/>
-    </row>
-    <row r="3" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="C3" s="3" t="s">
+      <c r="P2" s="46"/>
+      <c r="Q2" s="46"/>
+    </row>
+    <row r="3" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="C3" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="D3" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="E3" s="5" t="s">
+      <c r="E3" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="G3" s="6" t="s">
+      <c r="G3" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="H3" s="7" t="s">
+      <c r="H3" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="I3" s="8" t="s">
+      <c r="I3" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="K3" s="6" t="s">
+      <c r="K3" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="L3" s="7" t="s">
+      <c r="L3" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="M3" s="8" t="s">
+      <c r="M3" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="O3" s="3" t="s">
+      <c r="O3" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="P3" s="4" t="s">
+      <c r="P3" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="Q3" s="5" t="s">
+      <c r="Q3" s="4" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B4" s="9" t="s">
+    <row r="4" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="B4" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="10">
+      <c r="C4" s="9">
         <f t="shared" ref="C4:D8" si="0">(G4+K4+O4)</f>
         <v>1500</v>
       </c>
-      <c r="D4" s="11">
+      <c r="D4" s="10">
         <f t="shared" si="0"/>
         <v>1275</v>
       </c>
-      <c r="E4" s="12">
+      <c r="E4" s="11">
         <f t="shared" ref="E4:E9" si="1">(C4-D4)</f>
         <v>225</v>
       </c>
-      <c r="G4" s="13">
-        <v>0</v>
-      </c>
-      <c r="H4" s="14">
-        <v>0</v>
-      </c>
-      <c r="I4" s="15">
+      <c r="G4" s="12">
+        <v>0</v>
+      </c>
+      <c r="H4" s="13">
+        <v>0</v>
+      </c>
+      <c r="I4" s="14">
         <f t="shared" ref="I4:I9" si="2">(G4-H4)</f>
         <v>0</v>
       </c>
-      <c r="K4" s="10">
+      <c r="K4" s="9">
         <v>1000</v>
       </c>
-      <c r="L4" s="11">
+      <c r="L4" s="10">
         <f>Meetings!B4*100</f>
         <v>400</v>
       </c>
-      <c r="M4" s="12">
+      <c r="M4" s="11">
         <f t="shared" ref="M4:M9" si="3">(K4-L4)</f>
         <v>600</v>
       </c>
-      <c r="O4" s="10">
+      <c r="O4" s="9">
         <f>(SA!C6)*100</f>
         <v>500</v>
       </c>
-      <c r="P4" s="11">
+      <c r="P4" s="10">
         <f>(SA!D6)*100</f>
         <v>875</v>
       </c>
-      <c r="Q4" s="12">
+      <c r="Q4" s="11">
         <f t="shared" ref="Q4:Q9" si="4">(O4-P4)</f>
         <v>-375</v>
       </c>
     </row>
-    <row r="5" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B5" s="3" t="s">
+    <row r="5" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="B5" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="13">
+      <c r="C5" s="12">
         <f t="shared" si="0"/>
         <v>1000</v>
       </c>
-      <c r="D5" s="14">
+      <c r="D5" s="13">
         <f t="shared" si="0"/>
         <v>350</v>
       </c>
-      <c r="E5" s="15">
+      <c r="E5" s="14">
         <f t="shared" si="1"/>
         <v>650</v>
       </c>
-      <c r="G5" s="13">
-        <v>0</v>
-      </c>
-      <c r="H5" s="14">
-        <v>0</v>
-      </c>
-      <c r="I5" s="15">
+      <c r="G5" s="12">
+        <v>0</v>
+      </c>
+      <c r="H5" s="13">
+        <v>0</v>
+      </c>
+      <c r="I5" s="14">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="K5" s="13">
+      <c r="K5" s="12">
         <v>1000</v>
       </c>
-      <c r="L5" s="14">
+      <c r="L5" s="13">
         <f>Meetings!B5*100</f>
         <v>350</v>
       </c>
-      <c r="M5" s="15">
+      <c r="M5" s="14">
         <f t="shared" si="3"/>
         <v>650</v>
       </c>
-      <c r="O5" s="13">
+      <c r="O5" s="12">
         <f>(SA!C11)*100</f>
         <v>0</v>
       </c>
-      <c r="P5" s="14">
+      <c r="P5" s="13">
         <f>(SA!D11)*100</f>
         <v>0</v>
       </c>
-      <c r="Q5" s="15">
+      <c r="Q5" s="14">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B6" s="3" t="s">
+    <row r="6" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="B6" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C6" s="13">
+      <c r="C6" s="12">
         <f t="shared" si="0"/>
         <v>2000</v>
       </c>
-      <c r="D6" s="14">
+      <c r="D6" s="13">
         <f t="shared" si="0"/>
         <v>1050</v>
       </c>
-      <c r="E6" s="15">
+      <c r="E6" s="14">
         <f t="shared" si="1"/>
         <v>950</v>
       </c>
-      <c r="G6" s="13">
-        <v>0</v>
-      </c>
-      <c r="H6" s="14">
-        <v>0</v>
-      </c>
-      <c r="I6" s="15">
+      <c r="G6" s="12">
+        <v>0</v>
+      </c>
+      <c r="H6" s="13">
+        <v>0</v>
+      </c>
+      <c r="I6" s="14">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="K6" s="13">
+      <c r="K6" s="12">
         <v>1000</v>
       </c>
-      <c r="L6" s="14">
+      <c r="L6" s="13">
         <f>Meetings!B6*100</f>
         <v>400</v>
       </c>
-      <c r="M6" s="15">
+      <c r="M6" s="14">
         <f t="shared" si="3"/>
         <v>600</v>
       </c>
-      <c r="O6" s="13">
+      <c r="O6" s="12">
         <f>(SA!C18)*100</f>
         <v>1000</v>
       </c>
-      <c r="P6" s="14">
+      <c r="P6" s="13">
         <f>(SA!D18)*100</f>
         <v>650</v>
       </c>
-      <c r="Q6" s="15">
+      <c r="Q6" s="14">
         <f t="shared" si="4"/>
         <v>350</v>
       </c>
     </row>
-    <row r="7" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B7" s="3" t="s">
+    <row r="7" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="B7" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C7" s="13">
+      <c r="C7" s="12">
         <f t="shared" si="0"/>
         <v>1600</v>
       </c>
-      <c r="D7" s="14">
+      <c r="D7" s="13">
         <f t="shared" si="0"/>
         <v>1000</v>
       </c>
-      <c r="E7" s="15">
+      <c r="E7" s="14">
         <f t="shared" si="1"/>
         <v>600</v>
       </c>
-      <c r="G7" s="13">
-        <v>0</v>
-      </c>
-      <c r="H7" s="14">
-        <v>0</v>
-      </c>
-      <c r="I7" s="15">
+      <c r="G7" s="12">
+        <v>0</v>
+      </c>
+      <c r="H7" s="13">
+        <v>0</v>
+      </c>
+      <c r="I7" s="14">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="K7" s="13">
+      <c r="K7" s="12">
         <v>1000</v>
       </c>
-      <c r="L7" s="14">
+      <c r="L7" s="13">
         <f>Meetings!B7*100</f>
         <v>400</v>
       </c>
-      <c r="M7" s="15">
+      <c r="M7" s="14">
         <f t="shared" si="3"/>
         <v>600</v>
       </c>
-      <c r="O7" s="13">
+      <c r="O7" s="12">
         <f>(SA!C28)*100</f>
         <v>600</v>
       </c>
-      <c r="P7" s="14">
+      <c r="P7" s="13">
         <f>(SA!D28)*100</f>
         <v>600</v>
       </c>
-      <c r="Q7" s="15">
+      <c r="Q7" s="14">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B8" s="16" t="s">
+    <row r="8" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="B8" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="C8" s="14">
+      <c r="C8" s="13">
         <f t="shared" si="0"/>
         <v>1000</v>
       </c>
-      <c r="D8" s="14">
+      <c r="D8" s="13">
         <f t="shared" si="0"/>
         <v>400</v>
       </c>
-      <c r="E8" s="15">
+      <c r="E8" s="14">
         <f t="shared" si="1"/>
         <v>600</v>
       </c>
-      <c r="G8" s="13">
-        <v>0</v>
-      </c>
-      <c r="H8" s="14">
-        <v>0</v>
-      </c>
-      <c r="I8" s="15">
+      <c r="G8" s="12">
+        <v>0</v>
+      </c>
+      <c r="H8" s="13">
+        <v>0</v>
+      </c>
+      <c r="I8" s="14">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="K8" s="13">
+      <c r="K8" s="12">
         <v>1000</v>
       </c>
-      <c r="L8" s="14">
+      <c r="L8" s="13">
         <f>Meetings!B8*100</f>
         <v>400</v>
       </c>
-      <c r="M8" s="15">
+      <c r="M8" s="14">
         <f t="shared" si="3"/>
         <v>600</v>
       </c>
-      <c r="O8" s="13">
-        <v>0</v>
-      </c>
-      <c r="P8" s="14">
-        <v>0</v>
-      </c>
-      <c r="Q8" s="15">
+      <c r="O8" s="12">
+        <v>0</v>
+      </c>
+      <c r="P8" s="13">
+        <v>0</v>
+      </c>
+      <c r="Q8" s="14">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B9" s="16" t="s">
+    <row r="9" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="B9" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="C9" s="14">
+      <c r="C9" s="13">
         <f>+(G9+K9+O9)</f>
         <v>1000</v>
       </c>
-      <c r="D9" s="14">
+      <c r="D9" s="13">
         <f>(H9+L9+P9)</f>
         <v>250</v>
       </c>
-      <c r="E9" s="17">
+      <c r="E9" s="16">
         <f t="shared" si="1"/>
         <v>750</v>
       </c>
-      <c r="G9" s="13">
-        <v>0</v>
-      </c>
-      <c r="H9" s="18">
-        <v>0</v>
-      </c>
-      <c r="I9" s="15">
+      <c r="G9" s="12">
+        <v>0</v>
+      </c>
+      <c r="H9" s="17">
+        <v>0</v>
+      </c>
+      <c r="I9" s="14">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="K9" s="19">
+      <c r="K9" s="18">
         <v>1000</v>
       </c>
-      <c r="L9" s="14">
+      <c r="L9" s="13">
         <f>Meetings!B9*100</f>
         <v>250</v>
       </c>
-      <c r="M9" s="15">
+      <c r="M9" s="14">
         <f t="shared" si="3"/>
         <v>750</v>
       </c>
-      <c r="O9" s="13">
-        <v>0</v>
-      </c>
-      <c r="P9" s="14">
-        <v>0</v>
-      </c>
-      <c r="Q9" s="15">
+      <c r="O9" s="12">
+        <v>0</v>
+      </c>
+      <c r="P9" s="13">
+        <v>0</v>
+      </c>
+      <c r="Q9" s="14">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B10" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="C10" s="20">
+    <row r="10" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="B10" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="C10" s="19">
         <f>SUM(C4:C9)</f>
         <v>8100</v>
       </c>
-      <c r="D10" s="21">
+      <c r="D10" s="20">
         <f>SUM(D4:D9)</f>
         <v>4325</v>
       </c>
-      <c r="E10" s="22">
+      <c r="E10" s="21">
         <f>SUM(E4:E9)</f>
         <v>3775</v>
       </c>
-      <c r="G10" s="20">
+      <c r="G10" s="19">
         <f>SUM(G5:G9)</f>
         <v>0</v>
       </c>
-      <c r="H10" s="21">
+      <c r="H10" s="20">
         <f>SUM(H5:H9)</f>
         <v>0</v>
       </c>
-      <c r="I10" s="22">
+      <c r="I10" s="21">
         <f>SUM(I5:I9)</f>
         <v>0</v>
       </c>
-      <c r="K10" s="20">
+      <c r="K10" s="19">
         <f>SUM(K5:K9)</f>
         <v>5000</v>
       </c>
-      <c r="L10" s="21">
+      <c r="L10" s="20">
         <f>SUM(L5:L9)</f>
         <v>1800</v>
       </c>
-      <c r="M10" s="22">
+      <c r="M10" s="21">
         <f>SUM(M5:M9)</f>
         <v>3200</v>
       </c>
-      <c r="O10" s="23">
+      <c r="O10" s="22">
         <f>SUM(O5:O9)</f>
         <v>1600</v>
       </c>
-      <c r="P10" s="24">
+      <c r="P10" s="23">
         <f>SUM(P5:P9)</f>
         <v>1250</v>
       </c>
-      <c r="Q10" s="25">
+      <c r="Q10" s="24">
         <f>SUM(Q5:Q9)</f>
         <v>350</v>
       </c>
@@ -1285,24 +1332,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AD55"/>
   <sheetViews>
     <sheetView topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="E34" sqref="E34:F34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="29" customWidth="1"/>
-    <col min="2" max="2" width="17.5703125" customWidth="1"/>
-    <col min="3" max="3" width="15.7109375" customWidth="1"/>
-    <col min="4" max="5" width="8.5703125" customWidth="1"/>
-    <col min="6" max="6" width="10.7109375" customWidth="1"/>
-    <col min="7" max="1025" width="8.5703125" customWidth="1"/>
+    <col min="2" max="2" width="17.5546875" customWidth="1"/>
+    <col min="3" max="3" width="15.6640625" customWidth="1"/>
+    <col min="4" max="5" width="8.5546875" customWidth="1"/>
+    <col min="6" max="6" width="10.6640625" customWidth="1"/>
+    <col min="7" max="1025" width="8.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:30" x14ac:dyDescent="0.3">
       <c r="B1" t="s">
         <v>13</v>
       </c>
@@ -1312,21 +1359,21 @@
       <c r="D1" t="s">
         <v>15</v>
       </c>
-      <c r="E1" s="26"/>
+      <c r="E1" s="25"/>
       <c r="F1" t="s">
         <v>16</v>
       </c>
-      <c r="H1" s="27"/>
+      <c r="H1" s="26"/>
       <c r="I1" t="s">
         <v>17</v>
       </c>
-      <c r="K1" s="28"/>
+      <c r="K1" s="27"/>
       <c r="L1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A2" s="29" t="s">
+    <row r="2" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="A2" s="28" t="s">
         <v>7</v>
       </c>
       <c r="D2" t="s">
@@ -1411,7 +1458,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="3" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>20</v>
       </c>
@@ -1422,7 +1469,7 @@
         <v>1.36</v>
       </c>
     </row>
-    <row r="4" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>21</v>
       </c>
@@ -1433,7 +1480,7 @@
         <v>0.45</v>
       </c>
     </row>
-    <row r="5" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>22</v>
       </c>
@@ -1441,7 +1488,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>23</v>
       </c>
@@ -1452,7 +1499,7 @@
         <v>3.52</v>
       </c>
     </row>
-    <row r="10" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>24</v>
       </c>
@@ -1465,12 +1512,12 @@
         <v>6.33</v>
       </c>
     </row>
-    <row r="11" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A11" s="30" t="s">
+    <row r="11" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="A11" s="29" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>24</v>
       </c>
@@ -1483,15 +1530,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" s="30" t="s">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A21" s="29" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="E22" s="31"/>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E22" s="30"/>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>24</v>
       </c>
@@ -1504,12 +1551,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A29" s="30" t="s">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A29" s="29" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>20</v>
       </c>
@@ -1519,9 +1566,9 @@
       <c r="C30">
         <v>2</v>
       </c>
-      <c r="E30" s="47"/>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E30" s="44"/>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>21</v>
       </c>
@@ -1531,39 +1578,39 @@
       <c r="C31">
         <v>2</v>
       </c>
-      <c r="E31" s="47"/>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E31" s="44"/>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>46</v>
       </c>
       <c r="B32">
         <v>6</v>
       </c>
-      <c r="E32" s="48"/>
-      <c r="F32" s="48"/>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E32" s="45"/>
+      <c r="F32" s="45"/>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>47</v>
       </c>
       <c r="B33">
         <v>5</v>
       </c>
-      <c r="E33" s="48"/>
-      <c r="F33" s="48"/>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E33" s="45"/>
+      <c r="F33" s="45"/>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>48</v>
       </c>
       <c r="B34">
         <v>6</v>
       </c>
-      <c r="E34" s="48"/>
-      <c r="F34" s="48"/>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E34" s="45"/>
+      <c r="F34" s="45"/>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>24</v>
       </c>
@@ -1576,12 +1623,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A37" s="30" t="s">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A37" s="29" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>25</v>
       </c>
@@ -1591,9 +1638,9 @@
       <c r="C38">
         <v>0</v>
       </c>
-      <c r="E38" s="28"/>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E38" s="27"/>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>26</v>
       </c>
@@ -1603,10 +1650,10 @@
       <c r="C39">
         <v>0</v>
       </c>
-      <c r="E39" s="28"/>
-      <c r="F39" s="28"/>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E39" s="27"/>
+      <c r="F39" s="27"/>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>27</v>
       </c>
@@ -1616,10 +1663,10 @@
       <c r="C40">
         <v>0</v>
       </c>
-      <c r="E40" s="28"/>
-      <c r="F40" s="28"/>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E40" s="27"/>
+      <c r="F40" s="27"/>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>24</v>
       </c>
@@ -1632,12 +1679,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A46" s="30" t="s">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A46" s="29" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>20</v>
       </c>
@@ -1647,9 +1694,9 @@
       <c r="C47">
         <v>1</v>
       </c>
-      <c r="E47" s="26"/>
-    </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E47" s="25"/>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>21</v>
       </c>
@@ -1659,9 +1706,9 @@
       <c r="C48">
         <v>1</v>
       </c>
-      <c r="E48" s="26"/>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E48" s="25"/>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>24</v>
       </c>
@@ -1674,7 +1721,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>28</v>
       </c>
@@ -1687,15 +1734,15 @@
         <v>12.33</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>29</v>
       </c>
-      <c r="B55" s="32">
+      <c r="B55" s="31">
         <f>B54*100</f>
         <v>4000</v>
       </c>
-      <c r="C55" s="32">
+      <c r="C55" s="31">
         <f>C54*100</f>
         <v>1233</v>
       </c>
@@ -1707,331 +1754,331 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:L12"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1025" width="8.5703125" customWidth="1"/>
+    <col min="1" max="1025" width="8.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B1" s="33" t="s">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="B1" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="C1" s="34">
+      <c r="C1" s="32">
         <v>43489</v>
       </c>
-      <c r="D1" s="34">
+      <c r="D1" s="32">
         <v>43494</v>
       </c>
-      <c r="E1" s="34">
+      <c r="E1" s="32">
         <v>43496</v>
       </c>
-      <c r="F1" s="34">
+      <c r="F1" s="32">
         <v>43497</v>
       </c>
-      <c r="G1" s="35">
+      <c r="G1" s="33">
         <v>43502</v>
       </c>
-      <c r="H1" s="33" t="s">
+      <c r="H1" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="I1" s="33" t="s">
+      <c r="I1" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="J1" s="33" t="s">
+      <c r="J1" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="K1" s="33" t="s">
+      <c r="K1" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="L1" s="33" t="s">
+      <c r="L1" s="3" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="62.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="33" t="s">
+    <row r="2" spans="1:12" ht="62.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B2" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="C2" s="36" t="s">
+      <c r="C2" s="34" t="s">
         <v>33</v>
       </c>
-      <c r="D2" s="36" t="s">
+      <c r="D2" s="34" t="s">
         <v>34</v>
       </c>
-      <c r="E2" s="36" t="s">
+      <c r="E2" s="34" t="s">
         <v>34</v>
       </c>
-      <c r="F2" s="36" t="s">
+      <c r="F2" s="34" t="s">
         <v>34</v>
       </c>
-      <c r="G2" s="36" t="s">
+      <c r="G2" s="34" t="s">
         <v>31</v>
       </c>
-      <c r="H2" s="36" t="s">
+      <c r="H2" s="34" t="s">
         <v>31</v>
       </c>
-      <c r="I2" s="36" t="s">
+      <c r="I2" s="34" t="s">
         <v>31</v>
       </c>
-      <c r="J2" s="36" t="s">
+      <c r="J2" s="34" t="s">
         <v>31</v>
       </c>
-      <c r="K2" s="36" t="s">
+      <c r="K2" s="34" t="s">
         <v>31</v>
       </c>
-      <c r="L2" s="36" t="s">
+      <c r="L2" s="34" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B3" s="33" t="s">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="B3" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="C3" s="33">
+      <c r="C3" s="3">
         <v>1.5</v>
       </c>
-      <c r="D3" s="33">
+      <c r="D3" s="3">
         <v>0.5</v>
       </c>
-      <c r="E3" s="33">
+      <c r="E3" s="3">
         <v>0.5</v>
       </c>
-      <c r="F3" s="33">
+      <c r="F3" s="3">
         <v>1</v>
       </c>
-      <c r="G3" s="33">
+      <c r="G3" s="3">
         <v>0.5</v>
       </c>
-      <c r="H3" s="33">
-        <v>0</v>
-      </c>
-      <c r="I3" s="33">
-        <v>0</v>
-      </c>
-      <c r="J3" s="33">
-        <v>0</v>
-      </c>
-      <c r="K3" s="33">
-        <v>0</v>
-      </c>
-      <c r="L3" s="33">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A4" s="33" t="s">
+      <c r="H3" s="3">
+        <v>0</v>
+      </c>
+      <c r="I3" s="3">
+        <v>0</v>
+      </c>
+      <c r="J3" s="3">
+        <v>0</v>
+      </c>
+      <c r="K3" s="3">
+        <v>0</v>
+      </c>
+      <c r="L3" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A4" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="33">
+      <c r="B4" s="3">
         <f t="shared" ref="B4:B9" si="0">SUMIF(C4:L4,A$12,C$3:Z$3)</f>
         <v>4</v>
       </c>
-      <c r="C4" s="37" t="s">
-        <v>36</v>
-      </c>
-      <c r="D4" s="37" t="s">
-        <v>36</v>
-      </c>
-      <c r="E4" s="37" t="s">
-        <v>36</v>
-      </c>
-      <c r="F4" s="37" t="s">
-        <v>36</v>
-      </c>
-      <c r="G4" s="37" t="s">
-        <v>36</v>
-      </c>
-      <c r="H4" s="37"/>
-      <c r="I4" s="37"/>
-      <c r="J4" s="37"/>
-      <c r="K4" s="37"/>
-      <c r="L4" s="37"/>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A5" s="33" t="s">
+      <c r="C4" s="35" t="s">
+        <v>36</v>
+      </c>
+      <c r="D4" s="35" t="s">
+        <v>36</v>
+      </c>
+      <c r="E4" s="35" t="s">
+        <v>36</v>
+      </c>
+      <c r="F4" s="35" t="s">
+        <v>36</v>
+      </c>
+      <c r="G4" s="35" t="s">
+        <v>36</v>
+      </c>
+      <c r="H4" s="35"/>
+      <c r="I4" s="35"/>
+      <c r="J4" s="35"/>
+      <c r="K4" s="35"/>
+      <c r="L4" s="35"/>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A5" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="33">
+      <c r="B5" s="3">
         <f t="shared" si="0"/>
         <v>3.5</v>
       </c>
-      <c r="C5" s="37" t="s">
-        <v>36</v>
-      </c>
-      <c r="D5" s="37"/>
-      <c r="E5" s="37" t="s">
-        <v>36</v>
-      </c>
-      <c r="F5" s="37" t="s">
-        <v>36</v>
-      </c>
-      <c r="G5" s="37" t="s">
-        <v>36</v>
-      </c>
-      <c r="J5" s="37"/>
-      <c r="K5" s="37"/>
-      <c r="L5" s="37"/>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A6" s="33" t="s">
+      <c r="C5" s="35" t="s">
+        <v>36</v>
+      </c>
+      <c r="D5" s="35"/>
+      <c r="E5" s="35" t="s">
+        <v>36</v>
+      </c>
+      <c r="F5" s="35" t="s">
+        <v>36</v>
+      </c>
+      <c r="G5" s="35" t="s">
+        <v>36</v>
+      </c>
+      <c r="J5" s="35"/>
+      <c r="K5" s="35"/>
+      <c r="L5" s="35"/>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A6" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B6" s="33">
+      <c r="B6" s="3">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="C6" s="37" t="s">
-        <v>36</v>
-      </c>
-      <c r="D6" s="37" t="s">
-        <v>36</v>
-      </c>
-      <c r="E6" s="37" t="s">
-        <v>36</v>
-      </c>
-      <c r="F6" s="37" t="s">
-        <v>36</v>
-      </c>
-      <c r="G6" s="37" t="s">
-        <v>36</v>
-      </c>
-      <c r="H6" s="37"/>
-      <c r="I6" s="37"/>
-      <c r="J6" s="37"/>
-      <c r="K6" s="37"/>
-      <c r="L6" s="37"/>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A7" s="33" t="s">
+      <c r="C6" s="35" t="s">
+        <v>36</v>
+      </c>
+      <c r="D6" s="35" t="s">
+        <v>36</v>
+      </c>
+      <c r="E6" s="35" t="s">
+        <v>36</v>
+      </c>
+      <c r="F6" s="35" t="s">
+        <v>36</v>
+      </c>
+      <c r="G6" s="35" t="s">
+        <v>36</v>
+      </c>
+      <c r="H6" s="35"/>
+      <c r="I6" s="35"/>
+      <c r="J6" s="35"/>
+      <c r="K6" s="35"/>
+      <c r="L6" s="35"/>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A7" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B7" s="33">
+      <c r="B7" s="3">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="C7" s="37" t="s">
-        <v>36</v>
-      </c>
-      <c r="D7" s="37" t="s">
-        <v>36</v>
-      </c>
-      <c r="E7" s="37" t="s">
-        <v>36</v>
-      </c>
-      <c r="F7" s="37" t="s">
-        <v>36</v>
-      </c>
-      <c r="G7" s="37" t="s">
-        <v>36</v>
-      </c>
-      <c r="H7" s="37"/>
-      <c r="I7" s="37"/>
-      <c r="J7" s="37"/>
-      <c r="K7" s="37"/>
-      <c r="L7" s="37"/>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A8" s="33" t="s">
+      <c r="C7" s="35" t="s">
+        <v>36</v>
+      </c>
+      <c r="D7" s="35" t="s">
+        <v>36</v>
+      </c>
+      <c r="E7" s="35" t="s">
+        <v>36</v>
+      </c>
+      <c r="F7" s="35" t="s">
+        <v>36</v>
+      </c>
+      <c r="G7" s="35" t="s">
+        <v>36</v>
+      </c>
+      <c r="H7" s="35"/>
+      <c r="I7" s="35"/>
+      <c r="J7" s="35"/>
+      <c r="K7" s="35"/>
+      <c r="L7" s="35"/>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A8" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B8" s="33">
+      <c r="B8" s="3">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="C8" s="37" t="s">
-        <v>36</v>
-      </c>
-      <c r="D8" s="37" t="s">
-        <v>36</v>
-      </c>
-      <c r="E8" s="37" t="s">
-        <v>36</v>
-      </c>
-      <c r="F8" s="37" t="s">
-        <v>36</v>
-      </c>
-      <c r="G8" s="37" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A9" s="33" t="s">
+      <c r="C8" s="35" t="s">
+        <v>36</v>
+      </c>
+      <c r="D8" s="35" t="s">
+        <v>36</v>
+      </c>
+      <c r="E8" s="35" t="s">
+        <v>36</v>
+      </c>
+      <c r="F8" s="35" t="s">
+        <v>36</v>
+      </c>
+      <c r="G8" s="35" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A9" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B9" s="33">
+      <c r="B9" s="3">
         <f t="shared" si="0"/>
         <v>2.5</v>
       </c>
-      <c r="D9" s="37" t="s">
-        <v>36</v>
-      </c>
-      <c r="E9" s="37" t="s">
-        <v>36</v>
-      </c>
-      <c r="F9" s="37" t="s">
-        <v>36</v>
-      </c>
-      <c r="G9" s="37" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A10" s="33" t="s">
-        <v>0</v>
-      </c>
-      <c r="B10" s="33">
+      <c r="D9" s="35" t="s">
+        <v>36</v>
+      </c>
+      <c r="E9" s="35" t="s">
+        <v>36</v>
+      </c>
+      <c r="F9" s="35" t="s">
+        <v>36</v>
+      </c>
+      <c r="G9" s="35" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A10" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B10" s="3">
         <f>SUM(B4:B7)</f>
         <v>15.5</v>
       </c>
-      <c r="C10" s="33">
+      <c r="C10" s="3">
         <f t="shared" ref="C10:L10" si="1">COUNTIF(C4:C7,"*ü*") * C3</f>
         <v>6</v>
       </c>
-      <c r="D10" s="33">
+      <c r="D10" s="3">
         <f t="shared" si="1"/>
         <v>1.5</v>
       </c>
-      <c r="E10" s="33">
+      <c r="E10" s="3">
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
-      <c r="F10" s="33">
+      <c r="F10" s="3">
         <f t="shared" si="1"/>
         <v>4</v>
       </c>
-      <c r="G10" s="33">
+      <c r="G10" s="3">
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
-      <c r="H10" s="33">
+      <c r="H10" s="3">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="I10" s="33">
+      <c r="I10" s="3">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="J10" s="33">
+      <c r="J10" s="3">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="K10" s="33">
+      <c r="K10" s="3">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="L10" s="33">
+      <c r="L10" s="3">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A12" s="37" t="s">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A12" s="35" t="s">
         <v>36</v>
       </c>
     </row>
@@ -2042,32 +2089,32 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:S34"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B32" sqref="B32"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E35" sqref="E35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="15" customWidth="1"/>
-    <col min="2" max="2" width="29.7109375" customWidth="1"/>
-    <col min="3" max="3" width="14.42578125" customWidth="1"/>
-    <col min="4" max="4" width="10.42578125" customWidth="1"/>
-    <col min="5" max="19" width="3.7109375" customWidth="1"/>
-    <col min="20" max="1025" width="8.5703125" customWidth="1"/>
+    <col min="2" max="2" width="29.6640625" customWidth="1"/>
+    <col min="3" max="3" width="14.44140625" customWidth="1"/>
+    <col min="4" max="4" width="10.44140625" customWidth="1"/>
+    <col min="5" max="19" width="3.6640625" customWidth="1"/>
+    <col min="20" max="1025" width="8.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A1" s="38"/>
-      <c r="B1" s="39" t="s">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A1" s="36"/>
+      <c r="B1" s="37" t="s">
         <v>37</v>
       </c>
-      <c r="C1" s="39" t="s">
+      <c r="C1" s="37" t="s">
         <v>38</v>
       </c>
-      <c r="D1" s="40" t="s">
+      <c r="D1" s="38" t="s">
         <v>39</v>
       </c>
       <c r="E1">
@@ -2116,365 +2163,377 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="C2" s="41"/>
-      <c r="D2" s="42"/>
-    </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B3" s="4" t="s">
+      <c r="D2" s="39"/>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="B3" s="3" t="s">
         <v>41</v>
       </c>
       <c r="C3">
         <v>1</v>
       </c>
-      <c r="D3" s="42">
+      <c r="D3" s="39">
         <v>0.75</v>
       </c>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B4" s="4" t="s">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="B4" s="3" t="s">
         <v>42</v>
       </c>
       <c r="C4">
         <v>3</v>
       </c>
-      <c r="D4" s="42">
+      <c r="D4" s="39">
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B5" s="4" t="s">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="B5" s="3" t="s">
         <v>43</v>
       </c>
       <c r="C5">
         <v>1</v>
       </c>
-      <c r="D5" s="42">
+      <c r="D5" s="39">
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A6" s="43"/>
-      <c r="B6" s="4" t="s">
+    <row r="6" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A6" s="40"/>
+      <c r="B6" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="C6" s="4">
+      <c r="C6" s="3">
         <f>SUM(C2:C5)</f>
         <v>5</v>
       </c>
-      <c r="D6" s="5">
+      <c r="D6" s="4">
         <f>SUM(D2:D5)</f>
         <v>8.75</v>
       </c>
     </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A7" s="3" t="s">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A7" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="4" t="s">
+      <c r="B7" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="C7" s="41"/>
-      <c r="D7" s="42"/>
-    </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B8" s="4" t="s">
+      <c r="D7" s="39"/>
+    </row>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="B8" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="D8" s="42"/>
-    </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B9" s="4" t="s">
+      <c r="D8" s="39"/>
+    </row>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="B9" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="D9" s="42"/>
-    </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B10" s="4" t="s">
+      <c r="D9" s="39"/>
+    </row>
+    <row r="10" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="B10" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="D10" s="42"/>
-    </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A11" s="43"/>
-      <c r="B11" s="4" t="s">
+      <c r="D10" s="39"/>
+    </row>
+    <row r="11" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A11" s="40"/>
+      <c r="B11" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="C11" s="4">
+      <c r="C11" s="3">
         <f>SUM(C7:C10)</f>
         <v>0</v>
       </c>
-      <c r="D11" s="5">
+      <c r="D11" s="4">
         <f>SUM(D7:D10)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A12" s="3" t="s">
+    <row r="12" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A12" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B12" s="4" t="s">
+      <c r="B12" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="C12" s="41"/>
-      <c r="D12" s="42"/>
-    </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B13" s="4" t="s">
+      <c r="D12" s="39"/>
+    </row>
+    <row r="13" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="B13" s="3" t="s">
         <v>45</v>
       </c>
       <c r="C13">
         <v>2</v>
       </c>
-      <c r="D13" s="42">
+      <c r="D13" s="39">
         <v>1.5</v>
       </c>
     </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B14" s="4" t="s">
+    <row r="14" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="B14" s="3" t="s">
         <v>42</v>
       </c>
       <c r="C14">
         <v>4</v>
       </c>
-      <c r="D14" s="42">
+      <c r="D14" s="39">
         <v>3</v>
       </c>
     </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B15" s="4" t="s">
+    <row r="15" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="B15" s="3" t="s">
         <v>43</v>
       </c>
       <c r="C15">
         <v>2</v>
       </c>
-      <c r="D15" s="42">
+      <c r="D15" s="39">
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B16" s="4" t="s">
+    <row r="16" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="B16" s="3" t="s">
         <v>20</v>
       </c>
       <c r="C16">
         <v>1</v>
       </c>
-      <c r="D16" s="42">
+      <c r="D16" s="39">
         <v>0.75</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B17" s="4" t="s">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B17" s="3" t="s">
         <v>21</v>
       </c>
       <c r="C17">
         <v>1</v>
       </c>
-      <c r="D17" s="42">
+      <c r="D17" s="39">
         <v>0.25</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A18" s="43"/>
-      <c r="B18" s="44" t="s">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A18" s="40"/>
+      <c r="B18" s="41" t="s">
         <v>44</v>
       </c>
-      <c r="C18" s="4">
+      <c r="C18" s="3">
         <f>SUM(C12:C17)</f>
         <v>10</v>
       </c>
-      <c r="D18" s="5">
+      <c r="D18" s="4">
         <f>SUM(D12:D17)</f>
         <v>6.5</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A19" s="3" t="s">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A19" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B19" s="4" t="s">
+      <c r="B19" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="C19" s="41">
+      <c r="C19">
         <v>1</v>
       </c>
-      <c r="D19" s="42">
+      <c r="D19" s="39">
         <v>1</v>
       </c>
-      <c r="E19" s="47"/>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B20" s="4" t="s">
+      <c r="E19" s="44"/>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B20" s="3" t="s">
         <v>45</v>
       </c>
       <c r="C20">
         <v>3</v>
       </c>
-      <c r="D20" s="42">
+      <c r="D20" s="39">
         <v>3</v>
       </c>
-      <c r="E20" s="47"/>
-      <c r="F20" s="47"/>
-      <c r="G20" s="47"/>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B21" s="4" t="s">
+      <c r="E20" s="44"/>
+      <c r="F20" s="44"/>
+      <c r="G20" s="44"/>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B21" s="3" t="s">
         <v>42</v>
       </c>
       <c r="C21">
         <v>6</v>
       </c>
-      <c r="D21" s="42">
+      <c r="D21" s="39">
         <v>7</v>
       </c>
-      <c r="E21" s="47"/>
-      <c r="F21" s="47"/>
-      <c r="G21" s="47"/>
-      <c r="H21" s="47"/>
-      <c r="I21" s="47"/>
-      <c r="J21" s="47"/>
-      <c r="K21" s="47"/>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B22" s="4" t="s">
+      <c r="E21" s="44"/>
+      <c r="F21" s="44"/>
+      <c r="G21" s="44"/>
+      <c r="H21" s="44"/>
+      <c r="I21" s="44"/>
+      <c r="J21" s="44"/>
+      <c r="K21" s="44"/>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B22" s="3" t="s">
         <v>43</v>
       </c>
       <c r="C22">
         <v>1</v>
       </c>
-      <c r="D22" s="42">
+      <c r="D22" s="39">
         <v>2</v>
       </c>
-      <c r="E22" s="47"/>
-      <c r="F22" s="47"/>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A23" s="43"/>
-      <c r="B23" s="44" t="s">
+      <c r="E22" s="44"/>
+      <c r="F22" s="44"/>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A23" s="40"/>
+      <c r="B23" s="41" t="s">
         <v>44</v>
       </c>
-      <c r="C23" s="4">
+      <c r="C23" s="3">
         <f>SUM(C19:C22)</f>
         <v>11</v>
       </c>
-      <c r="D23" s="5">
+      <c r="D23" s="4">
         <f>SUM(D19:D22)</f>
         <v>13</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A24" s="3" t="s">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A24" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B24" s="4" t="s">
+      <c r="B24" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="D24" s="42"/>
-    </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B25" s="4" t="s">
+      <c r="D24" s="39"/>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B25" s="3" t="s">
         <v>45</v>
       </c>
       <c r="C25">
         <v>1.5</v>
       </c>
-      <c r="D25" s="42">
+      <c r="D25" s="39">
         <v>1.5</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B26" s="4" t="s">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B26" s="3" t="s">
         <v>42</v>
       </c>
       <c r="C26">
         <v>3</v>
       </c>
-      <c r="D26" s="42">
+      <c r="D26" s="39">
         <v>3</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B27" s="4" t="s">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B27" s="3" t="s">
         <v>43</v>
       </c>
       <c r="C27">
         <v>1.5</v>
       </c>
-      <c r="D27" s="42">
+      <c r="D27" s="39">
         <v>1.5</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B28" s="44" t="s">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B28" s="41" t="s">
         <v>44</v>
       </c>
-      <c r="C28" s="4">
+      <c r="C28" s="3">
         <f>SUM(C24:C27)</f>
         <v>6</v>
       </c>
-      <c r="D28" s="5">
+      <c r="D28" s="4">
         <f>SUM(D24:D27)</f>
         <v>6</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A29" s="3" t="s">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A29" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B29" s="4" t="s">
+      <c r="B29" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="D29" s="42"/>
-    </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B30" s="4" t="s">
+      <c r="D29" s="39"/>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B30" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="D30" s="42"/>
-    </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B31" s="4" t="s">
+      <c r="C30">
+        <v>1</v>
+      </c>
+      <c r="D30" s="39">
+        <v>1</v>
+      </c>
+      <c r="E30" s="44"/>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B31" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="D31" s="42"/>
-    </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B32" s="4" t="s">
+      <c r="C31">
+        <v>2</v>
+      </c>
+      <c r="D31" s="39">
+        <v>1</v>
+      </c>
+      <c r="E31" s="44"/>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B32" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="D32" s="42"/>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B33" s="44" t="s">
+      <c r="C32">
+        <v>2</v>
+      </c>
+      <c r="D32" s="39"/>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B33" s="41" t="s">
         <v>44</v>
       </c>
-      <c r="C33" s="4">
+      <c r="C33" s="3">
         <f>SUM(C29:C32)</f>
-        <v>0</v>
-      </c>
-      <c r="D33" s="5">
+        <v>5</v>
+      </c>
+      <c r="D33" s="4">
         <f>SUM(D29:D32)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A34" s="45"/>
-      <c r="B34" s="46" t="s">
-        <v>0</v>
-      </c>
-      <c r="C34" s="7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A34" s="42"/>
+      <c r="B34" s="43" t="s">
+        <v>0</v>
+      </c>
+      <c r="C34" s="6">
         <f>SUM(C6,C11,C18,C23,C28,C33)</f>
-        <v>32</v>
-      </c>
-      <c r="D34" s="8">
+        <v>37</v>
+      </c>
+      <c r="D34" s="7">
         <f>SUM(D6,D11,D18,D23,D28,D33)</f>
-        <v>34.25</v>
+        <v>36.25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update Gantt Chart & Add Progress
</commit_message>
<xml_diff>
--- a/docs/ganttChart.xlsx
+++ b/docs/ganttChart.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11015"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\cs383 banana\banana\docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/blakelyfrechette/Desktop/banana/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B617824-3146-4047-985D-158131FC59C9}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CBFE3E4-7336-F54A-BF20-85981F78E2F4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="28065" windowHeight="16440" tabRatio="500" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" tabRatio="500" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Management Summary" sheetId="1" r:id="rId1"/>
@@ -18,14 +18,8 @@
     <sheet name="Meetings" sheetId="3" r:id="rId3"/>
     <sheet name="SA" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="179021"/>
   <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-      </xcalcf:calcFeatures>
-    </ext>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
     </ext>
@@ -34,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="61">
   <si>
     <t>Total</t>
   </si>
@@ -114,12 +108,6 @@
     <t>Import sounds in assets folder</t>
   </si>
   <si>
-    <t>Script classes for sound</t>
-  </si>
-  <si>
-    <t>Test cases</t>
-  </si>
-  <si>
     <t>group totals (hrs)</t>
   </si>
   <si>
@@ -205,6 +193,24 @@
   </si>
   <si>
     <t>Release Build</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Class Diagram </t>
+  </si>
+  <si>
+    <t>Create Sound Class</t>
+  </si>
+  <si>
+    <t>Haptic Response</t>
+  </si>
+  <si>
+    <t>Player Sound effects</t>
+  </si>
+  <si>
+    <t>Coding Standards</t>
+  </si>
+  <si>
+    <t>RFP (3.0 - 5.0)</t>
   </si>
 </sst>
 </file>
@@ -237,7 +243,7 @@
       <charset val="2"/>
     </font>
   </fonts>
-  <fills count="11">
+  <fills count="13">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -296,6 +302,18 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF000000"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
   </fills>
@@ -452,7 +470,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="48">
+  <cellXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -507,6 +525,9 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -919,28 +940,28 @@
       <selection activeCell="L7" sqref="L7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="2" width="8.5703125" customWidth="1"/>
-    <col min="3" max="3" width="14.140625" customWidth="1"/>
-    <col min="4" max="4" width="13.85546875" customWidth="1"/>
-    <col min="5" max="5" width="13.28515625" customWidth="1"/>
-    <col min="6" max="6" width="3.42578125" customWidth="1"/>
-    <col min="7" max="7" width="15.28515625" customWidth="1"/>
-    <col min="8" max="8" width="12.28515625" customWidth="1"/>
-    <col min="9" max="9" width="14.42578125" customWidth="1"/>
-    <col min="10" max="10" width="2.85546875" customWidth="1"/>
-    <col min="11" max="11" width="13.85546875" customWidth="1"/>
+    <col min="1" max="2" width="8.5" customWidth="1"/>
+    <col min="3" max="3" width="14.1640625" customWidth="1"/>
+    <col min="4" max="4" width="13.83203125" customWidth="1"/>
+    <col min="5" max="5" width="13.33203125" customWidth="1"/>
+    <col min="6" max="6" width="3.5" customWidth="1"/>
+    <col min="7" max="7" width="15.33203125" customWidth="1"/>
+    <col min="8" max="8" width="12.33203125" customWidth="1"/>
+    <col min="9" max="9" width="14.5" customWidth="1"/>
+    <col min="10" max="10" width="2.83203125" customWidth="1"/>
+    <col min="11" max="11" width="13.83203125" customWidth="1"/>
     <col min="12" max="12" width="14" customWidth="1"/>
-    <col min="13" max="13" width="14.140625" customWidth="1"/>
-    <col min="14" max="14" width="5.42578125" customWidth="1"/>
-    <col min="15" max="15" width="12.28515625" customWidth="1"/>
-    <col min="16" max="16" width="14.7109375" customWidth="1"/>
-    <col min="17" max="17" width="11.28515625" customWidth="1"/>
-    <col min="18" max="1025" width="8.5703125" customWidth="1"/>
+    <col min="13" max="13" width="14.1640625" customWidth="1"/>
+    <col min="14" max="14" width="5.5" customWidth="1"/>
+    <col min="15" max="15" width="12.33203125" customWidth="1"/>
+    <col min="16" max="16" width="14.6640625" customWidth="1"/>
+    <col min="17" max="17" width="11.33203125" customWidth="1"/>
+    <col min="18" max="1025" width="8.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:17" x14ac:dyDescent="0.2">
       <c r="C2" s="47" t="s">
         <v>0</v>
       </c>
@@ -963,7 +984,7 @@
       <c r="P2" s="47"/>
       <c r="Q2" s="47"/>
     </row>
-    <row r="3" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:17" x14ac:dyDescent="0.2">
       <c r="C3" s="2" t="s">
         <v>4</v>
       </c>
@@ -1001,7 +1022,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B4" s="8" t="s">
         <v>7</v>
       </c>
@@ -1051,7 +1072,7 @@
         <v>-375</v>
       </c>
     </row>
-    <row r="5" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B5" s="2" t="s">
         <v>8</v>
       </c>
@@ -1101,7 +1122,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B6" s="2" t="s">
         <v>9</v>
       </c>
@@ -1151,7 +1172,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="7" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B7" s="2" t="s">
         <v>10</v>
       </c>
@@ -1201,7 +1222,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B8" s="15" t="s">
         <v>11</v>
       </c>
@@ -1249,7 +1270,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B9" s="15" t="s">
         <v>12</v>
       </c>
@@ -1297,7 +1318,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B10" s="5" t="s">
         <v>0</v>
       </c>
@@ -1364,23 +1385,23 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:AD57"/>
+  <dimension ref="A1:AD62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="P20" sqref="P20"/>
+    <sheetView tabSelected="1" topLeftCell="A12" zoomScale="83" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H49" sqref="H49"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="29" customWidth="1"/>
-    <col min="2" max="2" width="17.5703125" customWidth="1"/>
-    <col min="3" max="3" width="15.7109375" customWidth="1"/>
-    <col min="4" max="5" width="8.5703125" customWidth="1"/>
-    <col min="6" max="6" width="10.7109375" customWidth="1"/>
-    <col min="7" max="1025" width="8.5703125" customWidth="1"/>
+    <col min="2" max="2" width="17.5" customWidth="1"/>
+    <col min="3" max="3" width="15.6640625" customWidth="1"/>
+    <col min="4" max="5" width="8.5" customWidth="1"/>
+    <col min="6" max="6" width="10.6640625" customWidth="1"/>
+    <col min="7" max="1025" width="8.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:30" x14ac:dyDescent="0.2">
       <c r="B1" t="s">
         <v>13</v>
       </c>
@@ -1403,7 +1424,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A2" s="28" t="s">
         <v>7</v>
       </c>
@@ -1489,7 +1510,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="3" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>20</v>
       </c>
@@ -1500,7 +1521,7 @@
         <v>1.36</v>
       </c>
     </row>
-    <row r="4" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>21</v>
       </c>
@@ -1511,7 +1532,7 @@
         <v>0.45</v>
       </c>
     </row>
-    <row r="5" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>22</v>
       </c>
@@ -1519,7 +1540,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>23</v>
       </c>
@@ -1530,7 +1551,7 @@
         <v>3.52</v>
       </c>
     </row>
-    <row r="10" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>24</v>
       </c>
@@ -1543,12 +1564,12 @@
         <v>6.33</v>
       </c>
     </row>
-    <row r="11" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A11" s="29" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>24</v>
       </c>
@@ -1561,14 +1582,14 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A21" s="29" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B22">
         <v>3</v>
@@ -1578,9 +1599,9 @@
       </c>
       <c r="E22" s="30"/>
     </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B23">
         <v>3</v>
@@ -1590,9 +1611,9 @@
       </c>
       <c r="F23" s="44"/>
     </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B24">
         <v>3</v>
@@ -1602,9 +1623,9 @@
       </c>
       <c r="G24" s="44"/>
     </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B25">
         <v>3</v>
@@ -1614,9 +1635,9 @@
       </c>
       <c r="H25" s="44"/>
     </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B26">
         <v>3</v>
@@ -1626,9 +1647,9 @@
       </c>
       <c r="I26" s="46"/>
     </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B27">
         <v>9</v>
@@ -1640,9 +1661,9 @@
       <c r="K27" s="45"/>
       <c r="L27" s="45"/>
     </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B28">
         <v>6</v>
@@ -1653,9 +1674,9 @@
       <c r="M28" s="45"/>
       <c r="N28" s="45"/>
     </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B29">
         <v>3</v>
@@ -1665,7 +1686,7 @@
       </c>
       <c r="O29" s="45"/>
     </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>24</v>
       </c>
@@ -1678,12 +1699,12 @@
         <v>9</v>
       </c>
     </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A31" s="29" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>20</v>
       </c>
@@ -1695,7 +1716,7 @@
       </c>
       <c r="E32" s="44"/>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>21</v>
       </c>
@@ -1707,9 +1728,9 @@
       </c>
       <c r="E33" s="44"/>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B34">
         <v>6</v>
@@ -1717,9 +1738,9 @@
       <c r="E34" s="45"/>
       <c r="F34" s="45"/>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B35">
         <v>5</v>
@@ -1727,9 +1748,9 @@
       <c r="E35" s="45"/>
       <c r="F35" s="45"/>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B36">
         <v>6</v>
@@ -1737,7 +1758,7 @@
       <c r="E36" s="45"/>
       <c r="F36" s="45"/>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>24</v>
       </c>
@@ -1750,128 +1771,205 @@
         <v>4</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A39" s="29" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
+        <v>60</v>
+      </c>
+      <c r="B40">
+        <v>1.5</v>
+      </c>
+      <c r="C40">
+        <v>1.5</v>
+      </c>
+      <c r="E40" s="44"/>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>55</v>
+      </c>
+      <c r="B41">
+        <v>1.5</v>
+      </c>
+      <c r="C41">
+        <v>1.5</v>
+      </c>
+      <c r="E41" s="44"/>
+      <c r="F41" s="48"/>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
+        <v>21</v>
+      </c>
+      <c r="B42">
+        <v>1</v>
+      </c>
+      <c r="C42">
+        <v>1</v>
+      </c>
+      <c r="E42" s="49"/>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
         <v>25</v>
       </c>
-      <c r="B40">
+      <c r="B43">
         <v>0.5</v>
       </c>
-      <c r="C40">
-        <v>0</v>
-      </c>
-      <c r="E40" s="27"/>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
+      <c r="C43">
+        <v>0.5</v>
+      </c>
+      <c r="E43" s="49"/>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
+        <v>46</v>
+      </c>
+      <c r="B44">
+        <v>7</v>
+      </c>
+      <c r="C44">
+        <v>2.5</v>
+      </c>
+      <c r="E44" s="49"/>
+      <c r="F44" s="46"/>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A45" t="s">
+        <v>56</v>
+      </c>
+      <c r="B45">
+        <v>4</v>
+      </c>
+      <c r="C45">
+        <v>4</v>
+      </c>
+      <c r="E45" s="49"/>
+      <c r="F45" s="49"/>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A46" t="s">
+        <v>57</v>
+      </c>
+      <c r="B46">
+        <v>12</v>
+      </c>
+      <c r="C46">
+        <v>0.5</v>
+      </c>
+      <c r="E46" s="49"/>
+      <c r="F46" s="46"/>
+      <c r="G46" s="45"/>
+      <c r="H46" s="50"/>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A47" t="s">
+        <v>58</v>
+      </c>
+      <c r="B47">
+        <v>4</v>
+      </c>
+      <c r="C47">
+        <v>1</v>
+      </c>
+      <c r="E47" s="49"/>
+      <c r="F47" s="45"/>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A48" t="s">
+        <v>59</v>
+      </c>
+      <c r="B48">
+        <v>1.5</v>
+      </c>
+      <c r="C48">
+        <v>0.25</v>
+      </c>
+      <c r="E48" s="46"/>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A52" t="s">
+        <v>24</v>
+      </c>
+      <c r="B52">
+        <f>SUM(B40:B51)</f>
+        <v>33</v>
+      </c>
+      <c r="C52">
+        <f>SUM(C40:C51)</f>
+        <v>12.75</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A53" s="29" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A54" t="s">
+        <v>20</v>
+      </c>
+      <c r="B54">
+        <v>1</v>
+      </c>
+      <c r="C54">
+        <v>1</v>
+      </c>
+      <c r="E54" s="25"/>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A55" t="s">
+        <v>21</v>
+      </c>
+      <c r="B55">
+        <v>1</v>
+      </c>
+      <c r="C55">
+        <v>1</v>
+      </c>
+      <c r="E55" s="25"/>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A60" t="s">
+        <v>24</v>
+      </c>
+      <c r="B60">
+        <f>SUM(B54:B59)</f>
+        <v>2</v>
+      </c>
+      <c r="C60">
+        <f>SUM(C54:C59)</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A61" t="s">
         <v>26</v>
       </c>
-      <c r="B41">
-        <v>6</v>
-      </c>
-      <c r="C41">
-        <v>0</v>
-      </c>
-      <c r="E41" s="27"/>
-      <c r="F41" s="27"/>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
+      <c r="B61">
+        <f>SUM(B30,B38,B20,B10,B52,B60)</f>
+        <v>93.5</v>
+      </c>
+      <c r="C61">
+        <f>SUM(C10,C20,C30,C38,C52,C60)</f>
+        <v>34.08</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A62" t="s">
         <v>27</v>
       </c>
-      <c r="B42">
-        <v>6</v>
-      </c>
-      <c r="C42">
-        <v>0</v>
-      </c>
-      <c r="E42" s="27"/>
-      <c r="F42" s="27"/>
-    </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A47" t="s">
-        <v>24</v>
-      </c>
-      <c r="B47">
-        <f>SUM(B40:B46)</f>
-        <v>12.5</v>
-      </c>
-      <c r="C47">
-        <f>SUM(C40:C46)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A48" s="29" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A49" t="s">
-        <v>20</v>
-      </c>
-      <c r="B49">
-        <v>1</v>
-      </c>
-      <c r="C49">
-        <v>1</v>
-      </c>
-      <c r="E49" s="25"/>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A50" t="s">
-        <v>21</v>
-      </c>
-      <c r="B50">
-        <v>1</v>
-      </c>
-      <c r="C50">
-        <v>1</v>
-      </c>
-      <c r="E50" s="25"/>
-    </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A55" t="s">
-        <v>24</v>
-      </c>
-      <c r="B55">
-        <f>SUM(B49:B54)</f>
-        <v>2</v>
-      </c>
-      <c r="C55">
-        <f>SUM(C49:C54)</f>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A56" t="s">
-        <v>28</v>
-      </c>
-      <c r="B56">
-        <f>SUM(B30,B38,B20,B10,B47,B55)</f>
-        <v>73</v>
-      </c>
-      <c r="C56">
-        <f>SUM(C10,C20,C30,C38,C47,C55)</f>
-        <v>21.33</v>
-      </c>
-    </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A57" t="s">
-        <v>29</v>
-      </c>
-      <c r="B57" s="31">
-        <f>B56*100</f>
-        <v>7300</v>
-      </c>
-      <c r="C57" s="31">
-        <f>C56*100</f>
-        <v>2133</v>
+      <c r="B62" s="31">
+        <f>B61*100</f>
+        <v>9350</v>
+      </c>
+      <c r="C62" s="31">
+        <f>C61*100</f>
+        <v>3408</v>
       </c>
     </row>
   </sheetData>
@@ -1888,14 +1986,14 @@
       <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1025" width="8.5703125" customWidth="1"/>
+    <col min="1" max="1025" width="8.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B1" s="3" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C1" s="32">
         <v>43489</v>
@@ -1913,59 +2011,59 @@
         <v>43502</v>
       </c>
       <c r="H1" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="L1" s="3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" ht="62.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B2" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C2" s="34" t="s">
         <v>31</v>
       </c>
-      <c r="I1" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="J1" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="K1" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="L1" s="3" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" ht="62.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="3" t="s">
+      <c r="D2" s="34" t="s">
         <v>32</v>
       </c>
-      <c r="C2" s="34" t="s">
+      <c r="E2" s="34" t="s">
+        <v>32</v>
+      </c>
+      <c r="F2" s="34" t="s">
+        <v>32</v>
+      </c>
+      <c r="G2" s="34" t="s">
+        <v>29</v>
+      </c>
+      <c r="H2" s="34" t="s">
+        <v>29</v>
+      </c>
+      <c r="I2" s="34" t="s">
+        <v>29</v>
+      </c>
+      <c r="J2" s="34" t="s">
+        <v>29</v>
+      </c>
+      <c r="K2" s="34" t="s">
+        <v>29</v>
+      </c>
+      <c r="L2" s="34" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="B3" s="3" t="s">
         <v>33</v>
-      </c>
-      <c r="D2" s="34" t="s">
-        <v>34</v>
-      </c>
-      <c r="E2" s="34" t="s">
-        <v>34</v>
-      </c>
-      <c r="F2" s="34" t="s">
-        <v>34</v>
-      </c>
-      <c r="G2" s="34" t="s">
-        <v>31</v>
-      </c>
-      <c r="H2" s="34" t="s">
-        <v>31</v>
-      </c>
-      <c r="I2" s="34" t="s">
-        <v>31</v>
-      </c>
-      <c r="J2" s="34" t="s">
-        <v>31</v>
-      </c>
-      <c r="K2" s="34" t="s">
-        <v>31</v>
-      </c>
-      <c r="L2" s="34" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B3" s="3" t="s">
-        <v>35</v>
       </c>
       <c r="C3" s="3">
         <v>1.5</v>
@@ -1998,7 +2096,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
         <v>7</v>
       </c>
@@ -2007,19 +2105,19 @@
         <v>4</v>
       </c>
       <c r="C4" s="35" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D4" s="35" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="E4" s="35" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="F4" s="35" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="G4" s="35" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="H4" s="35"/>
       <c r="I4" s="35"/>
@@ -2027,7 +2125,7 @@
       <c r="K4" s="35"/>
       <c r="L4" s="35"/>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
         <v>8</v>
       </c>
@@ -2036,23 +2134,23 @@
         <v>3.5</v>
       </c>
       <c r="C5" s="35" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D5" s="35"/>
       <c r="E5" s="35" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="F5" s="35" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="G5" s="35" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="J5" s="35"/>
       <c r="K5" s="35"/>
       <c r="L5" s="35"/>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
         <v>9</v>
       </c>
@@ -2061,19 +2159,19 @@
         <v>4</v>
       </c>
       <c r="C6" s="35" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D6" s="35" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="E6" s="35" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="F6" s="35" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="G6" s="35" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="H6" s="35"/>
       <c r="I6" s="35"/>
@@ -2081,7 +2179,7 @@
       <c r="K6" s="35"/>
       <c r="L6" s="35"/>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
         <v>10</v>
       </c>
@@ -2090,19 +2188,19 @@
         <v>4</v>
       </c>
       <c r="C7" s="35" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D7" s="35" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="E7" s="35" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="F7" s="35" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="G7" s="35" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="H7" s="35"/>
       <c r="I7" s="35"/>
@@ -2110,7 +2208,7 @@
       <c r="K7" s="35"/>
       <c r="L7" s="35"/>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
         <v>11</v>
       </c>
@@ -2119,22 +2217,22 @@
         <v>4</v>
       </c>
       <c r="C8" s="35" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D8" s="35" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="E8" s="35" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="F8" s="35" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="G8" s="35" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
         <v>12</v>
       </c>
@@ -2143,19 +2241,19 @@
         <v>2.5</v>
       </c>
       <c r="D9" s="35" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="E9" s="35" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="F9" s="35" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="G9" s="35" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
         <v>0</v>
       </c>
@@ -2204,9 +2302,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A12" s="35" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
   </sheetData>
@@ -2223,26 +2321,26 @@
       <selection activeCell="M29" sqref="M29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="15" customWidth="1"/>
-    <col min="2" max="2" width="29.7109375" customWidth="1"/>
-    <col min="3" max="3" width="14.42578125" customWidth="1"/>
-    <col min="4" max="4" width="10.42578125" customWidth="1"/>
-    <col min="5" max="19" width="3.7109375" customWidth="1"/>
-    <col min="20" max="1025" width="8.5703125" customWidth="1"/>
+    <col min="2" max="2" width="29.6640625" customWidth="1"/>
+    <col min="3" max="3" width="14.5" customWidth="1"/>
+    <col min="4" max="4" width="10.5" customWidth="1"/>
+    <col min="5" max="19" width="3.6640625" customWidth="1"/>
+    <col min="20" max="1025" width="8.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A1" s="36"/>
       <c r="B1" s="37" t="s">
+        <v>35</v>
+      </c>
+      <c r="C1" s="37" t="s">
+        <v>36</v>
+      </c>
+      <c r="D1" s="38" t="s">
         <v>37</v>
-      </c>
-      <c r="C1" s="37" t="s">
-        <v>38</v>
-      </c>
-      <c r="D1" s="38" t="s">
-        <v>39</v>
       </c>
       <c r="E1">
         <v>1</v>
@@ -2290,18 +2388,18 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D2" s="39"/>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.2">
       <c r="B3" s="3" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C3">
         <v>1</v>
@@ -2310,9 +2408,9 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.2">
       <c r="B4" s="3" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C4">
         <v>3</v>
@@ -2321,9 +2419,9 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.2">
       <c r="B5" s="3" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C5">
         <v>1</v>
@@ -2332,10 +2430,10 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A6" s="40"/>
       <c r="B6" s="3" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C6" s="3">
         <f>SUM(C2:C5)</f>
@@ -2346,37 +2444,37 @@
         <v>8.75</v>
       </c>
     </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
         <v>8</v>
       </c>
       <c r="B7" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="D7" s="39"/>
+    </row>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="B8" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="D8" s="39"/>
+    </row>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="B9" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="D7" s="39"/>
-    </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B8" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="D8" s="39"/>
-    </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B9" s="3" t="s">
-        <v>42</v>
-      </c>
       <c r="D9" s="39"/>
     </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:19" x14ac:dyDescent="0.2">
       <c r="B10" s="3" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D10" s="39"/>
     </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A11" s="40"/>
       <c r="B11" s="3" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C11" s="3">
         <f>SUM(C7:C10)</f>
@@ -2387,18 +2485,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
         <v>9</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D12" s="39"/>
     </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:19" x14ac:dyDescent="0.2">
       <c r="B13" s="3" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C13">
         <v>2</v>
@@ -2409,9 +2507,9 @@
       <c r="E13" s="44"/>
       <c r="F13" s="44"/>
     </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:19" x14ac:dyDescent="0.2">
       <c r="B14" s="3" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C14">
         <v>4</v>
@@ -2424,9 +2522,9 @@
       <c r="I14" s="44"/>
       <c r="J14" s="44"/>
     </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:19" x14ac:dyDescent="0.2">
       <c r="B15" s="3" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C15">
         <v>2</v>
@@ -2437,7 +2535,7 @@
       <c r="J15" s="44"/>
       <c r="K15" s="44"/>
     </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:19" x14ac:dyDescent="0.2">
       <c r="B16" s="3" t="s">
         <v>20</v>
       </c>
@@ -2449,7 +2547,7 @@
       </c>
       <c r="K16" s="44"/>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B17" s="3" t="s">
         <v>21</v>
       </c>
@@ -2461,10 +2559,10 @@
       </c>
       <c r="L17" s="44"/>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A18" s="40"/>
       <c r="B18" s="41" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C18" s="3">
         <f>SUM(C12:C17)</f>
@@ -2475,12 +2573,12 @@
         <v>6.5</v>
       </c>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
         <v>10</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C19">
         <v>1</v>
@@ -2490,9 +2588,9 @@
       </c>
       <c r="E19" s="44"/>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B20" s="3" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C20">
         <v>3</v>
@@ -2504,9 +2602,9 @@
       <c r="F20" s="44"/>
       <c r="G20" s="44"/>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B21" s="3" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C21">
         <v>6</v>
@@ -2522,9 +2620,9 @@
       <c r="J21" s="44"/>
       <c r="K21" s="44"/>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B22" s="3" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C22">
         <v>1</v>
@@ -2535,10 +2633,10 @@
       <c r="E22" s="44"/>
       <c r="F22" s="44"/>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A23" s="40"/>
       <c r="B23" s="41" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C23" s="3">
         <f>SUM(C19:C22)</f>
@@ -2549,18 +2647,18 @@
         <v>13</v>
       </c>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A24" s="2" t="s">
         <v>11</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D24" s="39"/>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B25" s="3" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C25">
         <v>1.5</v>
@@ -2569,9 +2667,9 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B26" s="3" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C26">
         <v>3</v>
@@ -2580,9 +2678,9 @@
         <v>3</v>
       </c>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B27" s="3" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C27">
         <v>1.5</v>
@@ -2591,9 +2689,9 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B28" s="41" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C28" s="3">
         <f>SUM(C24:C27)</f>
@@ -2604,18 +2702,18 @@
         <v>6</v>
       </c>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A29" s="2" t="s">
         <v>12</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D29" s="39"/>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B30" s="3" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C30">
         <v>1</v>
@@ -2625,9 +2723,9 @@
       </c>
       <c r="E30" s="44"/>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B31" s="3" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C31">
         <v>2</v>
@@ -2637,18 +2735,18 @@
       </c>
       <c r="E31" s="44"/>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B32" s="3" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C32">
         <v>2</v>
       </c>
       <c r="D32" s="39"/>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B33" s="41" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C33" s="3">
         <f>SUM(C29:C32)</f>
@@ -2659,7 +2757,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A34" s="42"/>
       <c r="B34" s="43" t="s">
         <v>0</v>

</xml_diff>

<commit_message>
Player can kill enemies
</commit_message>
<xml_diff>
--- a/docs/ganttChart.xlsx
+++ b/docs/ganttChart.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11015"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21425"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/blakelyfrechette/Desktop/banana/docs/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\cs383 banana\backup2\banana\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CBFE3E4-7336-F54A-BF20-85981F78E2F4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14DA953B-D8F6-409B-930D-6D9F9A4E3715}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" tabRatio="500" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="13200" yWindow="1020" windowWidth="14520" windowHeight="13080" tabRatio="500" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Management Summary" sheetId="1" r:id="rId1"/>
@@ -18,8 +18,14 @@
     <sheet name="Meetings" sheetId="3" r:id="rId3"/>
     <sheet name="SA" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="179021"/>
+  <calcPr calcId="191029"/>
   <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
+    </ext>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
     </ext>
@@ -28,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="364" uniqueCount="61">
   <si>
     <t>Total</t>
   </si>
@@ -522,12 +528,12 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -940,51 +946,51 @@
       <selection activeCell="L7" sqref="L7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="8.5" customWidth="1"/>
-    <col min="3" max="3" width="14.1640625" customWidth="1"/>
-    <col min="4" max="4" width="13.83203125" customWidth="1"/>
-    <col min="5" max="5" width="13.33203125" customWidth="1"/>
-    <col min="6" max="6" width="3.5" customWidth="1"/>
-    <col min="7" max="7" width="15.33203125" customWidth="1"/>
-    <col min="8" max="8" width="12.33203125" customWidth="1"/>
-    <col min="9" max="9" width="14.5" customWidth="1"/>
-    <col min="10" max="10" width="2.83203125" customWidth="1"/>
-    <col min="11" max="11" width="13.83203125" customWidth="1"/>
+    <col min="1" max="2" width="8.42578125" customWidth="1"/>
+    <col min="3" max="3" width="14.140625" customWidth="1"/>
+    <col min="4" max="4" width="13.85546875" customWidth="1"/>
+    <col min="5" max="5" width="13.28515625" customWidth="1"/>
+    <col min="6" max="6" width="3.42578125" customWidth="1"/>
+    <col min="7" max="7" width="15.28515625" customWidth="1"/>
+    <col min="8" max="8" width="12.28515625" customWidth="1"/>
+    <col min="9" max="9" width="14.42578125" customWidth="1"/>
+    <col min="10" max="10" width="2.85546875" customWidth="1"/>
+    <col min="11" max="11" width="13.85546875" customWidth="1"/>
     <col min="12" max="12" width="14" customWidth="1"/>
-    <col min="13" max="13" width="14.1640625" customWidth="1"/>
-    <col min="14" max="14" width="5.5" customWidth="1"/>
-    <col min="15" max="15" width="12.33203125" customWidth="1"/>
-    <col min="16" max="16" width="14.6640625" customWidth="1"/>
-    <col min="17" max="17" width="11.33203125" customWidth="1"/>
-    <col min="18" max="1025" width="8.5" customWidth="1"/>
+    <col min="13" max="13" width="14.140625" customWidth="1"/>
+    <col min="14" max="14" width="5.42578125" customWidth="1"/>
+    <col min="15" max="15" width="12.28515625" customWidth="1"/>
+    <col min="16" max="16" width="14.7109375" customWidth="1"/>
+    <col min="17" max="17" width="11.28515625" customWidth="1"/>
+    <col min="18" max="1025" width="8.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:17" x14ac:dyDescent="0.2">
-      <c r="C2" s="47" t="s">
-        <v>0</v>
-      </c>
-      <c r="D2" s="47"/>
-      <c r="E2" s="47"/>
+    <row r="2" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="C2" s="50" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2" s="50"/>
+      <c r="E2" s="50"/>
       <c r="F2" s="1"/>
-      <c r="G2" s="47" t="s">
+      <c r="G2" s="50" t="s">
         <v>1</v>
       </c>
-      <c r="H2" s="47"/>
-      <c r="I2" s="47"/>
-      <c r="K2" s="47" t="s">
+      <c r="H2" s="50"/>
+      <c r="I2" s="50"/>
+      <c r="K2" s="50" t="s">
         <v>2</v>
       </c>
-      <c r="L2" s="47"/>
-      <c r="M2" s="47"/>
-      <c r="O2" s="47" t="s">
+      <c r="L2" s="50"/>
+      <c r="M2" s="50"/>
+      <c r="O2" s="50" t="s">
         <v>3</v>
       </c>
-      <c r="P2" s="47"/>
-      <c r="Q2" s="47"/>
-    </row>
-    <row r="3" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="P2" s="50"/>
+      <c r="Q2" s="50"/>
+    </row>
+    <row r="3" spans="2:17" x14ac:dyDescent="0.25">
       <c r="C3" s="2" t="s">
         <v>4</v>
       </c>
@@ -1022,7 +1028,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B4" s="8" t="s">
         <v>7</v>
       </c>
@@ -1072,7 +1078,7 @@
         <v>-375</v>
       </c>
     </row>
-    <row r="5" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B5" s="2" t="s">
         <v>8</v>
       </c>
@@ -1122,7 +1128,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B6" s="2" t="s">
         <v>9</v>
       </c>
@@ -1172,7 +1178,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="7" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B7" s="2" t="s">
         <v>10</v>
       </c>
@@ -1222,7 +1228,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="8" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B8" s="15" t="s">
         <v>11</v>
       </c>
@@ -1270,7 +1276,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="9" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B9" s="15" t="s">
         <v>12</v>
       </c>
@@ -1318,7 +1324,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="10" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B10" s="5" t="s">
         <v>0</v>
       </c>
@@ -1387,21 +1393,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AD62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" zoomScale="83" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H49" sqref="H49"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="83" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J27" sqref="J27:L27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="29" customWidth="1"/>
-    <col min="2" max="2" width="17.5" customWidth="1"/>
-    <col min="3" max="3" width="15.6640625" customWidth="1"/>
-    <col min="4" max="5" width="8.5" customWidth="1"/>
-    <col min="6" max="6" width="10.6640625" customWidth="1"/>
-    <col min="7" max="1025" width="8.5" customWidth="1"/>
+    <col min="2" max="2" width="17.42578125" customWidth="1"/>
+    <col min="3" max="3" width="15.7109375" customWidth="1"/>
+    <col min="4" max="5" width="8.42578125" customWidth="1"/>
+    <col min="6" max="6" width="10.7109375" customWidth="1"/>
+    <col min="7" max="1025" width="8.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:30" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>13</v>
       </c>
@@ -1424,7 +1430,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A2" s="28" t="s">
         <v>7</v>
       </c>
@@ -1510,7 +1516,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="3" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>20</v>
       </c>
@@ -1521,7 +1527,7 @@
         <v>1.36</v>
       </c>
     </row>
-    <row r="4" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>21</v>
       </c>
@@ -1532,7 +1538,7 @@
         <v>0.45</v>
       </c>
     </row>
-    <row r="5" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>22</v>
       </c>
@@ -1540,7 +1546,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>23</v>
       </c>
@@ -1551,7 +1557,7 @@
         <v>3.52</v>
       </c>
     </row>
-    <row r="10" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>24</v>
       </c>
@@ -1564,12 +1570,12 @@
         <v>6.33</v>
       </c>
     </row>
-    <row r="11" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A11" s="29" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>24</v>
       </c>
@@ -1582,12 +1588,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A21" s="29" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>47</v>
       </c>
@@ -1599,7 +1605,7 @@
       </c>
       <c r="E22" s="30"/>
     </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>48</v>
       </c>
@@ -1611,7 +1617,7 @@
       </c>
       <c r="F23" s="44"/>
     </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>49</v>
       </c>
@@ -1623,7 +1629,7 @@
       </c>
       <c r="G24" s="44"/>
     </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>50</v>
       </c>
@@ -1635,7 +1641,7 @@
       </c>
       <c r="H25" s="44"/>
     </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>51</v>
       </c>
@@ -1645,9 +1651,9 @@
       <c r="C26">
         <v>1</v>
       </c>
-      <c r="I26" s="46"/>
-    </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="I26" s="44"/>
+    </row>
+    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>52</v>
       </c>
@@ -1657,11 +1663,11 @@
       <c r="C27">
         <v>0</v>
       </c>
-      <c r="J27" s="45"/>
-      <c r="K27" s="45"/>
-      <c r="L27" s="45"/>
-    </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="J27" s="46"/>
+      <c r="K27" s="46"/>
+      <c r="L27" s="46"/>
+    </row>
+    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>53</v>
       </c>
@@ -1674,7 +1680,7 @@
       <c r="M28" s="45"/>
       <c r="N28" s="45"/>
     </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>54</v>
       </c>
@@ -1686,7 +1692,7 @@
       </c>
       <c r="O29" s="45"/>
     </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>24</v>
       </c>
@@ -1699,12 +1705,12 @@
         <v>9</v>
       </c>
     </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A31" s="29" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>20</v>
       </c>
@@ -1716,7 +1722,7 @@
       </c>
       <c r="E32" s="44"/>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>21</v>
       </c>
@@ -1728,7 +1734,7 @@
       </c>
       <c r="E33" s="44"/>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>44</v>
       </c>
@@ -1738,7 +1744,7 @@
       <c r="E34" s="45"/>
       <c r="F34" s="45"/>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>45</v>
       </c>
@@ -1748,7 +1754,7 @@
       <c r="E35" s="45"/>
       <c r="F35" s="45"/>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>46</v>
       </c>
@@ -1758,7 +1764,7 @@
       <c r="E36" s="45"/>
       <c r="F36" s="45"/>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>24</v>
       </c>
@@ -1771,12 +1777,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" s="29" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>60</v>
       </c>
@@ -1788,7 +1794,7 @@
       </c>
       <c r="E40" s="44"/>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>55</v>
       </c>
@@ -1799,9 +1805,9 @@
         <v>1.5</v>
       </c>
       <c r="E41" s="44"/>
-      <c r="F41" s="48"/>
-    </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F41" s="47"/>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>21</v>
       </c>
@@ -1811,9 +1817,9 @@
       <c r="C42">
         <v>1</v>
       </c>
-      <c r="E42" s="49"/>
-    </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="E42" s="48"/>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>25</v>
       </c>
@@ -1823,9 +1829,9 @@
       <c r="C43">
         <v>0.5</v>
       </c>
-      <c r="E43" s="49"/>
-    </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="E43" s="48"/>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>46</v>
       </c>
@@ -1835,10 +1841,10 @@
       <c r="C44">
         <v>2.5</v>
       </c>
-      <c r="E44" s="49"/>
+      <c r="E44" s="48"/>
       <c r="F44" s="46"/>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>56</v>
       </c>
@@ -1848,10 +1854,10 @@
       <c r="C45">
         <v>4</v>
       </c>
-      <c r="E45" s="49"/>
-      <c r="F45" s="49"/>
-    </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="E45" s="48"/>
+      <c r="F45" s="48"/>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>57</v>
       </c>
@@ -1861,12 +1867,12 @@
       <c r="C46">
         <v>0.5</v>
       </c>
-      <c r="E46" s="49"/>
+      <c r="E46" s="48"/>
       <c r="F46" s="46"/>
       <c r="G46" s="45"/>
-      <c r="H46" s="50"/>
-    </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H46" s="49"/>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>58</v>
       </c>
@@ -1876,10 +1882,10 @@
       <c r="C47">
         <v>1</v>
       </c>
-      <c r="E47" s="49"/>
+      <c r="E47" s="48"/>
       <c r="F47" s="45"/>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>59</v>
       </c>
@@ -1891,7 +1897,7 @@
       </c>
       <c r="E48" s="46"/>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>24</v>
       </c>
@@ -1904,12 +1910,12 @@
         <v>12.75</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" s="29" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>20</v>
       </c>
@@ -1921,7 +1927,7 @@
       </c>
       <c r="E54" s="25"/>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>21</v>
       </c>
@@ -1933,7 +1939,7 @@
       </c>
       <c r="E55" s="25"/>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>24</v>
       </c>
@@ -1946,7 +1952,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>26</v>
       </c>
@@ -1959,7 +1965,7 @@
         <v>34.08</v>
       </c>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>27</v>
       </c>
@@ -1986,12 +1992,12 @@
       <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1025" width="8.5" customWidth="1"/>
+    <col min="1" max="1025" width="8.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B1" s="3" t="s">
         <v>28</v>
       </c>
@@ -2026,7 +2032,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="62.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:12" ht="62.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="3" t="s">
         <v>30</v>
       </c>
@@ -2061,7 +2067,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B3" s="3" t="s">
         <v>33</v>
       </c>
@@ -2096,7 +2102,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>7</v>
       </c>
@@ -2125,7 +2131,7 @@
       <c r="K4" s="35"/>
       <c r="L4" s="35"/>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>8</v>
       </c>
@@ -2150,7 +2156,7 @@
       <c r="K5" s="35"/>
       <c r="L5" s="35"/>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>9</v>
       </c>
@@ -2179,7 +2185,7 @@
       <c r="K6" s="35"/>
       <c r="L6" s="35"/>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>10</v>
       </c>
@@ -2208,7 +2214,7 @@
       <c r="K7" s="35"/>
       <c r="L7" s="35"/>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>11</v>
       </c>
@@ -2232,7 +2238,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>12</v>
       </c>
@@ -2253,7 +2259,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>0</v>
       </c>
@@ -2302,7 +2308,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="35" t="s">
         <v>34</v>
       </c>
@@ -2321,17 +2327,17 @@
       <selection activeCell="M29" sqref="M29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15" customWidth="1"/>
-    <col min="2" max="2" width="29.6640625" customWidth="1"/>
-    <col min="3" max="3" width="14.5" customWidth="1"/>
-    <col min="4" max="4" width="10.5" customWidth="1"/>
-    <col min="5" max="19" width="3.6640625" customWidth="1"/>
-    <col min="20" max="1025" width="8.5" customWidth="1"/>
+    <col min="2" max="2" width="29.7109375" customWidth="1"/>
+    <col min="3" max="3" width="14.42578125" customWidth="1"/>
+    <col min="4" max="4" width="10.42578125" customWidth="1"/>
+    <col min="5" max="19" width="3.7109375" customWidth="1"/>
+    <col min="20" max="1025" width="8.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A1" s="36"/>
       <c r="B1" s="37" t="s">
         <v>35</v>
@@ -2388,7 +2394,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>7</v>
       </c>
@@ -2397,7 +2403,7 @@
       </c>
       <c r="D2" s="39"/>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B3" s="3" t="s">
         <v>39</v>
       </c>
@@ -2408,7 +2414,7 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B4" s="3" t="s">
         <v>40</v>
       </c>
@@ -2419,7 +2425,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B5" s="3" t="s">
         <v>41</v>
       </c>
@@ -2430,7 +2436,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A6" s="40"/>
       <c r="B6" s="3" t="s">
         <v>42</v>
@@ -2444,7 +2450,7 @@
         <v>8.75</v>
       </c>
     </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>8</v>
       </c>
@@ -2453,25 +2459,25 @@
       </c>
       <c r="D7" s="39"/>
     </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B8" s="3" t="s">
         <v>43</v>
       </c>
       <c r="D8" s="39"/>
     </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B9" s="3" t="s">
         <v>40</v>
       </c>
       <c r="D9" s="39"/>
     </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B10" s="3" t="s">
         <v>41</v>
       </c>
       <c r="D10" s="39"/>
     </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A11" s="40"/>
       <c r="B11" s="3" t="s">
         <v>42</v>
@@ -2485,7 +2491,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>9</v>
       </c>
@@ -2494,7 +2500,7 @@
       </c>
       <c r="D12" s="39"/>
     </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B13" s="3" t="s">
         <v>43</v>
       </c>
@@ -2507,7 +2513,7 @@
       <c r="E13" s="44"/>
       <c r="F13" s="44"/>
     </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B14" s="3" t="s">
         <v>40</v>
       </c>
@@ -2522,7 +2528,7 @@
       <c r="I14" s="44"/>
       <c r="J14" s="44"/>
     </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B15" s="3" t="s">
         <v>41</v>
       </c>
@@ -2535,7 +2541,7 @@
       <c r="J15" s="44"/>
       <c r="K15" s="44"/>
     </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B16" s="3" t="s">
         <v>20</v>
       </c>
@@ -2547,7 +2553,7 @@
       </c>
       <c r="K16" s="44"/>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B17" s="3" t="s">
         <v>21</v>
       </c>
@@ -2559,7 +2565,7 @@
       </c>
       <c r="L17" s="44"/>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" s="40"/>
       <c r="B18" s="41" t="s">
         <v>42</v>
@@ -2573,7 +2579,7 @@
         <v>6.5</v>
       </c>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>10</v>
       </c>
@@ -2588,7 +2594,7 @@
       </c>
       <c r="E19" s="44"/>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B20" s="3" t="s">
         <v>43</v>
       </c>
@@ -2602,7 +2608,7 @@
       <c r="F20" s="44"/>
       <c r="G20" s="44"/>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B21" s="3" t="s">
         <v>40</v>
       </c>
@@ -2620,7 +2626,7 @@
       <c r="J21" s="44"/>
       <c r="K21" s="44"/>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B22" s="3" t="s">
         <v>41</v>
       </c>
@@ -2633,7 +2639,7 @@
       <c r="E22" s="44"/>
       <c r="F22" s="44"/>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" s="40"/>
       <c r="B23" s="41" t="s">
         <v>42</v>
@@ -2647,7 +2653,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
         <v>11</v>
       </c>
@@ -2656,7 +2662,7 @@
       </c>
       <c r="D24" s="39"/>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B25" s="3" t="s">
         <v>43</v>
       </c>
@@ -2667,7 +2673,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B26" s="3" t="s">
         <v>40</v>
       </c>
@@ -2678,7 +2684,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B27" s="3" t="s">
         <v>41</v>
       </c>
@@ -2689,7 +2695,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B28" s="41" t="s">
         <v>42</v>
       </c>
@@ -2702,7 +2708,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
         <v>12</v>
       </c>
@@ -2711,7 +2717,7 @@
       </c>
       <c r="D29" s="39"/>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B30" s="3" t="s">
         <v>43</v>
       </c>
@@ -2723,7 +2729,7 @@
       </c>
       <c r="E30" s="44"/>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B31" s="3" t="s">
         <v>40</v>
       </c>
@@ -2735,7 +2741,7 @@
       </c>
       <c r="E31" s="44"/>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B32" s="3" t="s">
         <v>41</v>
       </c>
@@ -2744,7 +2750,7 @@
       </c>
       <c r="D32" s="39"/>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B33" s="41" t="s">
         <v>42</v>
       </c>
@@ -2757,7 +2763,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="42"/>
       <c r="B34" s="43" t="s">
         <v>0</v>

</xml_diff>